<commit_message>
Complete LO 1.1 define facilitation
</commit_message>
<xml_diff>
--- a/ACS-CF Mentee Mapping Learning Log TEMPLATE - Esuabom Dijemeni.xlsx
+++ b/ACS-CF Mentee Mapping Learning Log TEMPLATE - Esuabom Dijemeni.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esuabomdijemeni/Desktop/github/acs-cf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38810C16-DD0C-164C-95E3-A69EC7162DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9643DE-A2A7-3C41-BBFF-53AD3466D254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Note" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="222">
   <si>
     <t>A note about Bloom's Taxonomy</t>
   </si>
@@ -1825,6 +1825,18 @@
   <si>
     <t>Completed all sections of the Learning log, recieved feedback on all LOs and made any required adaptions</t>
   </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>LO 1.1 - 1.3</t>
+  </si>
+  <si>
+    <t>What is facilitation? Who is a facilitator?</t>
+  </si>
 </sst>
 </file>
 
@@ -2345,7 +2357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2522,53 +2534,54 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="23" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="20" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -16896,7 +16909,7 @@
   </sheetPr>
   <dimension ref="A1:AB1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -16975,18 +16988,18 @@
     </row>
     <row r="3" spans="1:28" ht="15.75" customHeight="1">
       <c r="A3" s="25"/>
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="86" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="72"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="88"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -17107,13 +17120,13 @@
     </row>
     <row r="6" spans="1:28" ht="78">
       <c r="A6" s="25"/>
-      <c r="B6" s="73">
+      <c r="B6" s="83">
         <v>1</v>
       </c>
-      <c r="C6" s="76" t="s">
+      <c r="C6" s="84" t="s">
         <v>123</v>
       </c>
-      <c r="D6" s="77" t="s">
+      <c r="D6" s="79" t="s">
         <v>124</v>
       </c>
       <c r="E6" s="50" t="s">
@@ -17147,9 +17160,9 @@
     </row>
     <row r="7" spans="1:28" ht="49.5" customHeight="1">
       <c r="A7" s="25"/>
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="75"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="72"/>
       <c r="E7" s="50" t="s">
         <v>127</v>
       </c>
@@ -17178,9 +17191,9 @@
     </row>
     <row r="8" spans="1:28" ht="49.5" customHeight="1">
       <c r="A8" s="25"/>
-      <c r="B8" s="74"/>
-      <c r="C8" s="74"/>
-      <c r="D8" s="77" t="s">
+      <c r="B8" s="71"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="79" t="s">
         <v>128</v>
       </c>
       <c r="E8" s="50" t="s">
@@ -17214,9 +17227,9 @@
     </row>
     <row r="9" spans="1:28" ht="49.5" customHeight="1">
       <c r="A9" s="25"/>
-      <c r="B9" s="75"/>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="72"/>
       <c r="E9" s="50" t="s">
         <v>131</v>
       </c>
@@ -17248,13 +17261,13 @@
     </row>
     <row r="10" spans="1:28" ht="49.5" customHeight="1">
       <c r="A10" s="25"/>
-      <c r="B10" s="78">
+      <c r="B10" s="85">
         <v>2</v>
       </c>
-      <c r="C10" s="79" t="s">
+      <c r="C10" s="75" t="s">
         <v>133</v>
       </c>
-      <c r="D10" s="77" t="s">
+      <c r="D10" s="79" t="s">
         <v>134</v>
       </c>
       <c r="E10" s="50" t="s">
@@ -17288,9 +17301,9 @@
     </row>
     <row r="11" spans="1:28" ht="78">
       <c r="A11" s="25"/>
-      <c r="B11" s="74"/>
-      <c r="C11" s="74"/>
-      <c r="D11" s="74"/>
+      <c r="B11" s="71"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="71"/>
       <c r="E11" s="50" t="s">
         <v>137</v>
       </c>
@@ -17322,9 +17335,9 @@
     </row>
     <row r="12" spans="1:28" ht="49.5" customHeight="1">
       <c r="A12" s="25"/>
-      <c r="B12" s="74"/>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="71"/>
       <c r="E12" s="50" t="s">
         <v>139</v>
       </c>
@@ -17356,9 +17369,9 @@
     </row>
     <row r="13" spans="1:28" ht="49.5" customHeight="1">
       <c r="A13" s="25"/>
-      <c r="B13" s="74"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
+      <c r="B13" s="71"/>
+      <c r="C13" s="71"/>
+      <c r="D13" s="71"/>
       <c r="E13" s="50" t="s">
         <v>141</v>
       </c>
@@ -17390,9 +17403,9 @@
     </row>
     <row r="14" spans="1:28" ht="49.5" customHeight="1">
       <c r="A14" s="25"/>
-      <c r="B14" s="74"/>
-      <c r="C14" s="74"/>
-      <c r="D14" s="74"/>
+      <c r="B14" s="71"/>
+      <c r="C14" s="71"/>
+      <c r="D14" s="71"/>
       <c r="E14" s="50" t="s">
         <v>143</v>
       </c>
@@ -17424,9 +17437,9 @@
     </row>
     <row r="15" spans="1:28" ht="104">
       <c r="A15" s="25"/>
-      <c r="B15" s="74"/>
-      <c r="C15" s="74"/>
-      <c r="D15" s="75"/>
+      <c r="B15" s="71"/>
+      <c r="C15" s="71"/>
+      <c r="D15" s="72"/>
       <c r="E15" s="50" t="s">
         <v>145</v>
       </c>
@@ -17458,9 +17471,9 @@
     </row>
     <row r="16" spans="1:28" ht="49.5" customHeight="1">
       <c r="A16" s="25"/>
-      <c r="B16" s="74"/>
-      <c r="C16" s="74"/>
-      <c r="D16" s="80" t="s">
+      <c r="B16" s="71"/>
+      <c r="C16" s="71"/>
+      <c r="D16" s="76" t="s">
         <v>147</v>
       </c>
       <c r="E16" s="50" t="s">
@@ -17494,9 +17507,9 @@
     </row>
     <row r="17" spans="1:28" ht="49.5" customHeight="1">
       <c r="A17" s="25"/>
-      <c r="B17" s="74"/>
-      <c r="C17" s="74"/>
-      <c r="D17" s="74"/>
+      <c r="B17" s="71"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="71"/>
       <c r="E17" s="50" t="s">
         <v>150</v>
       </c>
@@ -17528,9 +17541,9 @@
     </row>
     <row r="18" spans="1:28" ht="49.5" customHeight="1">
       <c r="A18" s="25"/>
-      <c r="B18" s="74"/>
-      <c r="C18" s="74"/>
-      <c r="D18" s="74"/>
+      <c r="B18" s="71"/>
+      <c r="C18" s="71"/>
+      <c r="D18" s="71"/>
       <c r="E18" s="50" t="s">
         <v>152</v>
       </c>
@@ -17562,9 +17575,9 @@
     </row>
     <row r="19" spans="1:28" ht="49.5" customHeight="1">
       <c r="A19" s="25"/>
-      <c r="B19" s="74"/>
-      <c r="C19" s="74"/>
-      <c r="D19" s="74"/>
+      <c r="B19" s="71"/>
+      <c r="C19" s="71"/>
+      <c r="D19" s="71"/>
       <c r="E19" s="50" t="s">
         <v>154</v>
       </c>
@@ -17596,9 +17609,9 @@
     </row>
     <row r="20" spans="1:28" ht="49.5" customHeight="1">
       <c r="A20" s="25"/>
-      <c r="B20" s="74"/>
-      <c r="C20" s="74"/>
-      <c r="D20" s="74"/>
+      <c r="B20" s="71"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="71"/>
       <c r="E20" s="50" t="s">
         <v>156</v>
       </c>
@@ -17630,9 +17643,9 @@
     </row>
     <row r="21" spans="1:28" ht="49.5" customHeight="1">
       <c r="A21" s="25"/>
-      <c r="B21" s="74"/>
-      <c r="C21" s="74"/>
-      <c r="D21" s="74"/>
+      <c r="B21" s="71"/>
+      <c r="C21" s="71"/>
+      <c r="D21" s="71"/>
       <c r="E21" s="50" t="s">
         <v>158</v>
       </c>
@@ -17664,9 +17677,9 @@
     </row>
     <row r="22" spans="1:28" ht="49.5" customHeight="1">
       <c r="A22" s="25"/>
-      <c r="B22" s="75"/>
-      <c r="C22" s="75"/>
-      <c r="D22" s="75"/>
+      <c r="B22" s="72"/>
+      <c r="C22" s="72"/>
+      <c r="D22" s="72"/>
       <c r="E22" s="50" t="s">
         <v>160</v>
       </c>
@@ -17698,13 +17711,13 @@
     </row>
     <row r="23" spans="1:28" ht="49.5" customHeight="1">
       <c r="A23" s="25"/>
-      <c r="B23" s="73">
+      <c r="B23" s="83">
         <v>3</v>
       </c>
-      <c r="C23" s="79" t="s">
+      <c r="C23" s="75" t="s">
         <v>162</v>
       </c>
-      <c r="D23" s="80" t="s">
+      <c r="D23" s="76" t="s">
         <v>163</v>
       </c>
       <c r="E23" s="50" t="s">
@@ -17738,9 +17751,9 @@
     </row>
     <row r="24" spans="1:28" ht="49.5" customHeight="1">
       <c r="A24" s="25"/>
-      <c r="B24" s="74"/>
-      <c r="C24" s="74"/>
-      <c r="D24" s="74"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="71"/>
       <c r="E24" s="55" t="s">
         <v>166</v>
       </c>
@@ -17772,9 +17785,9 @@
     </row>
     <row r="25" spans="1:28" ht="49.5" customHeight="1">
       <c r="A25" s="25"/>
-      <c r="B25" s="74"/>
-      <c r="C25" s="74"/>
-      <c r="D25" s="75"/>
+      <c r="B25" s="71"/>
+      <c r="C25" s="71"/>
+      <c r="D25" s="72"/>
       <c r="E25" s="55" t="s">
         <v>168</v>
       </c>
@@ -17806,9 +17819,9 @@
     </row>
     <row r="26" spans="1:28" ht="49.5" customHeight="1">
       <c r="A26" s="25"/>
-      <c r="B26" s="74"/>
-      <c r="C26" s="74"/>
-      <c r="D26" s="77" t="s">
+      <c r="B26" s="71"/>
+      <c r="C26" s="71"/>
+      <c r="D26" s="79" t="s">
         <v>170</v>
       </c>
       <c r="E26" s="50" t="s">
@@ -17842,9 +17855,9 @@
     </row>
     <row r="27" spans="1:28" ht="104">
       <c r="A27" s="25"/>
-      <c r="B27" s="74"/>
-      <c r="C27" s="74"/>
-      <c r="D27" s="74"/>
+      <c r="B27" s="71"/>
+      <c r="C27" s="71"/>
+      <c r="D27" s="71"/>
       <c r="E27" s="50" t="s">
         <v>173</v>
       </c>
@@ -17876,9 +17889,9 @@
     </row>
     <row r="28" spans="1:28" ht="49.5" customHeight="1">
       <c r="A28" s="25"/>
-      <c r="B28" s="74"/>
-      <c r="C28" s="74"/>
-      <c r="D28" s="75"/>
+      <c r="B28" s="71"/>
+      <c r="C28" s="71"/>
+      <c r="D28" s="72"/>
       <c r="E28" s="50" t="s">
         <v>175</v>
       </c>
@@ -17910,9 +17923,9 @@
     </row>
     <row r="29" spans="1:28" ht="49.5" customHeight="1">
       <c r="A29" s="25"/>
-      <c r="B29" s="74"/>
-      <c r="C29" s="74"/>
-      <c r="D29" s="80" t="s">
+      <c r="B29" s="71"/>
+      <c r="C29" s="71"/>
+      <c r="D29" s="76" t="s">
         <v>177</v>
       </c>
       <c r="E29" s="50" t="s">
@@ -17946,9 +17959,9 @@
     </row>
     <row r="30" spans="1:28" ht="49.5" customHeight="1">
       <c r="A30" s="25"/>
-      <c r="B30" s="75"/>
-      <c r="C30" s="75"/>
-      <c r="D30" s="75"/>
+      <c r="B30" s="72"/>
+      <c r="C30" s="72"/>
+      <c r="D30" s="72"/>
       <c r="E30" s="50" t="s">
         <v>180</v>
       </c>
@@ -17980,13 +17993,13 @@
     </row>
     <row r="31" spans="1:28" ht="49.5" customHeight="1">
       <c r="A31" s="25"/>
-      <c r="B31" s="73">
+      <c r="B31" s="83">
         <v>4</v>
       </c>
-      <c r="C31" s="76" t="s">
+      <c r="C31" s="84" t="s">
         <v>182</v>
       </c>
-      <c r="D31" s="80" t="s">
+      <c r="D31" s="76" t="s">
         <v>182</v>
       </c>
       <c r="E31" s="50" t="s">
@@ -18020,9 +18033,9 @@
     </row>
     <row r="32" spans="1:28" ht="49.5" customHeight="1">
       <c r="A32" s="25"/>
-      <c r="B32" s="74"/>
-      <c r="C32" s="74"/>
-      <c r="D32" s="74"/>
+      <c r="B32" s="71"/>
+      <c r="C32" s="71"/>
+      <c r="D32" s="71"/>
       <c r="E32" s="50" t="s">
         <v>185</v>
       </c>
@@ -18054,9 +18067,9 @@
     </row>
     <row r="33" spans="1:28" ht="49.5" customHeight="1">
       <c r="A33" s="25"/>
-      <c r="B33" s="75"/>
-      <c r="C33" s="75"/>
-      <c r="D33" s="75"/>
+      <c r="B33" s="72"/>
+      <c r="C33" s="72"/>
+      <c r="D33" s="72"/>
       <c r="E33" s="50" t="s">
         <v>187</v>
       </c>
@@ -18088,10 +18101,10 @@
     </row>
     <row r="34" spans="1:28" ht="105">
       <c r="A34" s="25"/>
-      <c r="B34" s="78">
+      <c r="B34" s="85">
         <v>5</v>
       </c>
-      <c r="C34" s="79" t="s">
+      <c r="C34" s="75" t="s">
         <v>189</v>
       </c>
       <c r="D34" s="57" t="s">
@@ -18128,8 +18141,8 @@
     </row>
     <row r="35" spans="1:28" ht="49.5" customHeight="1">
       <c r="A35" s="25"/>
-      <c r="B35" s="74"/>
-      <c r="C35" s="74"/>
+      <c r="B35" s="71"/>
+      <c r="C35" s="71"/>
       <c r="D35" s="57" t="s">
         <v>193</v>
       </c>
@@ -18164,9 +18177,9 @@
     </row>
     <row r="36" spans="1:28" ht="49.5" customHeight="1">
       <c r="A36" s="25"/>
-      <c r="B36" s="74"/>
-      <c r="C36" s="74"/>
-      <c r="D36" s="80" t="s">
+      <c r="B36" s="71"/>
+      <c r="C36" s="71"/>
+      <c r="D36" s="76" t="s">
         <v>196</v>
       </c>
       <c r="E36" s="50" t="s">
@@ -18200,9 +18213,9 @@
     </row>
     <row r="37" spans="1:28" ht="78">
       <c r="A37" s="25"/>
-      <c r="B37" s="75"/>
-      <c r="C37" s="75"/>
-      <c r="D37" s="75"/>
+      <c r="B37" s="72"/>
+      <c r="C37" s="72"/>
+      <c r="D37" s="72"/>
       <c r="E37" s="50" t="s">
         <v>199</v>
       </c>
@@ -18234,13 +18247,13 @@
     </row>
     <row r="38" spans="1:28" ht="49.5" customHeight="1">
       <c r="A38" s="25"/>
-      <c r="B38" s="78">
+      <c r="B38" s="85">
         <v>6</v>
       </c>
-      <c r="C38" s="79" t="s">
+      <c r="C38" s="75" t="s">
         <v>201</v>
       </c>
-      <c r="D38" s="80" t="s">
+      <c r="D38" s="76" t="s">
         <v>201</v>
       </c>
       <c r="E38" s="50" t="s">
@@ -18274,9 +18287,9 @@
     </row>
     <row r="39" spans="1:28" ht="49.5" customHeight="1">
       <c r="A39" s="25"/>
-      <c r="B39" s="75"/>
-      <c r="C39" s="75"/>
-      <c r="D39" s="75"/>
+      <c r="B39" s="72"/>
+      <c r="C39" s="72"/>
+      <c r="D39" s="72"/>
       <c r="E39" s="59" t="s">
         <v>204</v>
       </c>
@@ -18307,28 +18320,28 @@
       <c r="AB39" s="2"/>
     </row>
     <row r="40" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A40" s="86"/>
-      <c r="B40" s="86" t="s">
+      <c r="A40" s="77"/>
+      <c r="B40" s="77" t="s">
         <v>206</v>
       </c>
-      <c r="C40" s="87" t="s">
+      <c r="C40" s="78" t="s">
         <v>207</v>
       </c>
-      <c r="D40" s="77" t="s">
+      <c r="D40" s="79" t="s">
         <v>208</v>
       </c>
-      <c r="E40" s="88" t="s">
+      <c r="E40" s="80" t="s">
         <v>209</v>
       </c>
       <c r="F40" s="81" t="s">
         <v>210</v>
       </c>
-      <c r="G40" s="82"/>
-      <c r="H40" s="82"/>
-      <c r="I40" s="83"/>
-      <c r="J40" s="82"/>
-      <c r="K40" s="82"/>
-      <c r="L40" s="84"/>
+      <c r="G40" s="70"/>
+      <c r="H40" s="70"/>
+      <c r="I40" s="82"/>
+      <c r="J40" s="70"/>
+      <c r="K40" s="70"/>
+      <c r="L40" s="73"/>
       <c r="M40" s="15"/>
       <c r="N40" s="15"/>
       <c r="O40" s="15"/>
@@ -18347,18 +18360,18 @@
       <c r="AB40" s="2"/>
     </row>
     <row r="41" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A41" s="74"/>
-      <c r="B41" s="74"/>
-      <c r="C41" s="74"/>
-      <c r="D41" s="74"/>
-      <c r="E41" s="74"/>
-      <c r="F41" s="74"/>
-      <c r="G41" s="74"/>
-      <c r="H41" s="74"/>
-      <c r="I41" s="74"/>
-      <c r="J41" s="74"/>
-      <c r="K41" s="74"/>
-      <c r="L41" s="85"/>
+      <c r="A41" s="71"/>
+      <c r="B41" s="71"/>
+      <c r="C41" s="71"/>
+      <c r="D41" s="71"/>
+      <c r="E41" s="71"/>
+      <c r="F41" s="71"/>
+      <c r="G41" s="71"/>
+      <c r="H41" s="71"/>
+      <c r="I41" s="71"/>
+      <c r="J41" s="71"/>
+      <c r="K41" s="71"/>
+      <c r="L41" s="74"/>
       <c r="M41" s="15"/>
       <c r="N41" s="15"/>
       <c r="O41" s="15"/>
@@ -18377,18 +18390,18 @@
       <c r="AB41" s="2"/>
     </row>
     <row r="42" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A42" s="74"/>
-      <c r="B42" s="74"/>
-      <c r="C42" s="74"/>
-      <c r="D42" s="74"/>
-      <c r="E42" s="74"/>
-      <c r="F42" s="74"/>
-      <c r="G42" s="74"/>
-      <c r="H42" s="74"/>
-      <c r="I42" s="74"/>
-      <c r="J42" s="74"/>
-      <c r="K42" s="74"/>
-      <c r="L42" s="85"/>
+      <c r="A42" s="71"/>
+      <c r="B42" s="71"/>
+      <c r="C42" s="71"/>
+      <c r="D42" s="71"/>
+      <c r="E42" s="71"/>
+      <c r="F42" s="71"/>
+      <c r="G42" s="71"/>
+      <c r="H42" s="71"/>
+      <c r="I42" s="71"/>
+      <c r="J42" s="71"/>
+      <c r="K42" s="71"/>
+      <c r="L42" s="74"/>
       <c r="M42" s="15"/>
       <c r="N42" s="15"/>
       <c r="O42" s="15"/>
@@ -18407,18 +18420,18 @@
       <c r="AB42" s="2"/>
     </row>
     <row r="43" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A43" s="74"/>
-      <c r="B43" s="74"/>
-      <c r="C43" s="74"/>
-      <c r="D43" s="74"/>
-      <c r="E43" s="74"/>
-      <c r="F43" s="74"/>
-      <c r="G43" s="74"/>
-      <c r="H43" s="74"/>
-      <c r="I43" s="74"/>
-      <c r="J43" s="74"/>
-      <c r="K43" s="74"/>
-      <c r="L43" s="85"/>
+      <c r="A43" s="71"/>
+      <c r="B43" s="71"/>
+      <c r="C43" s="71"/>
+      <c r="D43" s="71"/>
+      <c r="E43" s="71"/>
+      <c r="F43" s="71"/>
+      <c r="G43" s="71"/>
+      <c r="H43" s="71"/>
+      <c r="I43" s="71"/>
+      <c r="J43" s="71"/>
+      <c r="K43" s="71"/>
+      <c r="L43" s="74"/>
       <c r="M43" s="15"/>
       <c r="N43" s="15"/>
       <c r="O43" s="15"/>
@@ -18437,18 +18450,18 @@
       <c r="AB43" s="2"/>
     </row>
     <row r="44" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A44" s="74"/>
-      <c r="B44" s="74"/>
-      <c r="C44" s="74"/>
-      <c r="D44" s="74"/>
-      <c r="E44" s="74"/>
-      <c r="F44" s="74"/>
-      <c r="G44" s="74"/>
-      <c r="H44" s="74"/>
-      <c r="I44" s="74"/>
-      <c r="J44" s="74"/>
-      <c r="K44" s="74"/>
-      <c r="L44" s="85"/>
+      <c r="A44" s="71"/>
+      <c r="B44" s="71"/>
+      <c r="C44" s="71"/>
+      <c r="D44" s="71"/>
+      <c r="E44" s="71"/>
+      <c r="F44" s="71"/>
+      <c r="G44" s="71"/>
+      <c r="H44" s="71"/>
+      <c r="I44" s="71"/>
+      <c r="J44" s="71"/>
+      <c r="K44" s="71"/>
+      <c r="L44" s="74"/>
       <c r="M44" s="15"/>
       <c r="N44" s="15"/>
       <c r="O44" s="15"/>
@@ -18467,18 +18480,18 @@
       <c r="AB44" s="2"/>
     </row>
     <row r="45" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A45" s="75"/>
-      <c r="B45" s="75"/>
-      <c r="C45" s="75"/>
-      <c r="D45" s="75"/>
-      <c r="E45" s="75"/>
-      <c r="F45" s="75"/>
-      <c r="G45" s="75"/>
-      <c r="H45" s="75"/>
-      <c r="I45" s="75"/>
-      <c r="J45" s="75"/>
-      <c r="K45" s="75"/>
-      <c r="L45" s="85"/>
+      <c r="A45" s="72"/>
+      <c r="B45" s="72"/>
+      <c r="C45" s="72"/>
+      <c r="D45" s="72"/>
+      <c r="E45" s="72"/>
+      <c r="F45" s="72"/>
+      <c r="G45" s="72"/>
+      <c r="H45" s="72"/>
+      <c r="I45" s="72"/>
+      <c r="J45" s="72"/>
+      <c r="K45" s="72"/>
+      <c r="L45" s="74"/>
       <c r="M45" s="15"/>
       <c r="N45" s="15"/>
       <c r="O45" s="15"/>
@@ -25113,6 +25126,27 @@
     <row r="1005" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="B10:B22"/>
+    <mergeCell ref="C10:C22"/>
+    <mergeCell ref="D10:D15"/>
+    <mergeCell ref="D16:D22"/>
+    <mergeCell ref="B23:B30"/>
+    <mergeCell ref="C23:C30"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="D31:D33"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="C34:C37"/>
     <mergeCell ref="K40:K45"/>
     <mergeCell ref="L40:L45"/>
     <mergeCell ref="C38:C39"/>
@@ -25127,27 +25161,6 @@
     <mergeCell ref="H40:H45"/>
     <mergeCell ref="I40:I45"/>
     <mergeCell ref="J40:J45"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="D31:D33"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="B10:B22"/>
-    <mergeCell ref="C10:C22"/>
-    <mergeCell ref="D10:D15"/>
-    <mergeCell ref="D16:D22"/>
-    <mergeCell ref="B23:B30"/>
-    <mergeCell ref="C23:C30"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D8:D9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
@@ -25161,19 +25174,22 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Y1000"/>
+  <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N35" sqref="N35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11.1640625" customWidth="1"/>
-    <col min="2" max="2" width="37.1640625" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" customWidth="1"/>
-    <col min="4" max="6" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="37.1640625" customWidth="1"/>
+    <col min="5" max="5" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15.75" customHeight="1">
+    <row r="1" spans="1:27" ht="15.75" customHeight="1">
       <c r="A1" s="62" t="s">
         <v>211</v>
       </c>
@@ -25181,10 +25197,14 @@
         <v>212</v>
       </c>
       <c r="C1" s="62" t="s">
+        <v>218</v>
+      </c>
+      <c r="D1" s="62" t="s">
+        <v>219</v>
+      </c>
+      <c r="E1" s="62" t="s">
         <v>213</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
       <c r="H1" s="15"/>
@@ -25205,13 +25225,25 @@
       <c r="W1" s="15"/>
       <c r="X1" s="15"/>
       <c r="Y1" s="15"/>
-    </row>
-    <row r="2" spans="1:25" ht="15.75" customHeight="1">
-      <c r="A2" s="63"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="15"/>
+    </row>
+    <row r="2" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A2" s="63">
+        <v>45468</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="C2" s="89">
+        <v>0.625</v>
+      </c>
+      <c r="D2" s="89">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>221</v>
+      </c>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
@@ -25232,13 +25264,15 @@
       <c r="W2" s="15"/>
       <c r="X2" s="15"/>
       <c r="Y2" s="15"/>
-    </row>
-    <row r="3" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z2" s="15"/>
+      <c r="AA2" s="15"/>
+    </row>
+    <row r="3" spans="1:27" ht="15.75" customHeight="1">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
@@ -25259,13 +25293,15 @@
       <c r="W3" s="15"/>
       <c r="X3" s="15"/>
       <c r="Y3" s="15"/>
-    </row>
-    <row r="4" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z3" s="15"/>
+      <c r="AA3" s="15"/>
+    </row>
+    <row r="4" spans="1:27" ht="15.75" customHeight="1">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
@@ -25286,13 +25322,15 @@
       <c r="W4" s="15"/>
       <c r="X4" s="15"/>
       <c r="Y4" s="15"/>
-    </row>
-    <row r="5" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z4" s="15"/>
+      <c r="AA4" s="15"/>
+    </row>
+    <row r="5" spans="1:27" ht="15.75" customHeight="1">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
@@ -25313,13 +25351,15 @@
       <c r="W5" s="15"/>
       <c r="X5" s="15"/>
       <c r="Y5" s="15"/>
-    </row>
-    <row r="6" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z5" s="15"/>
+      <c r="AA5" s="15"/>
+    </row>
+    <row r="6" spans="1:27" ht="15.75" customHeight="1">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
@@ -25340,13 +25380,15 @@
       <c r="W6" s="15"/>
       <c r="X6" s="15"/>
       <c r="Y6" s="15"/>
-    </row>
-    <row r="7" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z6" s="15"/>
+      <c r="AA6" s="15"/>
+    </row>
+    <row r="7" spans="1:27" ht="15.75" customHeight="1">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
@@ -25367,13 +25409,15 @@
       <c r="W7" s="15"/>
       <c r="X7" s="15"/>
       <c r="Y7" s="15"/>
-    </row>
-    <row r="8" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z7" s="15"/>
+      <c r="AA7" s="15"/>
+    </row>
+    <row r="8" spans="1:27" ht="15.75" customHeight="1">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
@@ -25394,13 +25438,15 @@
       <c r="W8" s="15"/>
       <c r="X8" s="15"/>
       <c r="Y8" s="15"/>
-    </row>
-    <row r="9" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z8" s="15"/>
+      <c r="AA8" s="15"/>
+    </row>
+    <row r="9" spans="1:27" ht="15.75" customHeight="1">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
@@ -25421,13 +25467,15 @@
       <c r="W9" s="15"/>
       <c r="X9" s="15"/>
       <c r="Y9" s="15"/>
-    </row>
-    <row r="10" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z9" s="15"/>
+      <c r="AA9" s="15"/>
+    </row>
+    <row r="10" spans="1:27" ht="15.75" customHeight="1">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
@@ -25448,13 +25496,15 @@
       <c r="W10" s="15"/>
       <c r="X10" s="15"/>
       <c r="Y10" s="15"/>
-    </row>
-    <row r="11" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z10" s="15"/>
+      <c r="AA10" s="15"/>
+    </row>
+    <row r="11" spans="1:27" ht="15.75" customHeight="1">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
@@ -25475,13 +25525,15 @@
       <c r="W11" s="15"/>
       <c r="X11" s="15"/>
       <c r="Y11" s="15"/>
-    </row>
-    <row r="12" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z11" s="15"/>
+      <c r="AA11" s="15"/>
+    </row>
+    <row r="12" spans="1:27" ht="15.75" customHeight="1">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
@@ -25502,13 +25554,15 @@
       <c r="W12" s="15"/>
       <c r="X12" s="15"/>
       <c r="Y12" s="15"/>
-    </row>
-    <row r="13" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z12" s="15"/>
+      <c r="AA12" s="15"/>
+    </row>
+    <row r="13" spans="1:27" ht="15.75" customHeight="1">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
@@ -25529,13 +25583,15 @@
       <c r="W13" s="15"/>
       <c r="X13" s="15"/>
       <c r="Y13" s="15"/>
-    </row>
-    <row r="14" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z13" s="15"/>
+      <c r="AA13" s="15"/>
+    </row>
+    <row r="14" spans="1:27" ht="15.75" customHeight="1">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
@@ -25556,13 +25612,15 @@
       <c r="W14" s="15"/>
       <c r="X14" s="15"/>
       <c r="Y14" s="15"/>
-    </row>
-    <row r="15" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z14" s="15"/>
+      <c r="AA14" s="15"/>
+    </row>
+    <row r="15" spans="1:27" ht="15.75" customHeight="1">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
@@ -25583,13 +25641,15 @@
       <c r="W15" s="15"/>
       <c r="X15" s="15"/>
       <c r="Y15" s="15"/>
-    </row>
-    <row r="16" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z15" s="15"/>
+      <c r="AA15" s="15"/>
+    </row>
+    <row r="16" spans="1:27" ht="15.75" customHeight="1">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
@@ -25610,13 +25670,15 @@
       <c r="W16" s="15"/>
       <c r="X16" s="15"/>
       <c r="Y16" s="15"/>
-    </row>
-    <row r="17" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z16" s="15"/>
+      <c r="AA16" s="15"/>
+    </row>
+    <row r="17" spans="1:27" ht="15.75" customHeight="1">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
@@ -25637,13 +25699,15 @@
       <c r="W17" s="15"/>
       <c r="X17" s="15"/>
       <c r="Y17" s="15"/>
-    </row>
-    <row r="18" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z17" s="15"/>
+      <c r="AA17" s="15"/>
+    </row>
+    <row r="18" spans="1:27" ht="15.75" customHeight="1">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
       <c r="F18" s="15"/>
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
@@ -25664,13 +25728,15 @@
       <c r="W18" s="15"/>
       <c r="X18" s="15"/>
       <c r="Y18" s="15"/>
-    </row>
-    <row r="19" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z18" s="15"/>
+      <c r="AA18" s="15"/>
+    </row>
+    <row r="19" spans="1:27" ht="15.75" customHeight="1">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
       <c r="F19" s="15"/>
       <c r="G19" s="15"/>
       <c r="H19" s="15"/>
@@ -25691,13 +25757,15 @@
       <c r="W19" s="15"/>
       <c r="X19" s="15"/>
       <c r="Y19" s="15"/>
-    </row>
-    <row r="20" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z19" s="15"/>
+      <c r="AA19" s="15"/>
+    </row>
+    <row r="20" spans="1:27" ht="15.75" customHeight="1">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
@@ -25718,13 +25786,15 @@
       <c r="W20" s="15"/>
       <c r="X20" s="15"/>
       <c r="Y20" s="15"/>
-    </row>
-    <row r="21" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z20" s="15"/>
+      <c r="AA20" s="15"/>
+    </row>
+    <row r="21" spans="1:27" ht="15.75" customHeight="1">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
       <c r="F21" s="15"/>
       <c r="G21" s="15"/>
       <c r="H21" s="15"/>
@@ -25745,13 +25815,15 @@
       <c r="W21" s="15"/>
       <c r="X21" s="15"/>
       <c r="Y21" s="15"/>
-    </row>
-    <row r="22" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z21" s="15"/>
+      <c r="AA21" s="15"/>
+    </row>
+    <row r="22" spans="1:27" ht="15.75" customHeight="1">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
@@ -25772,13 +25844,15 @@
       <c r="W22" s="15"/>
       <c r="X22" s="15"/>
       <c r="Y22" s="15"/>
-    </row>
-    <row r="23" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z22" s="15"/>
+      <c r="AA22" s="15"/>
+    </row>
+    <row r="23" spans="1:27" ht="15.75" customHeight="1">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
       <c r="F23" s="15"/>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
@@ -25799,13 +25873,15 @@
       <c r="W23" s="15"/>
       <c r="X23" s="15"/>
       <c r="Y23" s="15"/>
-    </row>
-    <row r="24" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z23" s="15"/>
+      <c r="AA23" s="15"/>
+    </row>
+    <row r="24" spans="1:27" ht="15.75" customHeight="1">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
@@ -25826,13 +25902,15 @@
       <c r="W24" s="15"/>
       <c r="X24" s="15"/>
       <c r="Y24" s="15"/>
-    </row>
-    <row r="25" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z24" s="15"/>
+      <c r="AA24" s="15"/>
+    </row>
+    <row r="25" spans="1:27" ht="15.75" customHeight="1">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
       <c r="F25" s="15"/>
       <c r="G25" s="15"/>
       <c r="H25" s="15"/>
@@ -25853,13 +25931,15 @@
       <c r="W25" s="15"/>
       <c r="X25" s="15"/>
       <c r="Y25" s="15"/>
-    </row>
-    <row r="26" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z25" s="15"/>
+      <c r="AA25" s="15"/>
+    </row>
+    <row r="26" spans="1:27" ht="15.75" customHeight="1">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
       <c r="H26" s="15"/>
@@ -25880,13 +25960,15 @@
       <c r="W26" s="15"/>
       <c r="X26" s="15"/>
       <c r="Y26" s="15"/>
-    </row>
-    <row r="27" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z26" s="15"/>
+      <c r="AA26" s="15"/>
+    </row>
+    <row r="27" spans="1:27" ht="15.75" customHeight="1">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
@@ -25907,13 +25989,15 @@
       <c r="W27" s="15"/>
       <c r="X27" s="15"/>
       <c r="Y27" s="15"/>
-    </row>
-    <row r="28" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z27" s="15"/>
+      <c r="AA27" s="15"/>
+    </row>
+    <row r="28" spans="1:27" ht="15.75" customHeight="1">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
@@ -25934,13 +26018,15 @@
       <c r="W28" s="15"/>
       <c r="X28" s="15"/>
       <c r="Y28" s="15"/>
-    </row>
-    <row r="29" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z28" s="15"/>
+      <c r="AA28" s="15"/>
+    </row>
+    <row r="29" spans="1:27" ht="15.75" customHeight="1">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
@@ -25961,13 +26047,15 @@
       <c r="W29" s="15"/>
       <c r="X29" s="15"/>
       <c r="Y29" s="15"/>
-    </row>
-    <row r="30" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z29" s="15"/>
+      <c r="AA29" s="15"/>
+    </row>
+    <row r="30" spans="1:27" ht="15.75" customHeight="1">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
       <c r="F30" s="15"/>
       <c r="G30" s="15"/>
       <c r="H30" s="15"/>
@@ -25988,13 +26076,15 @@
       <c r="W30" s="15"/>
       <c r="X30" s="15"/>
       <c r="Y30" s="15"/>
-    </row>
-    <row r="31" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z30" s="15"/>
+      <c r="AA30" s="15"/>
+    </row>
+    <row r="31" spans="1:27" ht="15.75" customHeight="1">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
       <c r="F31" s="15"/>
       <c r="G31" s="15"/>
       <c r="H31" s="15"/>
@@ -26015,13 +26105,15 @@
       <c r="W31" s="15"/>
       <c r="X31" s="15"/>
       <c r="Y31" s="15"/>
-    </row>
-    <row r="32" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z31" s="15"/>
+      <c r="AA31" s="15"/>
+    </row>
+    <row r="32" spans="1:27" ht="15.75" customHeight="1">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
       <c r="F32" s="15"/>
       <c r="G32" s="15"/>
       <c r="H32" s="15"/>
@@ -26042,8 +26134,10 @@
       <c r="W32" s="15"/>
       <c r="X32" s="15"/>
       <c r="Y32" s="15"/>
-    </row>
-    <row r="33" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z32" s="15"/>
+      <c r="AA32" s="15"/>
+    </row>
+    <row r="33" spans="1:27" ht="15.75" customHeight="1">
       <c r="A33" s="15"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
@@ -26069,8 +26163,10 @@
       <c r="W33" s="15"/>
       <c r="X33" s="15"/>
       <c r="Y33" s="15"/>
-    </row>
-    <row r="34" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z33" s="15"/>
+      <c r="AA33" s="15"/>
+    </row>
+    <row r="34" spans="1:27" ht="15.75" customHeight="1">
       <c r="A34" s="15"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
@@ -26096,8 +26192,10 @@
       <c r="W34" s="15"/>
       <c r="X34" s="15"/>
       <c r="Y34" s="15"/>
-    </row>
-    <row r="35" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z34" s="15"/>
+      <c r="AA34" s="15"/>
+    </row>
+    <row r="35" spans="1:27" ht="15.75" customHeight="1">
       <c r="A35" s="15"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
@@ -26123,8 +26221,10 @@
       <c r="W35" s="15"/>
       <c r="X35" s="15"/>
       <c r="Y35" s="15"/>
-    </row>
-    <row r="36" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z35" s="15"/>
+      <c r="AA35" s="15"/>
+    </row>
+    <row r="36" spans="1:27" ht="15.75" customHeight="1">
       <c r="A36" s="15"/>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
@@ -26150,8 +26250,10 @@
       <c r="W36" s="15"/>
       <c r="X36" s="15"/>
       <c r="Y36" s="15"/>
-    </row>
-    <row r="37" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z36" s="15"/>
+      <c r="AA36" s="15"/>
+    </row>
+    <row r="37" spans="1:27" ht="15.75" customHeight="1">
       <c r="A37" s="15"/>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
@@ -26177,8 +26279,10 @@
       <c r="W37" s="15"/>
       <c r="X37" s="15"/>
       <c r="Y37" s="15"/>
-    </row>
-    <row r="38" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z37" s="15"/>
+      <c r="AA37" s="15"/>
+    </row>
+    <row r="38" spans="1:27" ht="15.75" customHeight="1">
       <c r="A38" s="15"/>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
@@ -26204,8 +26308,10 @@
       <c r="W38" s="15"/>
       <c r="X38" s="15"/>
       <c r="Y38" s="15"/>
-    </row>
-    <row r="39" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z38" s="15"/>
+      <c r="AA38" s="15"/>
+    </row>
+    <row r="39" spans="1:27" ht="15.75" customHeight="1">
       <c r="A39" s="15"/>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
@@ -26231,8 +26337,10 @@
       <c r="W39" s="15"/>
       <c r="X39" s="15"/>
       <c r="Y39" s="15"/>
-    </row>
-    <row r="40" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z39" s="15"/>
+      <c r="AA39" s="15"/>
+    </row>
+    <row r="40" spans="1:27" ht="15.75" customHeight="1">
       <c r="A40" s="15"/>
       <c r="B40" s="15"/>
       <c r="C40" s="15"/>
@@ -26258,8 +26366,10 @@
       <c r="W40" s="15"/>
       <c r="X40" s="15"/>
       <c r="Y40" s="15"/>
-    </row>
-    <row r="41" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z40" s="15"/>
+      <c r="AA40" s="15"/>
+    </row>
+    <row r="41" spans="1:27" ht="15.75" customHeight="1">
       <c r="A41" s="15"/>
       <c r="B41" s="15"/>
       <c r="C41" s="15"/>
@@ -26285,8 +26395,10 @@
       <c r="W41" s="15"/>
       <c r="X41" s="15"/>
       <c r="Y41" s="15"/>
-    </row>
-    <row r="42" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z41" s="15"/>
+      <c r="AA41" s="15"/>
+    </row>
+    <row r="42" spans="1:27" ht="15.75" customHeight="1">
       <c r="A42" s="15"/>
       <c r="B42" s="15"/>
       <c r="C42" s="15"/>
@@ -26312,8 +26424,10 @@
       <c r="W42" s="15"/>
       <c r="X42" s="15"/>
       <c r="Y42" s="15"/>
-    </row>
-    <row r="43" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z42" s="15"/>
+      <c r="AA42" s="15"/>
+    </row>
+    <row r="43" spans="1:27" ht="15.75" customHeight="1">
       <c r="A43" s="15"/>
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
@@ -26339,8 +26453,10 @@
       <c r="W43" s="15"/>
       <c r="X43" s="15"/>
       <c r="Y43" s="15"/>
-    </row>
-    <row r="44" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z43" s="15"/>
+      <c r="AA43" s="15"/>
+    </row>
+    <row r="44" spans="1:27" ht="15.75" customHeight="1">
       <c r="A44" s="15"/>
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
@@ -26366,8 +26482,10 @@
       <c r="W44" s="15"/>
       <c r="X44" s="15"/>
       <c r="Y44" s="15"/>
-    </row>
-    <row r="45" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z44" s="15"/>
+      <c r="AA44" s="15"/>
+    </row>
+    <row r="45" spans="1:27" ht="15.75" customHeight="1">
       <c r="A45" s="15"/>
       <c r="B45" s="15"/>
       <c r="C45" s="15"/>
@@ -26393,8 +26511,10 @@
       <c r="W45" s="15"/>
       <c r="X45" s="15"/>
       <c r="Y45" s="15"/>
-    </row>
-    <row r="46" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z45" s="15"/>
+      <c r="AA45" s="15"/>
+    </row>
+    <row r="46" spans="1:27" ht="15.75" customHeight="1">
       <c r="A46" s="15"/>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
@@ -26420,8 +26540,10 @@
       <c r="W46" s="15"/>
       <c r="X46" s="15"/>
       <c r="Y46" s="15"/>
-    </row>
-    <row r="47" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z46" s="15"/>
+      <c r="AA46" s="15"/>
+    </row>
+    <row r="47" spans="1:27" ht="15.75" customHeight="1">
       <c r="A47" s="15"/>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>
@@ -26447,8 +26569,10 @@
       <c r="W47" s="15"/>
       <c r="X47" s="15"/>
       <c r="Y47" s="15"/>
-    </row>
-    <row r="48" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z47" s="15"/>
+      <c r="AA47" s="15"/>
+    </row>
+    <row r="48" spans="1:27" ht="15.75" customHeight="1">
       <c r="A48" s="15"/>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
@@ -26474,8 +26598,10 @@
       <c r="W48" s="15"/>
       <c r="X48" s="15"/>
       <c r="Y48" s="15"/>
-    </row>
-    <row r="49" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z48" s="15"/>
+      <c r="AA48" s="15"/>
+    </row>
+    <row r="49" spans="1:27" ht="15.75" customHeight="1">
       <c r="A49" s="15"/>
       <c r="B49" s="15"/>
       <c r="C49" s="15"/>
@@ -26501,8 +26627,10 @@
       <c r="W49" s="15"/>
       <c r="X49" s="15"/>
       <c r="Y49" s="15"/>
-    </row>
-    <row r="50" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z49" s="15"/>
+      <c r="AA49" s="15"/>
+    </row>
+    <row r="50" spans="1:27" ht="15.75" customHeight="1">
       <c r="A50" s="15"/>
       <c r="B50" s="15"/>
       <c r="C50" s="15"/>
@@ -26528,8 +26656,10 @@
       <c r="W50" s="15"/>
       <c r="X50" s="15"/>
       <c r="Y50" s="15"/>
-    </row>
-    <row r="51" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z50" s="15"/>
+      <c r="AA50" s="15"/>
+    </row>
+    <row r="51" spans="1:27" ht="15.75" customHeight="1">
       <c r="A51" s="15"/>
       <c r="B51" s="15"/>
       <c r="C51" s="15"/>
@@ -26555,8 +26685,10 @@
       <c r="W51" s="15"/>
       <c r="X51" s="15"/>
       <c r="Y51" s="15"/>
-    </row>
-    <row r="52" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z51" s="15"/>
+      <c r="AA51" s="15"/>
+    </row>
+    <row r="52" spans="1:27" ht="15.75" customHeight="1">
       <c r="A52" s="15"/>
       <c r="B52" s="15"/>
       <c r="C52" s="15"/>
@@ -26582,8 +26714,10 @@
       <c r="W52" s="15"/>
       <c r="X52" s="15"/>
       <c r="Y52" s="15"/>
-    </row>
-    <row r="53" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z52" s="15"/>
+      <c r="AA52" s="15"/>
+    </row>
+    <row r="53" spans="1:27" ht="15.75" customHeight="1">
       <c r="A53" s="15"/>
       <c r="B53" s="15"/>
       <c r="C53" s="15"/>
@@ -26609,8 +26743,10 @@
       <c r="W53" s="15"/>
       <c r="X53" s="15"/>
       <c r="Y53" s="15"/>
-    </row>
-    <row r="54" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z53" s="15"/>
+      <c r="AA53" s="15"/>
+    </row>
+    <row r="54" spans="1:27" ht="15.75" customHeight="1">
       <c r="A54" s="15"/>
       <c r="B54" s="15"/>
       <c r="C54" s="15"/>
@@ -26636,8 +26772,10 @@
       <c r="W54" s="15"/>
       <c r="X54" s="15"/>
       <c r="Y54" s="15"/>
-    </row>
-    <row r="55" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z54" s="15"/>
+      <c r="AA54" s="15"/>
+    </row>
+    <row r="55" spans="1:27" ht="15.75" customHeight="1">
       <c r="A55" s="15"/>
       <c r="B55" s="15"/>
       <c r="C55" s="15"/>
@@ -26663,8 +26801,10 @@
       <c r="W55" s="15"/>
       <c r="X55" s="15"/>
       <c r="Y55" s="15"/>
-    </row>
-    <row r="56" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z55" s="15"/>
+      <c r="AA55" s="15"/>
+    </row>
+    <row r="56" spans="1:27" ht="15.75" customHeight="1">
       <c r="A56" s="15"/>
       <c r="B56" s="15"/>
       <c r="C56" s="15"/>
@@ -26690,8 +26830,10 @@
       <c r="W56" s="15"/>
       <c r="X56" s="15"/>
       <c r="Y56" s="15"/>
-    </row>
-    <row r="57" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z56" s="15"/>
+      <c r="AA56" s="15"/>
+    </row>
+    <row r="57" spans="1:27" ht="15.75" customHeight="1">
       <c r="A57" s="15"/>
       <c r="B57" s="15"/>
       <c r="C57" s="15"/>
@@ -26717,8 +26859,10 @@
       <c r="W57" s="15"/>
       <c r="X57" s="15"/>
       <c r="Y57" s="15"/>
-    </row>
-    <row r="58" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z57" s="15"/>
+      <c r="AA57" s="15"/>
+    </row>
+    <row r="58" spans="1:27" ht="15.75" customHeight="1">
       <c r="A58" s="15"/>
       <c r="B58" s="15"/>
       <c r="C58" s="15"/>
@@ -26744,8 +26888,10 @@
       <c r="W58" s="15"/>
       <c r="X58" s="15"/>
       <c r="Y58" s="15"/>
-    </row>
-    <row r="59" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z58" s="15"/>
+      <c r="AA58" s="15"/>
+    </row>
+    <row r="59" spans="1:27" ht="15.75" customHeight="1">
       <c r="A59" s="15"/>
       <c r="B59" s="15"/>
       <c r="C59" s="15"/>
@@ -26771,8 +26917,10 @@
       <c r="W59" s="15"/>
       <c r="X59" s="15"/>
       <c r="Y59" s="15"/>
-    </row>
-    <row r="60" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z59" s="15"/>
+      <c r="AA59" s="15"/>
+    </row>
+    <row r="60" spans="1:27" ht="15.75" customHeight="1">
       <c r="A60" s="15"/>
       <c r="B60" s="15"/>
       <c r="C60" s="15"/>
@@ -26798,8 +26946,10 @@
       <c r="W60" s="15"/>
       <c r="X60" s="15"/>
       <c r="Y60" s="15"/>
-    </row>
-    <row r="61" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z60" s="15"/>
+      <c r="AA60" s="15"/>
+    </row>
+    <row r="61" spans="1:27" ht="15.75" customHeight="1">
       <c r="A61" s="15"/>
       <c r="B61" s="15"/>
       <c r="C61" s="15"/>
@@ -26825,8 +26975,10 @@
       <c r="W61" s="15"/>
       <c r="X61" s="15"/>
       <c r="Y61" s="15"/>
-    </row>
-    <row r="62" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z61" s="15"/>
+      <c r="AA61" s="15"/>
+    </row>
+    <row r="62" spans="1:27" ht="15.75" customHeight="1">
       <c r="A62" s="15"/>
       <c r="B62" s="15"/>
       <c r="C62" s="15"/>
@@ -26852,8 +27004,10 @@
       <c r="W62" s="15"/>
       <c r="X62" s="15"/>
       <c r="Y62" s="15"/>
-    </row>
-    <row r="63" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z62" s="15"/>
+      <c r="AA62" s="15"/>
+    </row>
+    <row r="63" spans="1:27" ht="15.75" customHeight="1">
       <c r="A63" s="15"/>
       <c r="B63" s="15"/>
       <c r="C63" s="15"/>
@@ -26879,8 +27033,10 @@
       <c r="W63" s="15"/>
       <c r="X63" s="15"/>
       <c r="Y63" s="15"/>
-    </row>
-    <row r="64" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z63" s="15"/>
+      <c r="AA63" s="15"/>
+    </row>
+    <row r="64" spans="1:27" ht="15.75" customHeight="1">
       <c r="A64" s="15"/>
       <c r="B64" s="15"/>
       <c r="C64" s="15"/>
@@ -26906,8 +27062,10 @@
       <c r="W64" s="15"/>
       <c r="X64" s="15"/>
       <c r="Y64" s="15"/>
-    </row>
-    <row r="65" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z64" s="15"/>
+      <c r="AA64" s="15"/>
+    </row>
+    <row r="65" spans="1:27" ht="15.75" customHeight="1">
       <c r="A65" s="15"/>
       <c r="B65" s="15"/>
       <c r="C65" s="15"/>
@@ -26933,8 +27091,10 @@
       <c r="W65" s="15"/>
       <c r="X65" s="15"/>
       <c r="Y65" s="15"/>
-    </row>
-    <row r="66" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z65" s="15"/>
+      <c r="AA65" s="15"/>
+    </row>
+    <row r="66" spans="1:27" ht="15.75" customHeight="1">
       <c r="A66" s="15"/>
       <c r="B66" s="15"/>
       <c r="C66" s="15"/>
@@ -26960,8 +27120,10 @@
       <c r="W66" s="15"/>
       <c r="X66" s="15"/>
       <c r="Y66" s="15"/>
-    </row>
-    <row r="67" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z66" s="15"/>
+      <c r="AA66" s="15"/>
+    </row>
+    <row r="67" spans="1:27" ht="15.75" customHeight="1">
       <c r="A67" s="15"/>
       <c r="B67" s="15"/>
       <c r="C67" s="15"/>
@@ -26987,8 +27149,10 @@
       <c r="W67" s="15"/>
       <c r="X67" s="15"/>
       <c r="Y67" s="15"/>
-    </row>
-    <row r="68" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z67" s="15"/>
+      <c r="AA67" s="15"/>
+    </row>
+    <row r="68" spans="1:27" ht="15.75" customHeight="1">
       <c r="A68" s="15"/>
       <c r="B68" s="15"/>
       <c r="C68" s="15"/>
@@ -27014,8 +27178,10 @@
       <c r="W68" s="15"/>
       <c r="X68" s="15"/>
       <c r="Y68" s="15"/>
-    </row>
-    <row r="69" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z68" s="15"/>
+      <c r="AA68" s="15"/>
+    </row>
+    <row r="69" spans="1:27" ht="15.75" customHeight="1">
       <c r="A69" s="15"/>
       <c r="B69" s="15"/>
       <c r="C69" s="15"/>
@@ -27041,8 +27207,10 @@
       <c r="W69" s="15"/>
       <c r="X69" s="15"/>
       <c r="Y69" s="15"/>
-    </row>
-    <row r="70" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z69" s="15"/>
+      <c r="AA69" s="15"/>
+    </row>
+    <row r="70" spans="1:27" ht="15.75" customHeight="1">
       <c r="A70" s="15"/>
       <c r="B70" s="15"/>
       <c r="C70" s="15"/>
@@ -27068,8 +27236,10 @@
       <c r="W70" s="15"/>
       <c r="X70" s="15"/>
       <c r="Y70" s="15"/>
-    </row>
-    <row r="71" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z70" s="15"/>
+      <c r="AA70" s="15"/>
+    </row>
+    <row r="71" spans="1:27" ht="15.75" customHeight="1">
       <c r="A71" s="15"/>
       <c r="B71" s="15"/>
       <c r="C71" s="15"/>
@@ -27095,8 +27265,10 @@
       <c r="W71" s="15"/>
       <c r="X71" s="15"/>
       <c r="Y71" s="15"/>
-    </row>
-    <row r="72" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z71" s="15"/>
+      <c r="AA71" s="15"/>
+    </row>
+    <row r="72" spans="1:27" ht="15.75" customHeight="1">
       <c r="A72" s="15"/>
       <c r="B72" s="15"/>
       <c r="C72" s="15"/>
@@ -27122,8 +27294,10 @@
       <c r="W72" s="15"/>
       <c r="X72" s="15"/>
       <c r="Y72" s="15"/>
-    </row>
-    <row r="73" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z72" s="15"/>
+      <c r="AA72" s="15"/>
+    </row>
+    <row r="73" spans="1:27" ht="15.75" customHeight="1">
       <c r="A73" s="15"/>
       <c r="B73" s="15"/>
       <c r="C73" s="15"/>
@@ -27149,8 +27323,10 @@
       <c r="W73" s="15"/>
       <c r="X73" s="15"/>
       <c r="Y73" s="15"/>
-    </row>
-    <row r="74" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z73" s="15"/>
+      <c r="AA73" s="15"/>
+    </row>
+    <row r="74" spans="1:27" ht="15.75" customHeight="1">
       <c r="A74" s="15"/>
       <c r="B74" s="15"/>
       <c r="C74" s="15"/>
@@ -27176,8 +27352,10 @@
       <c r="W74" s="15"/>
       <c r="X74" s="15"/>
       <c r="Y74" s="15"/>
-    </row>
-    <row r="75" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z74" s="15"/>
+      <c r="AA74" s="15"/>
+    </row>
+    <row r="75" spans="1:27" ht="15.75" customHeight="1">
       <c r="A75" s="15"/>
       <c r="B75" s="15"/>
       <c r="C75" s="15"/>
@@ -27203,8 +27381,10 @@
       <c r="W75" s="15"/>
       <c r="X75" s="15"/>
       <c r="Y75" s="15"/>
-    </row>
-    <row r="76" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z75" s="15"/>
+      <c r="AA75" s="15"/>
+    </row>
+    <row r="76" spans="1:27" ht="15.75" customHeight="1">
       <c r="A76" s="15"/>
       <c r="B76" s="15"/>
       <c r="C76" s="15"/>
@@ -27230,8 +27410,10 @@
       <c r="W76" s="15"/>
       <c r="X76" s="15"/>
       <c r="Y76" s="15"/>
-    </row>
-    <row r="77" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z76" s="15"/>
+      <c r="AA76" s="15"/>
+    </row>
+    <row r="77" spans="1:27" ht="15.75" customHeight="1">
       <c r="A77" s="15"/>
       <c r="B77" s="15"/>
       <c r="C77" s="15"/>
@@ -27257,8 +27439,10 @@
       <c r="W77" s="15"/>
       <c r="X77" s="15"/>
       <c r="Y77" s="15"/>
-    </row>
-    <row r="78" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z77" s="15"/>
+      <c r="AA77" s="15"/>
+    </row>
+    <row r="78" spans="1:27" ht="15.75" customHeight="1">
       <c r="A78" s="15"/>
       <c r="B78" s="15"/>
       <c r="C78" s="15"/>
@@ -27284,8 +27468,10 @@
       <c r="W78" s="15"/>
       <c r="X78" s="15"/>
       <c r="Y78" s="15"/>
-    </row>
-    <row r="79" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z78" s="15"/>
+      <c r="AA78" s="15"/>
+    </row>
+    <row r="79" spans="1:27" ht="15.75" customHeight="1">
       <c r="A79" s="15"/>
       <c r="B79" s="15"/>
       <c r="C79" s="15"/>
@@ -27311,8 +27497,10 @@
       <c r="W79" s="15"/>
       <c r="X79" s="15"/>
       <c r="Y79" s="15"/>
-    </row>
-    <row r="80" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z79" s="15"/>
+      <c r="AA79" s="15"/>
+    </row>
+    <row r="80" spans="1:27" ht="15.75" customHeight="1">
       <c r="A80" s="15"/>
       <c r="B80" s="15"/>
       <c r="C80" s="15"/>
@@ -27338,8 +27526,10 @@
       <c r="W80" s="15"/>
       <c r="X80" s="15"/>
       <c r="Y80" s="15"/>
-    </row>
-    <row r="81" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z80" s="15"/>
+      <c r="AA80" s="15"/>
+    </row>
+    <row r="81" spans="1:27" ht="15.75" customHeight="1">
       <c r="A81" s="15"/>
       <c r="B81" s="15"/>
       <c r="C81" s="15"/>
@@ -27365,8 +27555,10 @@
       <c r="W81" s="15"/>
       <c r="X81" s="15"/>
       <c r="Y81" s="15"/>
-    </row>
-    <row r="82" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z81" s="15"/>
+      <c r="AA81" s="15"/>
+    </row>
+    <row r="82" spans="1:27" ht="15.75" customHeight="1">
       <c r="A82" s="15"/>
       <c r="B82" s="15"/>
       <c r="C82" s="15"/>
@@ -27392,8 +27584,10 @@
       <c r="W82" s="15"/>
       <c r="X82" s="15"/>
       <c r="Y82" s="15"/>
-    </row>
-    <row r="83" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z82" s="15"/>
+      <c r="AA82" s="15"/>
+    </row>
+    <row r="83" spans="1:27" ht="15.75" customHeight="1">
       <c r="A83" s="15"/>
       <c r="B83" s="15"/>
       <c r="C83" s="15"/>
@@ -27419,8 +27613,10 @@
       <c r="W83" s="15"/>
       <c r="X83" s="15"/>
       <c r="Y83" s="15"/>
-    </row>
-    <row r="84" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z83" s="15"/>
+      <c r="AA83" s="15"/>
+    </row>
+    <row r="84" spans="1:27" ht="15.75" customHeight="1">
       <c r="A84" s="15"/>
       <c r="B84" s="15"/>
       <c r="C84" s="15"/>
@@ -27446,8 +27642,10 @@
       <c r="W84" s="15"/>
       <c r="X84" s="15"/>
       <c r="Y84" s="15"/>
-    </row>
-    <row r="85" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z84" s="15"/>
+      <c r="AA84" s="15"/>
+    </row>
+    <row r="85" spans="1:27" ht="15.75" customHeight="1">
       <c r="A85" s="15"/>
       <c r="B85" s="15"/>
       <c r="C85" s="15"/>
@@ -27473,8 +27671,10 @@
       <c r="W85" s="15"/>
       <c r="X85" s="15"/>
       <c r="Y85" s="15"/>
-    </row>
-    <row r="86" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z85" s="15"/>
+      <c r="AA85" s="15"/>
+    </row>
+    <row r="86" spans="1:27" ht="15.75" customHeight="1">
       <c r="A86" s="15"/>
       <c r="B86" s="15"/>
       <c r="C86" s="15"/>
@@ -27500,8 +27700,10 @@
       <c r="W86" s="15"/>
       <c r="X86" s="15"/>
       <c r="Y86" s="15"/>
-    </row>
-    <row r="87" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z86" s="15"/>
+      <c r="AA86" s="15"/>
+    </row>
+    <row r="87" spans="1:27" ht="15.75" customHeight="1">
       <c r="A87" s="15"/>
       <c r="B87" s="15"/>
       <c r="C87" s="15"/>
@@ -27527,8 +27729,10 @@
       <c r="W87" s="15"/>
       <c r="X87" s="15"/>
       <c r="Y87" s="15"/>
-    </row>
-    <row r="88" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z87" s="15"/>
+      <c r="AA87" s="15"/>
+    </row>
+    <row r="88" spans="1:27" ht="15.75" customHeight="1">
       <c r="A88" s="15"/>
       <c r="B88" s="15"/>
       <c r="C88" s="15"/>
@@ -27554,8 +27758,10 @@
       <c r="W88" s="15"/>
       <c r="X88" s="15"/>
       <c r="Y88" s="15"/>
-    </row>
-    <row r="89" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z88" s="15"/>
+      <c r="AA88" s="15"/>
+    </row>
+    <row r="89" spans="1:27" ht="15.75" customHeight="1">
       <c r="A89" s="15"/>
       <c r="B89" s="15"/>
       <c r="C89" s="15"/>
@@ -27581,8 +27787,10 @@
       <c r="W89" s="15"/>
       <c r="X89" s="15"/>
       <c r="Y89" s="15"/>
-    </row>
-    <row r="90" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z89" s="15"/>
+      <c r="AA89" s="15"/>
+    </row>
+    <row r="90" spans="1:27" ht="15.75" customHeight="1">
       <c r="A90" s="15"/>
       <c r="B90" s="15"/>
       <c r="C90" s="15"/>
@@ -27608,8 +27816,10 @@
       <c r="W90" s="15"/>
       <c r="X90" s="15"/>
       <c r="Y90" s="15"/>
-    </row>
-    <row r="91" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z90" s="15"/>
+      <c r="AA90" s="15"/>
+    </row>
+    <row r="91" spans="1:27" ht="15.75" customHeight="1">
       <c r="A91" s="15"/>
       <c r="B91" s="15"/>
       <c r="C91" s="15"/>
@@ -27635,8 +27845,10 @@
       <c r="W91" s="15"/>
       <c r="X91" s="15"/>
       <c r="Y91" s="15"/>
-    </row>
-    <row r="92" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z91" s="15"/>
+      <c r="AA91" s="15"/>
+    </row>
+    <row r="92" spans="1:27" ht="15.75" customHeight="1">
       <c r="A92" s="15"/>
       <c r="B92" s="15"/>
       <c r="C92" s="15"/>
@@ -27662,8 +27874,10 @@
       <c r="W92" s="15"/>
       <c r="X92" s="15"/>
       <c r="Y92" s="15"/>
-    </row>
-    <row r="93" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z92" s="15"/>
+      <c r="AA92" s="15"/>
+    </row>
+    <row r="93" spans="1:27" ht="15.75" customHeight="1">
       <c r="A93" s="15"/>
       <c r="B93" s="15"/>
       <c r="C93" s="15"/>
@@ -27689,8 +27903,10 @@
       <c r="W93" s="15"/>
       <c r="X93" s="15"/>
       <c r="Y93" s="15"/>
-    </row>
-    <row r="94" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z93" s="15"/>
+      <c r="AA93" s="15"/>
+    </row>
+    <row r="94" spans="1:27" ht="15.75" customHeight="1">
       <c r="A94" s="15"/>
       <c r="B94" s="15"/>
       <c r="C94" s="15"/>
@@ -27716,8 +27932,10 @@
       <c r="W94" s="15"/>
       <c r="X94" s="15"/>
       <c r="Y94" s="15"/>
-    </row>
-    <row r="95" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z94" s="15"/>
+      <c r="AA94" s="15"/>
+    </row>
+    <row r="95" spans="1:27" ht="15.75" customHeight="1">
       <c r="A95" s="15"/>
       <c r="B95" s="15"/>
       <c r="C95" s="15"/>
@@ -27743,8 +27961,10 @@
       <c r="W95" s="15"/>
       <c r="X95" s="15"/>
       <c r="Y95" s="15"/>
-    </row>
-    <row r="96" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z95" s="15"/>
+      <c r="AA95" s="15"/>
+    </row>
+    <row r="96" spans="1:27" ht="15.75" customHeight="1">
       <c r="A96" s="15"/>
       <c r="B96" s="15"/>
       <c r="C96" s="15"/>
@@ -27770,8 +27990,10 @@
       <c r="W96" s="15"/>
       <c r="X96" s="15"/>
       <c r="Y96" s="15"/>
-    </row>
-    <row r="97" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z96" s="15"/>
+      <c r="AA96" s="15"/>
+    </row>
+    <row r="97" spans="1:27" ht="15.75" customHeight="1">
       <c r="A97" s="15"/>
       <c r="B97" s="15"/>
       <c r="C97" s="15"/>
@@ -27797,8 +28019,10 @@
       <c r="W97" s="15"/>
       <c r="X97" s="15"/>
       <c r="Y97" s="15"/>
-    </row>
-    <row r="98" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z97" s="15"/>
+      <c r="AA97" s="15"/>
+    </row>
+    <row r="98" spans="1:27" ht="15.75" customHeight="1">
       <c r="A98" s="15"/>
       <c r="B98" s="15"/>
       <c r="C98" s="15"/>
@@ -27824,8 +28048,10 @@
       <c r="W98" s="15"/>
       <c r="X98" s="15"/>
       <c r="Y98" s="15"/>
-    </row>
-    <row r="99" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z98" s="15"/>
+      <c r="AA98" s="15"/>
+    </row>
+    <row r="99" spans="1:27" ht="15.75" customHeight="1">
       <c r="A99" s="15"/>
       <c r="B99" s="15"/>
       <c r="C99" s="15"/>
@@ -27851,8 +28077,10 @@
       <c r="W99" s="15"/>
       <c r="X99" s="15"/>
       <c r="Y99" s="15"/>
-    </row>
-    <row r="100" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z99" s="15"/>
+      <c r="AA99" s="15"/>
+    </row>
+    <row r="100" spans="1:27" ht="15.75" customHeight="1">
       <c r="A100" s="15"/>
       <c r="B100" s="15"/>
       <c r="C100" s="15"/>
@@ -27878,8 +28106,10 @@
       <c r="W100" s="15"/>
       <c r="X100" s="15"/>
       <c r="Y100" s="15"/>
-    </row>
-    <row r="101" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z100" s="15"/>
+      <c r="AA100" s="15"/>
+    </row>
+    <row r="101" spans="1:27" ht="15.75" customHeight="1">
       <c r="A101" s="15"/>
       <c r="B101" s="15"/>
       <c r="C101" s="15"/>
@@ -27905,8 +28135,10 @@
       <c r="W101" s="15"/>
       <c r="X101" s="15"/>
       <c r="Y101" s="15"/>
-    </row>
-    <row r="102" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z101" s="15"/>
+      <c r="AA101" s="15"/>
+    </row>
+    <row r="102" spans="1:27" ht="15.75" customHeight="1">
       <c r="A102" s="15"/>
       <c r="B102" s="15"/>
       <c r="C102" s="15"/>
@@ -27932,8 +28164,10 @@
       <c r="W102" s="15"/>
       <c r="X102" s="15"/>
       <c r="Y102" s="15"/>
-    </row>
-    <row r="103" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z102" s="15"/>
+      <c r="AA102" s="15"/>
+    </row>
+    <row r="103" spans="1:27" ht="15.75" customHeight="1">
       <c r="A103" s="15"/>
       <c r="B103" s="15"/>
       <c r="C103" s="15"/>
@@ -27959,8 +28193,10 @@
       <c r="W103" s="15"/>
       <c r="X103" s="15"/>
       <c r="Y103" s="15"/>
-    </row>
-    <row r="104" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z103" s="15"/>
+      <c r="AA103" s="15"/>
+    </row>
+    <row r="104" spans="1:27" ht="15.75" customHeight="1">
       <c r="A104" s="15"/>
       <c r="B104" s="15"/>
       <c r="C104" s="15"/>
@@ -27986,8 +28222,10 @@
       <c r="W104" s="15"/>
       <c r="X104" s="15"/>
       <c r="Y104" s="15"/>
-    </row>
-    <row r="105" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z104" s="15"/>
+      <c r="AA104" s="15"/>
+    </row>
+    <row r="105" spans="1:27" ht="15.75" customHeight="1">
       <c r="A105" s="15"/>
       <c r="B105" s="15"/>
       <c r="C105" s="15"/>
@@ -28013,8 +28251,10 @@
       <c r="W105" s="15"/>
       <c r="X105" s="15"/>
       <c r="Y105" s="15"/>
-    </row>
-    <row r="106" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z105" s="15"/>
+      <c r="AA105" s="15"/>
+    </row>
+    <row r="106" spans="1:27" ht="15.75" customHeight="1">
       <c r="A106" s="15"/>
       <c r="B106" s="15"/>
       <c r="C106" s="15"/>
@@ -28040,8 +28280,10 @@
       <c r="W106" s="15"/>
       <c r="X106" s="15"/>
       <c r="Y106" s="15"/>
-    </row>
-    <row r="107" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z106" s="15"/>
+      <c r="AA106" s="15"/>
+    </row>
+    <row r="107" spans="1:27" ht="15.75" customHeight="1">
       <c r="A107" s="15"/>
       <c r="B107" s="15"/>
       <c r="C107" s="15"/>
@@ -28067,8 +28309,10 @@
       <c r="W107" s="15"/>
       <c r="X107" s="15"/>
       <c r="Y107" s="15"/>
-    </row>
-    <row r="108" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z107" s="15"/>
+      <c r="AA107" s="15"/>
+    </row>
+    <row r="108" spans="1:27" ht="15.75" customHeight="1">
       <c r="A108" s="15"/>
       <c r="B108" s="15"/>
       <c r="C108" s="15"/>
@@ -28094,8 +28338,10 @@
       <c r="W108" s="15"/>
       <c r="X108" s="15"/>
       <c r="Y108" s="15"/>
-    </row>
-    <row r="109" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z108" s="15"/>
+      <c r="AA108" s="15"/>
+    </row>
+    <row r="109" spans="1:27" ht="15.75" customHeight="1">
       <c r="A109" s="15"/>
       <c r="B109" s="15"/>
       <c r="C109" s="15"/>
@@ -28121,8 +28367,10 @@
       <c r="W109" s="15"/>
       <c r="X109" s="15"/>
       <c r="Y109" s="15"/>
-    </row>
-    <row r="110" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z109" s="15"/>
+      <c r="AA109" s="15"/>
+    </row>
+    <row r="110" spans="1:27" ht="15.75" customHeight="1">
       <c r="A110" s="15"/>
       <c r="B110" s="15"/>
       <c r="C110" s="15"/>
@@ -28148,8 +28396,10 @@
       <c r="W110" s="15"/>
       <c r="X110" s="15"/>
       <c r="Y110" s="15"/>
-    </row>
-    <row r="111" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z110" s="15"/>
+      <c r="AA110" s="15"/>
+    </row>
+    <row r="111" spans="1:27" ht="15.75" customHeight="1">
       <c r="A111" s="15"/>
       <c r="B111" s="15"/>
       <c r="C111" s="15"/>
@@ -28175,8 +28425,10 @@
       <c r="W111" s="15"/>
       <c r="X111" s="15"/>
       <c r="Y111" s="15"/>
-    </row>
-    <row r="112" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z111" s="15"/>
+      <c r="AA111" s="15"/>
+    </row>
+    <row r="112" spans="1:27" ht="15.75" customHeight="1">
       <c r="A112" s="15"/>
       <c r="B112" s="15"/>
       <c r="C112" s="15"/>
@@ -28202,8 +28454,10 @@
       <c r="W112" s="15"/>
       <c r="X112" s="15"/>
       <c r="Y112" s="15"/>
-    </row>
-    <row r="113" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z112" s="15"/>
+      <c r="AA112" s="15"/>
+    </row>
+    <row r="113" spans="1:27" ht="15.75" customHeight="1">
       <c r="A113" s="15"/>
       <c r="B113" s="15"/>
       <c r="C113" s="15"/>
@@ -28229,8 +28483,10 @@
       <c r="W113" s="15"/>
       <c r="X113" s="15"/>
       <c r="Y113" s="15"/>
-    </row>
-    <row r="114" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z113" s="15"/>
+      <c r="AA113" s="15"/>
+    </row>
+    <row r="114" spans="1:27" ht="15.75" customHeight="1">
       <c r="A114" s="15"/>
       <c r="B114" s="15"/>
       <c r="C114" s="15"/>
@@ -28256,8 +28512,10 @@
       <c r="W114" s="15"/>
       <c r="X114" s="15"/>
       <c r="Y114" s="15"/>
-    </row>
-    <row r="115" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z114" s="15"/>
+      <c r="AA114" s="15"/>
+    </row>
+    <row r="115" spans="1:27" ht="15.75" customHeight="1">
       <c r="A115" s="15"/>
       <c r="B115" s="15"/>
       <c r="C115" s="15"/>
@@ -28283,8 +28541,10 @@
       <c r="W115" s="15"/>
       <c r="X115" s="15"/>
       <c r="Y115" s="15"/>
-    </row>
-    <row r="116" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z115" s="15"/>
+      <c r="AA115" s="15"/>
+    </row>
+    <row r="116" spans="1:27" ht="15.75" customHeight="1">
       <c r="A116" s="15"/>
       <c r="B116" s="15"/>
       <c r="C116" s="15"/>
@@ -28310,8 +28570,10 @@
       <c r="W116" s="15"/>
       <c r="X116" s="15"/>
       <c r="Y116" s="15"/>
-    </row>
-    <row r="117" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z116" s="15"/>
+      <c r="AA116" s="15"/>
+    </row>
+    <row r="117" spans="1:27" ht="15.75" customHeight="1">
       <c r="A117" s="15"/>
       <c r="B117" s="15"/>
       <c r="C117" s="15"/>
@@ -28337,8 +28599,10 @@
       <c r="W117" s="15"/>
       <c r="X117" s="15"/>
       <c r="Y117" s="15"/>
-    </row>
-    <row r="118" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z117" s="15"/>
+      <c r="AA117" s="15"/>
+    </row>
+    <row r="118" spans="1:27" ht="15.75" customHeight="1">
       <c r="A118" s="15"/>
       <c r="B118" s="15"/>
       <c r="C118" s="15"/>
@@ -28364,8 +28628,10 @@
       <c r="W118" s="15"/>
       <c r="X118" s="15"/>
       <c r="Y118" s="15"/>
-    </row>
-    <row r="119" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z118" s="15"/>
+      <c r="AA118" s="15"/>
+    </row>
+    <row r="119" spans="1:27" ht="15.75" customHeight="1">
       <c r="A119" s="15"/>
       <c r="B119" s="15"/>
       <c r="C119" s="15"/>
@@ -28391,8 +28657,10 @@
       <c r="W119" s="15"/>
       <c r="X119" s="15"/>
       <c r="Y119" s="15"/>
-    </row>
-    <row r="120" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z119" s="15"/>
+      <c r="AA119" s="15"/>
+    </row>
+    <row r="120" spans="1:27" ht="15.75" customHeight="1">
       <c r="A120" s="15"/>
       <c r="B120" s="15"/>
       <c r="C120" s="15"/>
@@ -28418,8 +28686,10 @@
       <c r="W120" s="15"/>
       <c r="X120" s="15"/>
       <c r="Y120" s="15"/>
-    </row>
-    <row r="121" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z120" s="15"/>
+      <c r="AA120" s="15"/>
+    </row>
+    <row r="121" spans="1:27" ht="15.75" customHeight="1">
       <c r="A121" s="15"/>
       <c r="B121" s="15"/>
       <c r="C121" s="15"/>
@@ -28445,8 +28715,10 @@
       <c r="W121" s="15"/>
       <c r="X121" s="15"/>
       <c r="Y121" s="15"/>
-    </row>
-    <row r="122" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z121" s="15"/>
+      <c r="AA121" s="15"/>
+    </row>
+    <row r="122" spans="1:27" ht="15.75" customHeight="1">
       <c r="A122" s="15"/>
       <c r="B122" s="15"/>
       <c r="C122" s="15"/>
@@ -28472,8 +28744,10 @@
       <c r="W122" s="15"/>
       <c r="X122" s="15"/>
       <c r="Y122" s="15"/>
-    </row>
-    <row r="123" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z122" s="15"/>
+      <c r="AA122" s="15"/>
+    </row>
+    <row r="123" spans="1:27" ht="15.75" customHeight="1">
       <c r="A123" s="15"/>
       <c r="B123" s="15"/>
       <c r="C123" s="15"/>
@@ -28499,8 +28773,10 @@
       <c r="W123" s="15"/>
       <c r="X123" s="15"/>
       <c r="Y123" s="15"/>
-    </row>
-    <row r="124" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z123" s="15"/>
+      <c r="AA123" s="15"/>
+    </row>
+    <row r="124" spans="1:27" ht="15.75" customHeight="1">
       <c r="A124" s="15"/>
       <c r="B124" s="15"/>
       <c r="C124" s="15"/>
@@ -28526,8 +28802,10 @@
       <c r="W124" s="15"/>
       <c r="X124" s="15"/>
       <c r="Y124" s="15"/>
-    </row>
-    <row r="125" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z124" s="15"/>
+      <c r="AA124" s="15"/>
+    </row>
+    <row r="125" spans="1:27" ht="15.75" customHeight="1">
       <c r="A125" s="15"/>
       <c r="B125" s="15"/>
       <c r="C125" s="15"/>
@@ -28553,8 +28831,10 @@
       <c r="W125" s="15"/>
       <c r="X125" s="15"/>
       <c r="Y125" s="15"/>
-    </row>
-    <row r="126" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z125" s="15"/>
+      <c r="AA125" s="15"/>
+    </row>
+    <row r="126" spans="1:27" ht="15.75" customHeight="1">
       <c r="A126" s="15"/>
       <c r="B126" s="15"/>
       <c r="C126" s="15"/>
@@ -28580,8 +28860,10 @@
       <c r="W126" s="15"/>
       <c r="X126" s="15"/>
       <c r="Y126" s="15"/>
-    </row>
-    <row r="127" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z126" s="15"/>
+      <c r="AA126" s="15"/>
+    </row>
+    <row r="127" spans="1:27" ht="15.75" customHeight="1">
       <c r="A127" s="15"/>
       <c r="B127" s="15"/>
       <c r="C127" s="15"/>
@@ -28607,8 +28889,10 @@
       <c r="W127" s="15"/>
       <c r="X127" s="15"/>
       <c r="Y127" s="15"/>
-    </row>
-    <row r="128" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z127" s="15"/>
+      <c r="AA127" s="15"/>
+    </row>
+    <row r="128" spans="1:27" ht="15.75" customHeight="1">
       <c r="A128" s="15"/>
       <c r="B128" s="15"/>
       <c r="C128" s="15"/>
@@ -28634,8 +28918,10 @@
       <c r="W128" s="15"/>
       <c r="X128" s="15"/>
       <c r="Y128" s="15"/>
-    </row>
-    <row r="129" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z128" s="15"/>
+      <c r="AA128" s="15"/>
+    </row>
+    <row r="129" spans="1:27" ht="15.75" customHeight="1">
       <c r="A129" s="15"/>
       <c r="B129" s="15"/>
       <c r="C129" s="15"/>
@@ -28661,8 +28947,10 @@
       <c r="W129" s="15"/>
       <c r="X129" s="15"/>
       <c r="Y129" s="15"/>
-    </row>
-    <row r="130" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z129" s="15"/>
+      <c r="AA129" s="15"/>
+    </row>
+    <row r="130" spans="1:27" ht="15.75" customHeight="1">
       <c r="A130" s="15"/>
       <c r="B130" s="15"/>
       <c r="C130" s="15"/>
@@ -28688,8 +28976,10 @@
       <c r="W130" s="15"/>
       <c r="X130" s="15"/>
       <c r="Y130" s="15"/>
-    </row>
-    <row r="131" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z130" s="15"/>
+      <c r="AA130" s="15"/>
+    </row>
+    <row r="131" spans="1:27" ht="15.75" customHeight="1">
       <c r="A131" s="15"/>
       <c r="B131" s="15"/>
       <c r="C131" s="15"/>
@@ -28715,8 +29005,10 @@
       <c r="W131" s="15"/>
       <c r="X131" s="15"/>
       <c r="Y131" s="15"/>
-    </row>
-    <row r="132" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z131" s="15"/>
+      <c r="AA131" s="15"/>
+    </row>
+    <row r="132" spans="1:27" ht="15.75" customHeight="1">
       <c r="A132" s="15"/>
       <c r="B132" s="15"/>
       <c r="C132" s="15"/>
@@ -28742,8 +29034,10 @@
       <c r="W132" s="15"/>
       <c r="X132" s="15"/>
       <c r="Y132" s="15"/>
-    </row>
-    <row r="133" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z132" s="15"/>
+      <c r="AA132" s="15"/>
+    </row>
+    <row r="133" spans="1:27" ht="15.75" customHeight="1">
       <c r="A133" s="15"/>
       <c r="B133" s="15"/>
       <c r="C133" s="15"/>
@@ -28769,8 +29063,10 @@
       <c r="W133" s="15"/>
       <c r="X133" s="15"/>
       <c r="Y133" s="15"/>
-    </row>
-    <row r="134" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z133" s="15"/>
+      <c r="AA133" s="15"/>
+    </row>
+    <row r="134" spans="1:27" ht="15.75" customHeight="1">
       <c r="A134" s="15"/>
       <c r="B134" s="15"/>
       <c r="C134" s="15"/>
@@ -28796,8 +29092,10 @@
       <c r="W134" s="15"/>
       <c r="X134" s="15"/>
       <c r="Y134" s="15"/>
-    </row>
-    <row r="135" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z134" s="15"/>
+      <c r="AA134" s="15"/>
+    </row>
+    <row r="135" spans="1:27" ht="15.75" customHeight="1">
       <c r="A135" s="15"/>
       <c r="B135" s="15"/>
       <c r="C135" s="15"/>
@@ -28823,8 +29121,10 @@
       <c r="W135" s="15"/>
       <c r="X135" s="15"/>
       <c r="Y135" s="15"/>
-    </row>
-    <row r="136" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z135" s="15"/>
+      <c r="AA135" s="15"/>
+    </row>
+    <row r="136" spans="1:27" ht="15.75" customHeight="1">
       <c r="A136" s="15"/>
       <c r="B136" s="15"/>
       <c r="C136" s="15"/>
@@ -28850,8 +29150,10 @@
       <c r="W136" s="15"/>
       <c r="X136" s="15"/>
       <c r="Y136" s="15"/>
-    </row>
-    <row r="137" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z136" s="15"/>
+      <c r="AA136" s="15"/>
+    </row>
+    <row r="137" spans="1:27" ht="15.75" customHeight="1">
       <c r="A137" s="15"/>
       <c r="B137" s="15"/>
       <c r="C137" s="15"/>
@@ -28877,8 +29179,10 @@
       <c r="W137" s="15"/>
       <c r="X137" s="15"/>
       <c r="Y137" s="15"/>
-    </row>
-    <row r="138" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z137" s="15"/>
+      <c r="AA137" s="15"/>
+    </row>
+    <row r="138" spans="1:27" ht="15.75" customHeight="1">
       <c r="A138" s="15"/>
       <c r="B138" s="15"/>
       <c r="C138" s="15"/>
@@ -28904,8 +29208,10 @@
       <c r="W138" s="15"/>
       <c r="X138" s="15"/>
       <c r="Y138" s="15"/>
-    </row>
-    <row r="139" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z138" s="15"/>
+      <c r="AA138" s="15"/>
+    </row>
+    <row r="139" spans="1:27" ht="15.75" customHeight="1">
       <c r="A139" s="15"/>
       <c r="B139" s="15"/>
       <c r="C139" s="15"/>
@@ -28931,8 +29237,10 @@
       <c r="W139" s="15"/>
       <c r="X139" s="15"/>
       <c r="Y139" s="15"/>
-    </row>
-    <row r="140" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z139" s="15"/>
+      <c r="AA139" s="15"/>
+    </row>
+    <row r="140" spans="1:27" ht="15.75" customHeight="1">
       <c r="A140" s="15"/>
       <c r="B140" s="15"/>
       <c r="C140" s="15"/>
@@ -28958,8 +29266,10 @@
       <c r="W140" s="15"/>
       <c r="X140" s="15"/>
       <c r="Y140" s="15"/>
-    </row>
-    <row r="141" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z140" s="15"/>
+      <c r="AA140" s="15"/>
+    </row>
+    <row r="141" spans="1:27" ht="15.75" customHeight="1">
       <c r="A141" s="15"/>
       <c r="B141" s="15"/>
       <c r="C141" s="15"/>
@@ -28985,8 +29295,10 @@
       <c r="W141" s="15"/>
       <c r="X141" s="15"/>
       <c r="Y141" s="15"/>
-    </row>
-    <row r="142" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z141" s="15"/>
+      <c r="AA141" s="15"/>
+    </row>
+    <row r="142" spans="1:27" ht="15.75" customHeight="1">
       <c r="A142" s="15"/>
       <c r="B142" s="15"/>
       <c r="C142" s="15"/>
@@ -29012,8 +29324,10 @@
       <c r="W142" s="15"/>
       <c r="X142" s="15"/>
       <c r="Y142" s="15"/>
-    </row>
-    <row r="143" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z142" s="15"/>
+      <c r="AA142" s="15"/>
+    </row>
+    <row r="143" spans="1:27" ht="15.75" customHeight="1">
       <c r="A143" s="15"/>
       <c r="B143" s="15"/>
       <c r="C143" s="15"/>
@@ -29039,8 +29353,10 @@
       <c r="W143" s="15"/>
       <c r="X143" s="15"/>
       <c r="Y143" s="15"/>
-    </row>
-    <row r="144" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z143" s="15"/>
+      <c r="AA143" s="15"/>
+    </row>
+    <row r="144" spans="1:27" ht="15.75" customHeight="1">
       <c r="A144" s="15"/>
       <c r="B144" s="15"/>
       <c r="C144" s="15"/>
@@ -29066,8 +29382,10 @@
       <c r="W144" s="15"/>
       <c r="X144" s="15"/>
       <c r="Y144" s="15"/>
-    </row>
-    <row r="145" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z144" s="15"/>
+      <c r="AA144" s="15"/>
+    </row>
+    <row r="145" spans="1:27" ht="15.75" customHeight="1">
       <c r="A145" s="15"/>
       <c r="B145" s="15"/>
       <c r="C145" s="15"/>
@@ -29093,8 +29411,10 @@
       <c r="W145" s="15"/>
       <c r="X145" s="15"/>
       <c r="Y145" s="15"/>
-    </row>
-    <row r="146" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z145" s="15"/>
+      <c r="AA145" s="15"/>
+    </row>
+    <row r="146" spans="1:27" ht="15.75" customHeight="1">
       <c r="A146" s="15"/>
       <c r="B146" s="15"/>
       <c r="C146" s="15"/>
@@ -29120,8 +29440,10 @@
       <c r="W146" s="15"/>
       <c r="X146" s="15"/>
       <c r="Y146" s="15"/>
-    </row>
-    <row r="147" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z146" s="15"/>
+      <c r="AA146" s="15"/>
+    </row>
+    <row r="147" spans="1:27" ht="15.75" customHeight="1">
       <c r="A147" s="15"/>
       <c r="B147" s="15"/>
       <c r="C147" s="15"/>
@@ -29147,8 +29469,10 @@
       <c r="W147" s="15"/>
       <c r="X147" s="15"/>
       <c r="Y147" s="15"/>
-    </row>
-    <row r="148" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z147" s="15"/>
+      <c r="AA147" s="15"/>
+    </row>
+    <row r="148" spans="1:27" ht="15.75" customHeight="1">
       <c r="A148" s="15"/>
       <c r="B148" s="15"/>
       <c r="C148" s="15"/>
@@ -29174,8 +29498,10 @@
       <c r="W148" s="15"/>
       <c r="X148" s="15"/>
       <c r="Y148" s="15"/>
-    </row>
-    <row r="149" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z148" s="15"/>
+      <c r="AA148" s="15"/>
+    </row>
+    <row r="149" spans="1:27" ht="15.75" customHeight="1">
       <c r="A149" s="15"/>
       <c r="B149" s="15"/>
       <c r="C149" s="15"/>
@@ -29201,8 +29527,10 @@
       <c r="W149" s="15"/>
       <c r="X149" s="15"/>
       <c r="Y149" s="15"/>
-    </row>
-    <row r="150" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z149" s="15"/>
+      <c r="AA149" s="15"/>
+    </row>
+    <row r="150" spans="1:27" ht="15.75" customHeight="1">
       <c r="A150" s="15"/>
       <c r="B150" s="15"/>
       <c r="C150" s="15"/>
@@ -29228,8 +29556,10 @@
       <c r="W150" s="15"/>
       <c r="X150" s="15"/>
       <c r="Y150" s="15"/>
-    </row>
-    <row r="151" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z150" s="15"/>
+      <c r="AA150" s="15"/>
+    </row>
+    <row r="151" spans="1:27" ht="15.75" customHeight="1">
       <c r="A151" s="15"/>
       <c r="B151" s="15"/>
       <c r="C151" s="15"/>
@@ -29255,8 +29585,10 @@
       <c r="W151" s="15"/>
       <c r="X151" s="15"/>
       <c r="Y151" s="15"/>
-    </row>
-    <row r="152" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z151" s="15"/>
+      <c r="AA151" s="15"/>
+    </row>
+    <row r="152" spans="1:27" ht="15.75" customHeight="1">
       <c r="A152" s="15"/>
       <c r="B152" s="15"/>
       <c r="C152" s="15"/>
@@ -29282,8 +29614,10 @@
       <c r="W152" s="15"/>
       <c r="X152" s="15"/>
       <c r="Y152" s="15"/>
-    </row>
-    <row r="153" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z152" s="15"/>
+      <c r="AA152" s="15"/>
+    </row>
+    <row r="153" spans="1:27" ht="15.75" customHeight="1">
       <c r="A153" s="15"/>
       <c r="B153" s="15"/>
       <c r="C153" s="15"/>
@@ -29309,8 +29643,10 @@
       <c r="W153" s="15"/>
       <c r="X153" s="15"/>
       <c r="Y153" s="15"/>
-    </row>
-    <row r="154" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z153" s="15"/>
+      <c r="AA153" s="15"/>
+    </row>
+    <row r="154" spans="1:27" ht="15.75" customHeight="1">
       <c r="A154" s="15"/>
       <c r="B154" s="15"/>
       <c r="C154" s="15"/>
@@ -29336,8 +29672,10 @@
       <c r="W154" s="15"/>
       <c r="X154" s="15"/>
       <c r="Y154" s="15"/>
-    </row>
-    <row r="155" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z154" s="15"/>
+      <c r="AA154" s="15"/>
+    </row>
+    <row r="155" spans="1:27" ht="15.75" customHeight="1">
       <c r="A155" s="15"/>
       <c r="B155" s="15"/>
       <c r="C155" s="15"/>
@@ -29363,8 +29701,10 @@
       <c r="W155" s="15"/>
       <c r="X155" s="15"/>
       <c r="Y155" s="15"/>
-    </row>
-    <row r="156" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z155" s="15"/>
+      <c r="AA155" s="15"/>
+    </row>
+    <row r="156" spans="1:27" ht="15.75" customHeight="1">
       <c r="A156" s="15"/>
       <c r="B156" s="15"/>
       <c r="C156" s="15"/>
@@ -29390,8 +29730,10 @@
       <c r="W156" s="15"/>
       <c r="X156" s="15"/>
       <c r="Y156" s="15"/>
-    </row>
-    <row r="157" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z156" s="15"/>
+      <c r="AA156" s="15"/>
+    </row>
+    <row r="157" spans="1:27" ht="15.75" customHeight="1">
       <c r="A157" s="15"/>
       <c r="B157" s="15"/>
       <c r="C157" s="15"/>
@@ -29417,8 +29759,10 @@
       <c r="W157" s="15"/>
       <c r="X157" s="15"/>
       <c r="Y157" s="15"/>
-    </row>
-    <row r="158" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z157" s="15"/>
+      <c r="AA157" s="15"/>
+    </row>
+    <row r="158" spans="1:27" ht="15.75" customHeight="1">
       <c r="A158" s="15"/>
       <c r="B158" s="15"/>
       <c r="C158" s="15"/>
@@ -29444,8 +29788,10 @@
       <c r="W158" s="15"/>
       <c r="X158" s="15"/>
       <c r="Y158" s="15"/>
-    </row>
-    <row r="159" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z158" s="15"/>
+      <c r="AA158" s="15"/>
+    </row>
+    <row r="159" spans="1:27" ht="15.75" customHeight="1">
       <c r="A159" s="15"/>
       <c r="B159" s="15"/>
       <c r="C159" s="15"/>
@@ -29471,8 +29817,10 @@
       <c r="W159" s="15"/>
       <c r="X159" s="15"/>
       <c r="Y159" s="15"/>
-    </row>
-    <row r="160" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z159" s="15"/>
+      <c r="AA159" s="15"/>
+    </row>
+    <row r="160" spans="1:27" ht="15.75" customHeight="1">
       <c r="A160" s="15"/>
       <c r="B160" s="15"/>
       <c r="C160" s="15"/>
@@ -29498,8 +29846,10 @@
       <c r="W160" s="15"/>
       <c r="X160" s="15"/>
       <c r="Y160" s="15"/>
-    </row>
-    <row r="161" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z160" s="15"/>
+      <c r="AA160" s="15"/>
+    </row>
+    <row r="161" spans="1:27" ht="15.75" customHeight="1">
       <c r="A161" s="15"/>
       <c r="B161" s="15"/>
       <c r="C161" s="15"/>
@@ -29525,8 +29875,10 @@
       <c r="W161" s="15"/>
       <c r="X161" s="15"/>
       <c r="Y161" s="15"/>
-    </row>
-    <row r="162" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z161" s="15"/>
+      <c r="AA161" s="15"/>
+    </row>
+    <row r="162" spans="1:27" ht="15.75" customHeight="1">
       <c r="A162" s="15"/>
       <c r="B162" s="15"/>
       <c r="C162" s="15"/>
@@ -29552,8 +29904,10 @@
       <c r="W162" s="15"/>
       <c r="X162" s="15"/>
       <c r="Y162" s="15"/>
-    </row>
-    <row r="163" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z162" s="15"/>
+      <c r="AA162" s="15"/>
+    </row>
+    <row r="163" spans="1:27" ht="15.75" customHeight="1">
       <c r="A163" s="15"/>
       <c r="B163" s="15"/>
       <c r="C163" s="15"/>
@@ -29579,8 +29933,10 @@
       <c r="W163" s="15"/>
       <c r="X163" s="15"/>
       <c r="Y163" s="15"/>
-    </row>
-    <row r="164" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z163" s="15"/>
+      <c r="AA163" s="15"/>
+    </row>
+    <row r="164" spans="1:27" ht="15.75" customHeight="1">
       <c r="A164" s="15"/>
       <c r="B164" s="15"/>
       <c r="C164" s="15"/>
@@ -29606,8 +29962,10 @@
       <c r="W164" s="15"/>
       <c r="X164" s="15"/>
       <c r="Y164" s="15"/>
-    </row>
-    <row r="165" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z164" s="15"/>
+      <c r="AA164" s="15"/>
+    </row>
+    <row r="165" spans="1:27" ht="15.75" customHeight="1">
       <c r="A165" s="15"/>
       <c r="B165" s="15"/>
       <c r="C165" s="15"/>
@@ -29633,8 +29991,10 @@
       <c r="W165" s="15"/>
       <c r="X165" s="15"/>
       <c r="Y165" s="15"/>
-    </row>
-    <row r="166" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z165" s="15"/>
+      <c r="AA165" s="15"/>
+    </row>
+    <row r="166" spans="1:27" ht="15.75" customHeight="1">
       <c r="A166" s="15"/>
       <c r="B166" s="15"/>
       <c r="C166" s="15"/>
@@ -29660,8 +30020,10 @@
       <c r="W166" s="15"/>
       <c r="X166" s="15"/>
       <c r="Y166" s="15"/>
-    </row>
-    <row r="167" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z166" s="15"/>
+      <c r="AA166" s="15"/>
+    </row>
+    <row r="167" spans="1:27" ht="15.75" customHeight="1">
       <c r="A167" s="15"/>
       <c r="B167" s="15"/>
       <c r="C167" s="15"/>
@@ -29687,8 +30049,10 @@
       <c r="W167" s="15"/>
       <c r="X167" s="15"/>
       <c r="Y167" s="15"/>
-    </row>
-    <row r="168" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z167" s="15"/>
+      <c r="AA167" s="15"/>
+    </row>
+    <row r="168" spans="1:27" ht="15.75" customHeight="1">
       <c r="A168" s="15"/>
       <c r="B168" s="15"/>
       <c r="C168" s="15"/>
@@ -29714,8 +30078,10 @@
       <c r="W168" s="15"/>
       <c r="X168" s="15"/>
       <c r="Y168" s="15"/>
-    </row>
-    <row r="169" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z168" s="15"/>
+      <c r="AA168" s="15"/>
+    </row>
+    <row r="169" spans="1:27" ht="15.75" customHeight="1">
       <c r="A169" s="15"/>
       <c r="B169" s="15"/>
       <c r="C169" s="15"/>
@@ -29741,8 +30107,10 @@
       <c r="W169" s="15"/>
       <c r="X169" s="15"/>
       <c r="Y169" s="15"/>
-    </row>
-    <row r="170" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z169" s="15"/>
+      <c r="AA169" s="15"/>
+    </row>
+    <row r="170" spans="1:27" ht="15.75" customHeight="1">
       <c r="A170" s="15"/>
       <c r="B170" s="15"/>
       <c r="C170" s="15"/>
@@ -29768,8 +30136,10 @@
       <c r="W170" s="15"/>
       <c r="X170" s="15"/>
       <c r="Y170" s="15"/>
-    </row>
-    <row r="171" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z170" s="15"/>
+      <c r="AA170" s="15"/>
+    </row>
+    <row r="171" spans="1:27" ht="15.75" customHeight="1">
       <c r="A171" s="15"/>
       <c r="B171" s="15"/>
       <c r="C171" s="15"/>
@@ -29795,8 +30165,10 @@
       <c r="W171" s="15"/>
       <c r="X171" s="15"/>
       <c r="Y171" s="15"/>
-    </row>
-    <row r="172" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z171" s="15"/>
+      <c r="AA171" s="15"/>
+    </row>
+    <row r="172" spans="1:27" ht="15.75" customHeight="1">
       <c r="A172" s="15"/>
       <c r="B172" s="15"/>
       <c r="C172" s="15"/>
@@ -29822,8 +30194,10 @@
       <c r="W172" s="15"/>
       <c r="X172" s="15"/>
       <c r="Y172" s="15"/>
-    </row>
-    <row r="173" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z172" s="15"/>
+      <c r="AA172" s="15"/>
+    </row>
+    <row r="173" spans="1:27" ht="15.75" customHeight="1">
       <c r="A173" s="15"/>
       <c r="B173" s="15"/>
       <c r="C173" s="15"/>
@@ -29849,8 +30223,10 @@
       <c r="W173" s="15"/>
       <c r="X173" s="15"/>
       <c r="Y173" s="15"/>
-    </row>
-    <row r="174" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z173" s="15"/>
+      <c r="AA173" s="15"/>
+    </row>
+    <row r="174" spans="1:27" ht="15.75" customHeight="1">
       <c r="A174" s="15"/>
       <c r="B174" s="15"/>
       <c r="C174" s="15"/>
@@ -29876,8 +30252,10 @@
       <c r="W174" s="15"/>
       <c r="X174" s="15"/>
       <c r="Y174" s="15"/>
-    </row>
-    <row r="175" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z174" s="15"/>
+      <c r="AA174" s="15"/>
+    </row>
+    <row r="175" spans="1:27" ht="15.75" customHeight="1">
       <c r="A175" s="15"/>
       <c r="B175" s="15"/>
       <c r="C175" s="15"/>
@@ -29903,8 +30281,10 @@
       <c r="W175" s="15"/>
       <c r="X175" s="15"/>
       <c r="Y175" s="15"/>
-    </row>
-    <row r="176" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z175" s="15"/>
+      <c r="AA175" s="15"/>
+    </row>
+    <row r="176" spans="1:27" ht="15.75" customHeight="1">
       <c r="A176" s="15"/>
       <c r="B176" s="15"/>
       <c r="C176" s="15"/>
@@ -29930,8 +30310,10 @@
       <c r="W176" s="15"/>
       <c r="X176" s="15"/>
       <c r="Y176" s="15"/>
-    </row>
-    <row r="177" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z176" s="15"/>
+      <c r="AA176" s="15"/>
+    </row>
+    <row r="177" spans="1:27" ht="15.75" customHeight="1">
       <c r="A177" s="15"/>
       <c r="B177" s="15"/>
       <c r="C177" s="15"/>
@@ -29957,8 +30339,10 @@
       <c r="W177" s="15"/>
       <c r="X177" s="15"/>
       <c r="Y177" s="15"/>
-    </row>
-    <row r="178" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z177" s="15"/>
+      <c r="AA177" s="15"/>
+    </row>
+    <row r="178" spans="1:27" ht="15.75" customHeight="1">
       <c r="A178" s="15"/>
       <c r="B178" s="15"/>
       <c r="C178" s="15"/>
@@ -29984,8 +30368,10 @@
       <c r="W178" s="15"/>
       <c r="X178" s="15"/>
       <c r="Y178" s="15"/>
-    </row>
-    <row r="179" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z178" s="15"/>
+      <c r="AA178" s="15"/>
+    </row>
+    <row r="179" spans="1:27" ht="15.75" customHeight="1">
       <c r="A179" s="15"/>
       <c r="B179" s="15"/>
       <c r="C179" s="15"/>
@@ -30011,8 +30397,10 @@
       <c r="W179" s="15"/>
       <c r="X179" s="15"/>
       <c r="Y179" s="15"/>
-    </row>
-    <row r="180" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z179" s="15"/>
+      <c r="AA179" s="15"/>
+    </row>
+    <row r="180" spans="1:27" ht="15.75" customHeight="1">
       <c r="A180" s="15"/>
       <c r="B180" s="15"/>
       <c r="C180" s="15"/>
@@ -30038,8 +30426,10 @@
       <c r="W180" s="15"/>
       <c r="X180" s="15"/>
       <c r="Y180" s="15"/>
-    </row>
-    <row r="181" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z180" s="15"/>
+      <c r="AA180" s="15"/>
+    </row>
+    <row r="181" spans="1:27" ht="15.75" customHeight="1">
       <c r="A181" s="15"/>
       <c r="B181" s="15"/>
       <c r="C181" s="15"/>
@@ -30065,8 +30455,10 @@
       <c r="W181" s="15"/>
       <c r="X181" s="15"/>
       <c r="Y181" s="15"/>
-    </row>
-    <row r="182" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z181" s="15"/>
+      <c r="AA181" s="15"/>
+    </row>
+    <row r="182" spans="1:27" ht="15.75" customHeight="1">
       <c r="A182" s="15"/>
       <c r="B182" s="15"/>
       <c r="C182" s="15"/>
@@ -30092,8 +30484,10 @@
       <c r="W182" s="15"/>
       <c r="X182" s="15"/>
       <c r="Y182" s="15"/>
-    </row>
-    <row r="183" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z182" s="15"/>
+      <c r="AA182" s="15"/>
+    </row>
+    <row r="183" spans="1:27" ht="15.75" customHeight="1">
       <c r="A183" s="15"/>
       <c r="B183" s="15"/>
       <c r="C183" s="15"/>
@@ -30119,8 +30513,10 @@
       <c r="W183" s="15"/>
       <c r="X183" s="15"/>
       <c r="Y183" s="15"/>
-    </row>
-    <row r="184" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z183" s="15"/>
+      <c r="AA183" s="15"/>
+    </row>
+    <row r="184" spans="1:27" ht="15.75" customHeight="1">
       <c r="A184" s="15"/>
       <c r="B184" s="15"/>
       <c r="C184" s="15"/>
@@ -30146,8 +30542,10 @@
       <c r="W184" s="15"/>
       <c r="X184" s="15"/>
       <c r="Y184" s="15"/>
-    </row>
-    <row r="185" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z184" s="15"/>
+      <c r="AA184" s="15"/>
+    </row>
+    <row r="185" spans="1:27" ht="15.75" customHeight="1">
       <c r="A185" s="15"/>
       <c r="B185" s="15"/>
       <c r="C185" s="15"/>
@@ -30173,8 +30571,10 @@
       <c r="W185" s="15"/>
       <c r="X185" s="15"/>
       <c r="Y185" s="15"/>
-    </row>
-    <row r="186" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z185" s="15"/>
+      <c r="AA185" s="15"/>
+    </row>
+    <row r="186" spans="1:27" ht="15.75" customHeight="1">
       <c r="A186" s="15"/>
       <c r="B186" s="15"/>
       <c r="C186" s="15"/>
@@ -30200,8 +30600,10 @@
       <c r="W186" s="15"/>
       <c r="X186" s="15"/>
       <c r="Y186" s="15"/>
-    </row>
-    <row r="187" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z186" s="15"/>
+      <c r="AA186" s="15"/>
+    </row>
+    <row r="187" spans="1:27" ht="15.75" customHeight="1">
       <c r="A187" s="15"/>
       <c r="B187" s="15"/>
       <c r="C187" s="15"/>
@@ -30227,8 +30629,10 @@
       <c r="W187" s="15"/>
       <c r="X187" s="15"/>
       <c r="Y187" s="15"/>
-    </row>
-    <row r="188" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z187" s="15"/>
+      <c r="AA187" s="15"/>
+    </row>
+    <row r="188" spans="1:27" ht="15.75" customHeight="1">
       <c r="A188" s="15"/>
       <c r="B188" s="15"/>
       <c r="C188" s="15"/>
@@ -30254,8 +30658,10 @@
       <c r="W188" s="15"/>
       <c r="X188" s="15"/>
       <c r="Y188" s="15"/>
-    </row>
-    <row r="189" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z188" s="15"/>
+      <c r="AA188" s="15"/>
+    </row>
+    <row r="189" spans="1:27" ht="15.75" customHeight="1">
       <c r="A189" s="15"/>
       <c r="B189" s="15"/>
       <c r="C189" s="15"/>
@@ -30281,8 +30687,10 @@
       <c r="W189" s="15"/>
       <c r="X189" s="15"/>
       <c r="Y189" s="15"/>
-    </row>
-    <row r="190" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z189" s="15"/>
+      <c r="AA189" s="15"/>
+    </row>
+    <row r="190" spans="1:27" ht="15.75" customHeight="1">
       <c r="A190" s="15"/>
       <c r="B190" s="15"/>
       <c r="C190" s="15"/>
@@ -30308,8 +30716,10 @@
       <c r="W190" s="15"/>
       <c r="X190" s="15"/>
       <c r="Y190" s="15"/>
-    </row>
-    <row r="191" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z190" s="15"/>
+      <c r="AA190" s="15"/>
+    </row>
+    <row r="191" spans="1:27" ht="15.75" customHeight="1">
       <c r="A191" s="15"/>
       <c r="B191" s="15"/>
       <c r="C191" s="15"/>
@@ -30335,8 +30745,10 @@
       <c r="W191" s="15"/>
       <c r="X191" s="15"/>
       <c r="Y191" s="15"/>
-    </row>
-    <row r="192" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z191" s="15"/>
+      <c r="AA191" s="15"/>
+    </row>
+    <row r="192" spans="1:27" ht="15.75" customHeight="1">
       <c r="A192" s="15"/>
       <c r="B192" s="15"/>
       <c r="C192" s="15"/>
@@ -30362,8 +30774,10 @@
       <c r="W192" s="15"/>
       <c r="X192" s="15"/>
       <c r="Y192" s="15"/>
-    </row>
-    <row r="193" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z192" s="15"/>
+      <c r="AA192" s="15"/>
+    </row>
+    <row r="193" spans="1:27" ht="15.75" customHeight="1">
       <c r="A193" s="15"/>
       <c r="B193" s="15"/>
       <c r="C193" s="15"/>
@@ -30389,8 +30803,10 @@
       <c r="W193" s="15"/>
       <c r="X193" s="15"/>
       <c r="Y193" s="15"/>
-    </row>
-    <row r="194" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z193" s="15"/>
+      <c r="AA193" s="15"/>
+    </row>
+    <row r="194" spans="1:27" ht="15.75" customHeight="1">
       <c r="A194" s="15"/>
       <c r="B194" s="15"/>
       <c r="C194" s="15"/>
@@ -30416,8 +30832,10 @@
       <c r="W194" s="15"/>
       <c r="X194" s="15"/>
       <c r="Y194" s="15"/>
-    </row>
-    <row r="195" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z194" s="15"/>
+      <c r="AA194" s="15"/>
+    </row>
+    <row r="195" spans="1:27" ht="15.75" customHeight="1">
       <c r="A195" s="15"/>
       <c r="B195" s="15"/>
       <c r="C195" s="15"/>
@@ -30443,8 +30861,10 @@
       <c r="W195" s="15"/>
       <c r="X195" s="15"/>
       <c r="Y195" s="15"/>
-    </row>
-    <row r="196" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z195" s="15"/>
+      <c r="AA195" s="15"/>
+    </row>
+    <row r="196" spans="1:27" ht="15.75" customHeight="1">
       <c r="A196" s="15"/>
       <c r="B196" s="15"/>
       <c r="C196" s="15"/>
@@ -30470,8 +30890,10 @@
       <c r="W196" s="15"/>
       <c r="X196" s="15"/>
       <c r="Y196" s="15"/>
-    </row>
-    <row r="197" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z196" s="15"/>
+      <c r="AA196" s="15"/>
+    </row>
+    <row r="197" spans="1:27" ht="15.75" customHeight="1">
       <c r="A197" s="15"/>
       <c r="B197" s="15"/>
       <c r="C197" s="15"/>
@@ -30497,8 +30919,10 @@
       <c r="W197" s="15"/>
       <c r="X197" s="15"/>
       <c r="Y197" s="15"/>
-    </row>
-    <row r="198" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z197" s="15"/>
+      <c r="AA197" s="15"/>
+    </row>
+    <row r="198" spans="1:27" ht="15.75" customHeight="1">
       <c r="A198" s="15"/>
       <c r="B198" s="15"/>
       <c r="C198" s="15"/>
@@ -30524,8 +30948,10 @@
       <c r="W198" s="15"/>
       <c r="X198" s="15"/>
       <c r="Y198" s="15"/>
-    </row>
-    <row r="199" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z198" s="15"/>
+      <c r="AA198" s="15"/>
+    </row>
+    <row r="199" spans="1:27" ht="15.75" customHeight="1">
       <c r="A199" s="15"/>
       <c r="B199" s="15"/>
       <c r="C199" s="15"/>
@@ -30551,8 +30977,10 @@
       <c r="W199" s="15"/>
       <c r="X199" s="15"/>
       <c r="Y199" s="15"/>
-    </row>
-    <row r="200" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z199" s="15"/>
+      <c r="AA199" s="15"/>
+    </row>
+    <row r="200" spans="1:27" ht="15.75" customHeight="1">
       <c r="A200" s="15"/>
       <c r="B200" s="15"/>
       <c r="C200" s="15"/>
@@ -30578,8 +31006,10 @@
       <c r="W200" s="15"/>
       <c r="X200" s="15"/>
       <c r="Y200" s="15"/>
-    </row>
-    <row r="201" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z200" s="15"/>
+      <c r="AA200" s="15"/>
+    </row>
+    <row r="201" spans="1:27" ht="15.75" customHeight="1">
       <c r="A201" s="15"/>
       <c r="B201" s="15"/>
       <c r="C201" s="15"/>
@@ -30605,8 +31035,10 @@
       <c r="W201" s="15"/>
       <c r="X201" s="15"/>
       <c r="Y201" s="15"/>
-    </row>
-    <row r="202" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z201" s="15"/>
+      <c r="AA201" s="15"/>
+    </row>
+    <row r="202" spans="1:27" ht="15.75" customHeight="1">
       <c r="A202" s="15"/>
       <c r="B202" s="15"/>
       <c r="C202" s="15"/>
@@ -30632,8 +31064,10 @@
       <c r="W202" s="15"/>
       <c r="X202" s="15"/>
       <c r="Y202" s="15"/>
-    </row>
-    <row r="203" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z202" s="15"/>
+      <c r="AA202" s="15"/>
+    </row>
+    <row r="203" spans="1:27" ht="15.75" customHeight="1">
       <c r="A203" s="15"/>
       <c r="B203" s="15"/>
       <c r="C203" s="15"/>
@@ -30659,8 +31093,10 @@
       <c r="W203" s="15"/>
       <c r="X203" s="15"/>
       <c r="Y203" s="15"/>
-    </row>
-    <row r="204" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z203" s="15"/>
+      <c r="AA203" s="15"/>
+    </row>
+    <row r="204" spans="1:27" ht="15.75" customHeight="1">
       <c r="A204" s="15"/>
       <c r="B204" s="15"/>
       <c r="C204" s="15"/>
@@ -30686,8 +31122,10 @@
       <c r="W204" s="15"/>
       <c r="X204" s="15"/>
       <c r="Y204" s="15"/>
-    </row>
-    <row r="205" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z204" s="15"/>
+      <c r="AA204" s="15"/>
+    </row>
+    <row r="205" spans="1:27" ht="15.75" customHeight="1">
       <c r="A205" s="15"/>
       <c r="B205" s="15"/>
       <c r="C205" s="15"/>
@@ -30713,8 +31151,10 @@
       <c r="W205" s="15"/>
       <c r="X205" s="15"/>
       <c r="Y205" s="15"/>
-    </row>
-    <row r="206" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z205" s="15"/>
+      <c r="AA205" s="15"/>
+    </row>
+    <row r="206" spans="1:27" ht="15.75" customHeight="1">
       <c r="A206" s="15"/>
       <c r="B206" s="15"/>
       <c r="C206" s="15"/>
@@ -30740,8 +31180,10 @@
       <c r="W206" s="15"/>
       <c r="X206" s="15"/>
       <c r="Y206" s="15"/>
-    </row>
-    <row r="207" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z206" s="15"/>
+      <c r="AA206" s="15"/>
+    </row>
+    <row r="207" spans="1:27" ht="15.75" customHeight="1">
       <c r="A207" s="15"/>
       <c r="B207" s="15"/>
       <c r="C207" s="15"/>
@@ -30767,8 +31209,10 @@
       <c r="W207" s="15"/>
       <c r="X207" s="15"/>
       <c r="Y207" s="15"/>
-    </row>
-    <row r="208" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z207" s="15"/>
+      <c r="AA207" s="15"/>
+    </row>
+    <row r="208" spans="1:27" ht="15.75" customHeight="1">
       <c r="A208" s="15"/>
       <c r="B208" s="15"/>
       <c r="C208" s="15"/>
@@ -30794,8 +31238,10 @@
       <c r="W208" s="15"/>
       <c r="X208" s="15"/>
       <c r="Y208" s="15"/>
-    </row>
-    <row r="209" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z208" s="15"/>
+      <c r="AA208" s="15"/>
+    </row>
+    <row r="209" spans="1:27" ht="15.75" customHeight="1">
       <c r="A209" s="15"/>
       <c r="B209" s="15"/>
       <c r="C209" s="15"/>
@@ -30821,8 +31267,10 @@
       <c r="W209" s="15"/>
       <c r="X209" s="15"/>
       <c r="Y209" s="15"/>
-    </row>
-    <row r="210" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z209" s="15"/>
+      <c r="AA209" s="15"/>
+    </row>
+    <row r="210" spans="1:27" ht="15.75" customHeight="1">
       <c r="A210" s="15"/>
       <c r="B210" s="15"/>
       <c r="C210" s="15"/>
@@ -30848,8 +31296,10 @@
       <c r="W210" s="15"/>
       <c r="X210" s="15"/>
       <c r="Y210" s="15"/>
-    </row>
-    <row r="211" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z210" s="15"/>
+      <c r="AA210" s="15"/>
+    </row>
+    <row r="211" spans="1:27" ht="15.75" customHeight="1">
       <c r="A211" s="15"/>
       <c r="B211" s="15"/>
       <c r="C211" s="15"/>
@@ -30875,8 +31325,10 @@
       <c r="W211" s="15"/>
       <c r="X211" s="15"/>
       <c r="Y211" s="15"/>
-    </row>
-    <row r="212" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z211" s="15"/>
+      <c r="AA211" s="15"/>
+    </row>
+    <row r="212" spans="1:27" ht="15.75" customHeight="1">
       <c r="A212" s="15"/>
       <c r="B212" s="15"/>
       <c r="C212" s="15"/>
@@ -30902,8 +31354,10 @@
       <c r="W212" s="15"/>
       <c r="X212" s="15"/>
       <c r="Y212" s="15"/>
-    </row>
-    <row r="213" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z212" s="15"/>
+      <c r="AA212" s="15"/>
+    </row>
+    <row r="213" spans="1:27" ht="15.75" customHeight="1">
       <c r="A213" s="15"/>
       <c r="B213" s="15"/>
       <c r="C213" s="15"/>
@@ -30929,8 +31383,10 @@
       <c r="W213" s="15"/>
       <c r="X213" s="15"/>
       <c r="Y213" s="15"/>
-    </row>
-    <row r="214" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z213" s="15"/>
+      <c r="AA213" s="15"/>
+    </row>
+    <row r="214" spans="1:27" ht="15.75" customHeight="1">
       <c r="A214" s="15"/>
       <c r="B214" s="15"/>
       <c r="C214" s="15"/>
@@ -30956,8 +31412,10 @@
       <c r="W214" s="15"/>
       <c r="X214" s="15"/>
       <c r="Y214" s="15"/>
-    </row>
-    <row r="215" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z214" s="15"/>
+      <c r="AA214" s="15"/>
+    </row>
+    <row r="215" spans="1:27" ht="15.75" customHeight="1">
       <c r="A215" s="15"/>
       <c r="B215" s="15"/>
       <c r="C215" s="15"/>
@@ -30983,8 +31441,10 @@
       <c r="W215" s="15"/>
       <c r="X215" s="15"/>
       <c r="Y215" s="15"/>
-    </row>
-    <row r="216" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z215" s="15"/>
+      <c r="AA215" s="15"/>
+    </row>
+    <row r="216" spans="1:27" ht="15.75" customHeight="1">
       <c r="A216" s="15"/>
       <c r="B216" s="15"/>
       <c r="C216" s="15"/>
@@ -31010,8 +31470,10 @@
       <c r="W216" s="15"/>
       <c r="X216" s="15"/>
       <c r="Y216" s="15"/>
-    </row>
-    <row r="217" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z216" s="15"/>
+      <c r="AA216" s="15"/>
+    </row>
+    <row r="217" spans="1:27" ht="15.75" customHeight="1">
       <c r="A217" s="15"/>
       <c r="B217" s="15"/>
       <c r="C217" s="15"/>
@@ -31037,8 +31499,10 @@
       <c r="W217" s="15"/>
       <c r="X217" s="15"/>
       <c r="Y217" s="15"/>
-    </row>
-    <row r="218" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z217" s="15"/>
+      <c r="AA217" s="15"/>
+    </row>
+    <row r="218" spans="1:27" ht="15.75" customHeight="1">
       <c r="A218" s="15"/>
       <c r="B218" s="15"/>
       <c r="C218" s="15"/>
@@ -31064,8 +31528,10 @@
       <c r="W218" s="15"/>
       <c r="X218" s="15"/>
       <c r="Y218" s="15"/>
-    </row>
-    <row r="219" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z218" s="15"/>
+      <c r="AA218" s="15"/>
+    </row>
+    <row r="219" spans="1:27" ht="15.75" customHeight="1">
       <c r="A219" s="15"/>
       <c r="B219" s="15"/>
       <c r="C219" s="15"/>
@@ -31091,8 +31557,10 @@
       <c r="W219" s="15"/>
       <c r="X219" s="15"/>
       <c r="Y219" s="15"/>
-    </row>
-    <row r="220" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z219" s="15"/>
+      <c r="AA219" s="15"/>
+    </row>
+    <row r="220" spans="1:27" ht="15.75" customHeight="1">
       <c r="A220" s="15"/>
       <c r="B220" s="15"/>
       <c r="C220" s="15"/>
@@ -31118,11 +31586,13 @@
       <c r="W220" s="15"/>
       <c r="X220" s="15"/>
       <c r="Y220" s="15"/>
-    </row>
-    <row r="221" spans="1:25" ht="15.75" customHeight="1"/>
-    <row r="222" spans="1:25" ht="15.75" customHeight="1"/>
-    <row r="223" spans="1:25" ht="15.75" customHeight="1"/>
-    <row r="224" spans="1:25" ht="15.75" customHeight="1"/>
+      <c r="Z220" s="15"/>
+      <c r="AA220" s="15"/>
+    </row>
+    <row r="221" spans="1:27" ht="15.75" customHeight="1"/>
+    <row r="222" spans="1:27" ht="15.75" customHeight="1"/>
+    <row r="223" spans="1:27" ht="15.75" customHeight="1"/>
+    <row r="224" spans="1:27" ht="15.75" customHeight="1"/>
     <row r="225" ht="15.75" customHeight="1"/>
     <row r="226" ht="15.75" customHeight="1"/>
     <row r="227" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Completed L0 2.1 identify the purpose and intended outcomes for the session
</commit_message>
<xml_diff>
--- a/ACS-CF Mentee Mapping Learning Log TEMPLATE - Esuabom Dijemeni.xlsx
+++ b/ACS-CF Mentee Mapping Learning Log TEMPLATE - Esuabom Dijemeni.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esuabomdijemeni/Desktop/github/acs-cf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9643DE-A2A7-3C41-BBFF-53AD3466D254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A728DA-D375-864F-A6D3-103785391C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10520" yWindow="500" windowWidth="30200" windowHeight="26600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Note" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="226">
   <si>
     <t>A note about Bloom's Taxonomy</t>
   </si>
@@ -693,36 +693,6 @@
     <t>1.4</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">... </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="20"/>
-        <color rgb="FF02B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>practice</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> the mindset of an effective facilitator.</t>
-    </r>
-  </si>
-  <si>
     <t>Understanding Group's Context and Needs</t>
   </si>
   <si>
@@ -730,36 +700,6 @@
   </si>
   <si>
     <t>2.1</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">… </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="20"/>
-        <color rgb="FF833CA3"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>identify</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> the purpose and intended outcomes for the session.</t>
-    </r>
   </si>
   <si>
     <t>2.2</t>
@@ -1837,6 +1777,66 @@
   <si>
     <t>What is facilitation? Who is a facilitator?</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">... </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="20"/>
+        <color rgb="FF02B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>practice</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> the mindset of an effective facilitator.</t>
+    </r>
+  </si>
+  <si>
+    <t>L0 1.4</t>
+  </si>
+  <si>
+    <t>Wrote a case study on effective facilitation</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">… </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="20"/>
+        <color rgb="FF833CA3"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>identify</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> the purpose and intended outcomes for the session.</t>
+    </r>
+  </si>
+  <si>
+    <t>LO 2.1</t>
+  </si>
+  <si>
+    <t>The facilitation canvas</t>
+  </si>
 </sst>
 </file>
 
@@ -2357,7 +2357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2534,6 +2534,8 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -2581,7 +2583,8 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -16909,8 +16912,8 @@
   </sheetPr>
   <dimension ref="A1:AB1005"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -16988,18 +16991,18 @@
     </row>
     <row r="3" spans="1:28" ht="15.75" customHeight="1">
       <c r="A3" s="25"/>
-      <c r="B3" s="86" t="s">
+      <c r="B3" s="88" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="88"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="90"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -17120,13 +17123,13 @@
     </row>
     <row r="6" spans="1:28" ht="78">
       <c r="A6" s="25"/>
-      <c r="B6" s="83">
+      <c r="B6" s="85">
         <v>1</v>
       </c>
-      <c r="C6" s="84" t="s">
+      <c r="C6" s="86" t="s">
         <v>123</v>
       </c>
-      <c r="D6" s="79" t="s">
+      <c r="D6" s="81" t="s">
         <v>124</v>
       </c>
       <c r="E6" s="50" t="s">
@@ -17160,9 +17163,9 @@
     </row>
     <row r="7" spans="1:28" ht="49.5" customHeight="1">
       <c r="A7" s="25"/>
-      <c r="B7" s="71"/>
-      <c r="C7" s="71"/>
-      <c r="D7" s="72"/>
+      <c r="B7" s="73"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="74"/>
       <c r="E7" s="50" t="s">
         <v>127</v>
       </c>
@@ -17191,9 +17194,9 @@
     </row>
     <row r="8" spans="1:28" ht="49.5" customHeight="1">
       <c r="A8" s="25"/>
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="79" t="s">
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="81" t="s">
         <v>128</v>
       </c>
       <c r="E8" s="50" t="s">
@@ -17227,14 +17230,14 @@
     </row>
     <row r="9" spans="1:28" ht="49.5" customHeight="1">
       <c r="A9" s="25"/>
-      <c r="B9" s="72"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72"/>
+      <c r="B9" s="74"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="74"/>
       <c r="E9" s="50" t="s">
         <v>131</v>
       </c>
       <c r="F9" s="52" t="s">
-        <v>132</v>
+        <v>220</v>
       </c>
       <c r="G9" s="33"/>
       <c r="H9" s="33"/>
@@ -17261,20 +17264,20 @@
     </row>
     <row r="10" spans="1:28" ht="49.5" customHeight="1">
       <c r="A10" s="25"/>
-      <c r="B10" s="85">
+      <c r="B10" s="87">
         <v>2</v>
       </c>
-      <c r="C10" s="75" t="s">
+      <c r="C10" s="77" t="s">
+        <v>132</v>
+      </c>
+      <c r="D10" s="81" t="s">
         <v>133</v>
       </c>
-      <c r="D10" s="79" t="s">
+      <c r="E10" s="50" t="s">
         <v>134</v>
       </c>
-      <c r="E10" s="50" t="s">
-        <v>135</v>
-      </c>
       <c r="F10" s="51" t="s">
-        <v>136</v>
+        <v>223</v>
       </c>
       <c r="G10" s="33"/>
       <c r="H10" s="33"/>
@@ -17301,14 +17304,14 @@
     </row>
     <row r="11" spans="1:28" ht="78">
       <c r="A11" s="25"/>
-      <c r="B11" s="71"/>
-      <c r="C11" s="71"/>
-      <c r="D11" s="71"/>
+      <c r="B11" s="73"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
       <c r="E11" s="50" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F11" s="51" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G11" s="53"/>
       <c r="H11" s="33"/>
@@ -17335,14 +17338,14 @@
     </row>
     <row r="12" spans="1:28" ht="49.5" customHeight="1">
       <c r="A12" s="25"/>
-      <c r="B12" s="71"/>
-      <c r="C12" s="71"/>
-      <c r="D12" s="71"/>
+      <c r="B12" s="73"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="73"/>
       <c r="E12" s="50" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F12" s="54" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G12" s="29"/>
       <c r="H12" s="33"/>
@@ -17369,14 +17372,14 @@
     </row>
     <row r="13" spans="1:28" ht="49.5" customHeight="1">
       <c r="A13" s="25"/>
-      <c r="B13" s="71"/>
-      <c r="C13" s="71"/>
-      <c r="D13" s="71"/>
+      <c r="B13" s="73"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="73"/>
       <c r="E13" s="50" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F13" s="52" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G13" s="29"/>
       <c r="H13" s="33"/>
@@ -17403,14 +17406,14 @@
     </row>
     <row r="14" spans="1:28" ht="49.5" customHeight="1">
       <c r="A14" s="25"/>
-      <c r="B14" s="71"/>
-      <c r="C14" s="71"/>
-      <c r="D14" s="71"/>
+      <c r="B14" s="73"/>
+      <c r="C14" s="73"/>
+      <c r="D14" s="73"/>
       <c r="E14" s="50" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F14" s="52" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G14" s="29"/>
       <c r="H14" s="33"/>
@@ -17437,14 +17440,14 @@
     </row>
     <row r="15" spans="1:28" ht="104">
       <c r="A15" s="25"/>
-      <c r="B15" s="71"/>
-      <c r="C15" s="71"/>
-      <c r="D15" s="72"/>
+      <c r="B15" s="73"/>
+      <c r="C15" s="73"/>
+      <c r="D15" s="74"/>
       <c r="E15" s="50" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F15" s="52" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G15" s="33"/>
       <c r="H15" s="33"/>
@@ -17471,16 +17474,16 @@
     </row>
     <row r="16" spans="1:28" ht="49.5" customHeight="1">
       <c r="A16" s="25"/>
-      <c r="B16" s="71"/>
-      <c r="C16" s="71"/>
-      <c r="D16" s="76" t="s">
-        <v>147</v>
+      <c r="B16" s="73"/>
+      <c r="C16" s="73"/>
+      <c r="D16" s="78" t="s">
+        <v>145</v>
       </c>
       <c r="E16" s="50" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F16" s="52" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G16" s="33"/>
       <c r="H16" s="33"/>
@@ -17507,14 +17510,14 @@
     </row>
     <row r="17" spans="1:28" ht="49.5" customHeight="1">
       <c r="A17" s="25"/>
-      <c r="B17" s="71"/>
-      <c r="C17" s="71"/>
-      <c r="D17" s="71"/>
+      <c r="B17" s="73"/>
+      <c r="C17" s="73"/>
+      <c r="D17" s="73"/>
       <c r="E17" s="50" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F17" s="51" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G17" s="33"/>
       <c r="H17" s="33"/>
@@ -17541,14 +17544,14 @@
     </row>
     <row r="18" spans="1:28" ht="49.5" customHeight="1">
       <c r="A18" s="25"/>
-      <c r="B18" s="71"/>
-      <c r="C18" s="71"/>
-      <c r="D18" s="71"/>
+      <c r="B18" s="73"/>
+      <c r="C18" s="73"/>
+      <c r="D18" s="73"/>
       <c r="E18" s="50" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F18" s="52" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G18" s="33"/>
       <c r="H18" s="33"/>
@@ -17575,14 +17578,14 @@
     </row>
     <row r="19" spans="1:28" ht="49.5" customHeight="1">
       <c r="A19" s="25"/>
-      <c r="B19" s="71"/>
-      <c r="C19" s="71"/>
-      <c r="D19" s="71"/>
+      <c r="B19" s="73"/>
+      <c r="C19" s="73"/>
+      <c r="D19" s="73"/>
       <c r="E19" s="50" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F19" s="51" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G19" s="33"/>
       <c r="H19" s="33"/>
@@ -17609,14 +17612,14 @@
     </row>
     <row r="20" spans="1:28" ht="49.5" customHeight="1">
       <c r="A20" s="25"/>
-      <c r="B20" s="71"/>
-      <c r="C20" s="71"/>
-      <c r="D20" s="71"/>
+      <c r="B20" s="73"/>
+      <c r="C20" s="73"/>
+      <c r="D20" s="73"/>
       <c r="E20" s="50" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F20" s="52" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G20" s="33"/>
       <c r="H20" s="33"/>
@@ -17643,14 +17646,14 @@
     </row>
     <row r="21" spans="1:28" ht="49.5" customHeight="1">
       <c r="A21" s="25"/>
-      <c r="B21" s="71"/>
-      <c r="C21" s="71"/>
-      <c r="D21" s="71"/>
+      <c r="B21" s="73"/>
+      <c r="C21" s="73"/>
+      <c r="D21" s="73"/>
       <c r="E21" s="50" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F21" s="52" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G21" s="33"/>
       <c r="H21" s="33"/>
@@ -17677,14 +17680,14 @@
     </row>
     <row r="22" spans="1:28" ht="49.5" customHeight="1">
       <c r="A22" s="25"/>
-      <c r="B22" s="72"/>
-      <c r="C22" s="72"/>
-      <c r="D22" s="72"/>
+      <c r="B22" s="74"/>
+      <c r="C22" s="74"/>
+      <c r="D22" s="74"/>
       <c r="E22" s="50" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F22" s="51" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G22" s="33"/>
       <c r="H22" s="33"/>
@@ -17711,20 +17714,20 @@
     </row>
     <row r="23" spans="1:28" ht="49.5" customHeight="1">
       <c r="A23" s="25"/>
-      <c r="B23" s="83">
+      <c r="B23" s="85">
         <v>3</v>
       </c>
-      <c r="C23" s="75" t="s">
+      <c r="C23" s="77" t="s">
+        <v>160</v>
+      </c>
+      <c r="D23" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="E23" s="50" t="s">
         <v>162</v>
       </c>
-      <c r="D23" s="76" t="s">
+      <c r="F23" s="51" t="s">
         <v>163</v>
-      </c>
-      <c r="E23" s="50" t="s">
-        <v>164</v>
-      </c>
-      <c r="F23" s="51" t="s">
-        <v>165</v>
       </c>
       <c r="G23" s="53"/>
       <c r="H23" s="33"/>
@@ -17751,14 +17754,14 @@
     </row>
     <row r="24" spans="1:28" ht="49.5" customHeight="1">
       <c r="A24" s="25"/>
-      <c r="B24" s="71"/>
-      <c r="C24" s="71"/>
-      <c r="D24" s="71"/>
+      <c r="B24" s="73"/>
+      <c r="C24" s="73"/>
+      <c r="D24" s="73"/>
       <c r="E24" s="55" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F24" s="56" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G24" s="53"/>
       <c r="H24" s="33"/>
@@ -17785,14 +17788,14 @@
     </row>
     <row r="25" spans="1:28" ht="49.5" customHeight="1">
       <c r="A25" s="25"/>
-      <c r="B25" s="71"/>
-      <c r="C25" s="71"/>
-      <c r="D25" s="72"/>
+      <c r="B25" s="73"/>
+      <c r="C25" s="73"/>
+      <c r="D25" s="74"/>
       <c r="E25" s="55" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F25" s="51" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G25" s="33"/>
       <c r="H25" s="33"/>
@@ -17819,16 +17822,16 @@
     </row>
     <row r="26" spans="1:28" ht="49.5" customHeight="1">
       <c r="A26" s="25"/>
-      <c r="B26" s="71"/>
-      <c r="C26" s="71"/>
-      <c r="D26" s="79" t="s">
-        <v>170</v>
+      <c r="B26" s="73"/>
+      <c r="C26" s="73"/>
+      <c r="D26" s="81" t="s">
+        <v>168</v>
       </c>
       <c r="E26" s="50" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F26" s="51" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G26" s="33"/>
       <c r="H26" s="33"/>
@@ -17855,14 +17858,14 @@
     </row>
     <row r="27" spans="1:28" ht="104">
       <c r="A27" s="25"/>
-      <c r="B27" s="71"/>
-      <c r="C27" s="71"/>
-      <c r="D27" s="71"/>
+      <c r="B27" s="73"/>
+      <c r="C27" s="73"/>
+      <c r="D27" s="73"/>
       <c r="E27" s="50" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F27" s="52" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G27" s="33"/>
       <c r="H27" s="33"/>
@@ -17889,14 +17892,14 @@
     </row>
     <row r="28" spans="1:28" ht="49.5" customHeight="1">
       <c r="A28" s="25"/>
-      <c r="B28" s="71"/>
-      <c r="C28" s="71"/>
-      <c r="D28" s="72"/>
+      <c r="B28" s="73"/>
+      <c r="C28" s="73"/>
+      <c r="D28" s="74"/>
       <c r="E28" s="50" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F28" s="51" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G28" s="33"/>
       <c r="H28" s="33"/>
@@ -17923,16 +17926,16 @@
     </row>
     <row r="29" spans="1:28" ht="49.5" customHeight="1">
       <c r="A29" s="25"/>
-      <c r="B29" s="71"/>
-      <c r="C29" s="71"/>
-      <c r="D29" s="76" t="s">
-        <v>177</v>
+      <c r="B29" s="73"/>
+      <c r="C29" s="73"/>
+      <c r="D29" s="78" t="s">
+        <v>175</v>
       </c>
       <c r="E29" s="50" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F29" s="51" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G29" s="33"/>
       <c r="H29" s="33"/>
@@ -17959,14 +17962,14 @@
     </row>
     <row r="30" spans="1:28" ht="49.5" customHeight="1">
       <c r="A30" s="25"/>
-      <c r="B30" s="72"/>
-      <c r="C30" s="72"/>
-      <c r="D30" s="72"/>
+      <c r="B30" s="74"/>
+      <c r="C30" s="74"/>
+      <c r="D30" s="74"/>
       <c r="E30" s="50" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F30" s="51" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G30" s="33"/>
       <c r="H30" s="33"/>
@@ -17993,20 +17996,20 @@
     </row>
     <row r="31" spans="1:28" ht="49.5" customHeight="1">
       <c r="A31" s="25"/>
-      <c r="B31" s="83">
+      <c r="B31" s="85">
         <v>4</v>
       </c>
-      <c r="C31" s="84" t="s">
-        <v>182</v>
+      <c r="C31" s="86" t="s">
+        <v>180</v>
       </c>
-      <c r="D31" s="76" t="s">
-        <v>182</v>
+      <c r="D31" s="78" t="s">
+        <v>180</v>
       </c>
       <c r="E31" s="50" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F31" s="51" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G31" s="33"/>
       <c r="H31" s="33"/>
@@ -18033,14 +18036,14 @@
     </row>
     <row r="32" spans="1:28" ht="49.5" customHeight="1">
       <c r="A32" s="25"/>
-      <c r="B32" s="71"/>
-      <c r="C32" s="71"/>
-      <c r="D32" s="71"/>
+      <c r="B32" s="73"/>
+      <c r="C32" s="73"/>
+      <c r="D32" s="73"/>
       <c r="E32" s="50" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F32" s="51" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G32" s="33"/>
       <c r="H32" s="33"/>
@@ -18067,14 +18070,14 @@
     </row>
     <row r="33" spans="1:28" ht="49.5" customHeight="1">
       <c r="A33" s="25"/>
-      <c r="B33" s="72"/>
-      <c r="C33" s="72"/>
-      <c r="D33" s="72"/>
+      <c r="B33" s="74"/>
+      <c r="C33" s="74"/>
+      <c r="D33" s="74"/>
       <c r="E33" s="50" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F33" s="51" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G33" s="33"/>
       <c r="H33" s="33"/>
@@ -18101,20 +18104,20 @@
     </row>
     <row r="34" spans="1:28" ht="105">
       <c r="A34" s="25"/>
-      <c r="B34" s="85">
+      <c r="B34" s="87">
         <v>5</v>
       </c>
-      <c r="C34" s="75" t="s">
+      <c r="C34" s="77" t="s">
+        <v>187</v>
+      </c>
+      <c r="D34" s="57" t="s">
+        <v>188</v>
+      </c>
+      <c r="E34" s="50" t="s">
         <v>189</v>
       </c>
-      <c r="D34" s="57" t="s">
+      <c r="F34" s="51" t="s">
         <v>190</v>
-      </c>
-      <c r="E34" s="50" t="s">
-        <v>191</v>
-      </c>
-      <c r="F34" s="51" t="s">
-        <v>192</v>
       </c>
       <c r="G34" s="33"/>
       <c r="H34" s="33"/>
@@ -18141,16 +18144,16 @@
     </row>
     <row r="35" spans="1:28" ht="49.5" customHeight="1">
       <c r="A35" s="25"/>
-      <c r="B35" s="71"/>
-      <c r="C35" s="71"/>
+      <c r="B35" s="73"/>
+      <c r="C35" s="73"/>
       <c r="D35" s="57" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E35" s="50" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F35" s="51" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G35" s="33"/>
       <c r="H35" s="33"/>
@@ -18177,16 +18180,16 @@
     </row>
     <row r="36" spans="1:28" ht="49.5" customHeight="1">
       <c r="A36" s="25"/>
-      <c r="B36" s="71"/>
-      <c r="C36" s="71"/>
-      <c r="D36" s="76" t="s">
-        <v>196</v>
+      <c r="B36" s="73"/>
+      <c r="C36" s="73"/>
+      <c r="D36" s="78" t="s">
+        <v>194</v>
       </c>
       <c r="E36" s="50" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F36" s="52" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G36" s="33"/>
       <c r="H36" s="33"/>
@@ -18213,14 +18216,14 @@
     </row>
     <row r="37" spans="1:28" ht="78">
       <c r="A37" s="25"/>
-      <c r="B37" s="72"/>
-      <c r="C37" s="72"/>
-      <c r="D37" s="72"/>
+      <c r="B37" s="74"/>
+      <c r="C37" s="74"/>
+      <c r="D37" s="74"/>
       <c r="E37" s="50" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F37" s="52" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G37" s="33"/>
       <c r="H37" s="33"/>
@@ -18247,20 +18250,20 @@
     </row>
     <row r="38" spans="1:28" ht="49.5" customHeight="1">
       <c r="A38" s="25"/>
-      <c r="B38" s="85">
+      <c r="B38" s="87">
         <v>6</v>
       </c>
-      <c r="C38" s="75" t="s">
-        <v>201</v>
+      <c r="C38" s="77" t="s">
+        <v>199</v>
       </c>
-      <c r="D38" s="76" t="s">
-        <v>201</v>
+      <c r="D38" s="78" t="s">
+        <v>199</v>
       </c>
       <c r="E38" s="50" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F38" s="58" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G38" s="33"/>
       <c r="H38" s="33"/>
@@ -18287,14 +18290,14 @@
     </row>
     <row r="39" spans="1:28" ht="49.5" customHeight="1">
       <c r="A39" s="25"/>
-      <c r="B39" s="72"/>
-      <c r="C39" s="72"/>
-      <c r="D39" s="72"/>
+      <c r="B39" s="74"/>
+      <c r="C39" s="74"/>
+      <c r="D39" s="74"/>
       <c r="E39" s="59" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F39" s="58" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G39" s="53"/>
       <c r="H39" s="33"/>
@@ -18320,28 +18323,28 @@
       <c r="AB39" s="2"/>
     </row>
     <row r="40" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A40" s="77"/>
-      <c r="B40" s="77" t="s">
+      <c r="A40" s="79"/>
+      <c r="B40" s="79" t="s">
+        <v>204</v>
+      </c>
+      <c r="C40" s="80" t="s">
+        <v>205</v>
+      </c>
+      <c r="D40" s="81" t="s">
         <v>206</v>
       </c>
-      <c r="C40" s="78" t="s">
+      <c r="E40" s="82" t="s">
         <v>207</v>
       </c>
-      <c r="D40" s="79" t="s">
+      <c r="F40" s="83" t="s">
         <v>208</v>
       </c>
-      <c r="E40" s="80" t="s">
-        <v>209</v>
-      </c>
-      <c r="F40" s="81" t="s">
-        <v>210</v>
-      </c>
-      <c r="G40" s="70"/>
-      <c r="H40" s="70"/>
-      <c r="I40" s="82"/>
-      <c r="J40" s="70"/>
-      <c r="K40" s="70"/>
-      <c r="L40" s="73"/>
+      <c r="G40" s="72"/>
+      <c r="H40" s="72"/>
+      <c r="I40" s="84"/>
+      <c r="J40" s="72"/>
+      <c r="K40" s="72"/>
+      <c r="L40" s="75"/>
       <c r="M40" s="15"/>
       <c r="N40" s="15"/>
       <c r="O40" s="15"/>
@@ -18360,18 +18363,18 @@
       <c r="AB40" s="2"/>
     </row>
     <row r="41" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A41" s="71"/>
-      <c r="B41" s="71"/>
-      <c r="C41" s="71"/>
-      <c r="D41" s="71"/>
-      <c r="E41" s="71"/>
-      <c r="F41" s="71"/>
-      <c r="G41" s="71"/>
-      <c r="H41" s="71"/>
-      <c r="I41" s="71"/>
-      <c r="J41" s="71"/>
-      <c r="K41" s="71"/>
-      <c r="L41" s="74"/>
+      <c r="A41" s="73"/>
+      <c r="B41" s="73"/>
+      <c r="C41" s="73"/>
+      <c r="D41" s="73"/>
+      <c r="E41" s="73"/>
+      <c r="F41" s="73"/>
+      <c r="G41" s="73"/>
+      <c r="H41" s="73"/>
+      <c r="I41" s="73"/>
+      <c r="J41" s="73"/>
+      <c r="K41" s="73"/>
+      <c r="L41" s="76"/>
       <c r="M41" s="15"/>
       <c r="N41" s="15"/>
       <c r="O41" s="15"/>
@@ -18390,18 +18393,18 @@
       <c r="AB41" s="2"/>
     </row>
     <row r="42" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A42" s="71"/>
-      <c r="B42" s="71"/>
-      <c r="C42" s="71"/>
-      <c r="D42" s="71"/>
-      <c r="E42" s="71"/>
-      <c r="F42" s="71"/>
-      <c r="G42" s="71"/>
-      <c r="H42" s="71"/>
-      <c r="I42" s="71"/>
-      <c r="J42" s="71"/>
-      <c r="K42" s="71"/>
-      <c r="L42" s="74"/>
+      <c r="A42" s="73"/>
+      <c r="B42" s="73"/>
+      <c r="C42" s="73"/>
+      <c r="D42" s="73"/>
+      <c r="E42" s="73"/>
+      <c r="F42" s="73"/>
+      <c r="G42" s="73"/>
+      <c r="H42" s="73"/>
+      <c r="I42" s="73"/>
+      <c r="J42" s="73"/>
+      <c r="K42" s="73"/>
+      <c r="L42" s="76"/>
       <c r="M42" s="15"/>
       <c r="N42" s="15"/>
       <c r="O42" s="15"/>
@@ -18420,18 +18423,18 @@
       <c r="AB42" s="2"/>
     </row>
     <row r="43" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A43" s="71"/>
-      <c r="B43" s="71"/>
-      <c r="C43" s="71"/>
-      <c r="D43" s="71"/>
-      <c r="E43" s="71"/>
-      <c r="F43" s="71"/>
-      <c r="G43" s="71"/>
-      <c r="H43" s="71"/>
-      <c r="I43" s="71"/>
-      <c r="J43" s="71"/>
-      <c r="K43" s="71"/>
-      <c r="L43" s="74"/>
+      <c r="A43" s="73"/>
+      <c r="B43" s="73"/>
+      <c r="C43" s="73"/>
+      <c r="D43" s="73"/>
+      <c r="E43" s="73"/>
+      <c r="F43" s="73"/>
+      <c r="G43" s="73"/>
+      <c r="H43" s="73"/>
+      <c r="I43" s="73"/>
+      <c r="J43" s="73"/>
+      <c r="K43" s="73"/>
+      <c r="L43" s="76"/>
       <c r="M43" s="15"/>
       <c r="N43" s="15"/>
       <c r="O43" s="15"/>
@@ -18450,18 +18453,18 @@
       <c r="AB43" s="2"/>
     </row>
     <row r="44" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A44" s="71"/>
-      <c r="B44" s="71"/>
-      <c r="C44" s="71"/>
-      <c r="D44" s="71"/>
-      <c r="E44" s="71"/>
-      <c r="F44" s="71"/>
-      <c r="G44" s="71"/>
-      <c r="H44" s="71"/>
-      <c r="I44" s="71"/>
-      <c r="J44" s="71"/>
-      <c r="K44" s="71"/>
-      <c r="L44" s="74"/>
+      <c r="A44" s="73"/>
+      <c r="B44" s="73"/>
+      <c r="C44" s="73"/>
+      <c r="D44" s="73"/>
+      <c r="E44" s="73"/>
+      <c r="F44" s="73"/>
+      <c r="G44" s="73"/>
+      <c r="H44" s="73"/>
+      <c r="I44" s="73"/>
+      <c r="J44" s="73"/>
+      <c r="K44" s="73"/>
+      <c r="L44" s="76"/>
       <c r="M44" s="15"/>
       <c r="N44" s="15"/>
       <c r="O44" s="15"/>
@@ -18480,18 +18483,18 @@
       <c r="AB44" s="2"/>
     </row>
     <row r="45" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A45" s="72"/>
-      <c r="B45" s="72"/>
-      <c r="C45" s="72"/>
-      <c r="D45" s="72"/>
-      <c r="E45" s="72"/>
-      <c r="F45" s="72"/>
-      <c r="G45" s="72"/>
-      <c r="H45" s="72"/>
-      <c r="I45" s="72"/>
-      <c r="J45" s="72"/>
-      <c r="K45" s="72"/>
-      <c r="L45" s="74"/>
+      <c r="A45" s="74"/>
+      <c r="B45" s="74"/>
+      <c r="C45" s="74"/>
+      <c r="D45" s="74"/>
+      <c r="E45" s="74"/>
+      <c r="F45" s="74"/>
+      <c r="G45" s="74"/>
+      <c r="H45" s="74"/>
+      <c r="I45" s="74"/>
+      <c r="J45" s="74"/>
+      <c r="K45" s="74"/>
+      <c r="L45" s="76"/>
       <c r="M45" s="15"/>
       <c r="N45" s="15"/>
       <c r="O45" s="15"/>
@@ -25176,13 +25179,13 @@
   </sheetPr>
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N35" sqref="N35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" style="92" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="37.1640625" customWidth="1"/>
     <col min="5" max="5" width="35.6640625" bestFit="1" customWidth="1"/>
@@ -25191,19 +25194,19 @@
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1">
       <c r="A1" s="62" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B1" s="62" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C1" s="62" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D1" s="62" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E1" s="62" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
@@ -25229,20 +25232,20 @@
       <c r="AA1" s="15"/>
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A2" s="63">
+      <c r="A2" s="71">
         <v>45468</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
-      <c r="C2" s="89">
+      <c r="C2" s="70">
         <v>0.625</v>
       </c>
-      <c r="D2" s="89">
+      <c r="D2" s="70">
         <v>0.72916666666666663</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
@@ -25268,11 +25271,21 @@
       <c r="AA2" s="15"/>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
+      <c r="A3" s="71">
+        <v>45329</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="C3" s="70">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D3" s="70">
+        <v>0.875</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>222</v>
+      </c>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
@@ -25297,11 +25310,21 @@
       <c r="AA3" s="15"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
+      <c r="A4" s="71">
+        <v>45542</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="C4" s="70">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D4" s="70">
+        <v>0.75</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>225</v>
+      </c>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
@@ -25326,7 +25349,7 @@
       <c r="AA4" s="15"/>
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A5" s="7"/>
+      <c r="A5" s="71"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -25355,7 +25378,7 @@
       <c r="AA5" s="15"/>
     </row>
     <row r="6" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A6" s="7"/>
+      <c r="A6" s="71"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -25384,7 +25407,7 @@
       <c r="AA6" s="15"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A7" s="7"/>
+      <c r="A7" s="71"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -25413,7 +25436,7 @@
       <c r="AA7" s="15"/>
     </row>
     <row r="8" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A8" s="7"/>
+      <c r="A8" s="71"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -25442,7 +25465,7 @@
       <c r="AA8" s="15"/>
     </row>
     <row r="9" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A9" s="7"/>
+      <c r="A9" s="71"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -25471,7 +25494,7 @@
       <c r="AA9" s="15"/>
     </row>
     <row r="10" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A10" s="7"/>
+      <c r="A10" s="71"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -25500,7 +25523,7 @@
       <c r="AA10" s="15"/>
     </row>
     <row r="11" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A11" s="7"/>
+      <c r="A11" s="71"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -25529,7 +25552,7 @@
       <c r="AA11" s="15"/>
     </row>
     <row r="12" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A12" s="7"/>
+      <c r="A12" s="71"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -25558,7 +25581,7 @@
       <c r="AA12" s="15"/>
     </row>
     <row r="13" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A13" s="7"/>
+      <c r="A13" s="71"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
@@ -25587,7 +25610,7 @@
       <c r="AA13" s="15"/>
     </row>
     <row r="14" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A14" s="7"/>
+      <c r="A14" s="71"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -25616,7 +25639,7 @@
       <c r="AA14" s="15"/>
     </row>
     <row r="15" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A15" s="7"/>
+      <c r="A15" s="71"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
@@ -25645,7 +25668,7 @@
       <c r="AA15" s="15"/>
     </row>
     <row r="16" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A16" s="7"/>
+      <c r="A16" s="71"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -25674,7 +25697,7 @@
       <c r="AA16" s="15"/>
     </row>
     <row r="17" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A17" s="7"/>
+      <c r="A17" s="71"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -25703,7 +25726,7 @@
       <c r="AA17" s="15"/>
     </row>
     <row r="18" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A18" s="7"/>
+      <c r="A18" s="71"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -25732,7 +25755,7 @@
       <c r="AA18" s="15"/>
     </row>
     <row r="19" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A19" s="7"/>
+      <c r="A19" s="71"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -25761,7 +25784,7 @@
       <c r="AA19" s="15"/>
     </row>
     <row r="20" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A20" s="7"/>
+      <c r="A20" s="71"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -25790,7 +25813,7 @@
       <c r="AA20" s="15"/>
     </row>
     <row r="21" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A21" s="7"/>
+      <c r="A21" s="71"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -25819,7 +25842,7 @@
       <c r="AA21" s="15"/>
     </row>
     <row r="22" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A22" s="7"/>
+      <c r="A22" s="71"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -25848,7 +25871,7 @@
       <c r="AA22" s="15"/>
     </row>
     <row r="23" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A23" s="7"/>
+      <c r="A23" s="71"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -25877,7 +25900,7 @@
       <c r="AA23" s="15"/>
     </row>
     <row r="24" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A24" s="7"/>
+      <c r="A24" s="71"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -25906,7 +25929,7 @@
       <c r="AA24" s="15"/>
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A25" s="7"/>
+      <c r="A25" s="71"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -25935,7 +25958,7 @@
       <c r="AA25" s="15"/>
     </row>
     <row r="26" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A26" s="7"/>
+      <c r="A26" s="71"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -25964,7 +25987,7 @@
       <c r="AA26" s="15"/>
     </row>
     <row r="27" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A27" s="7"/>
+      <c r="A27" s="71"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -25993,7 +26016,7 @@
       <c r="AA27" s="15"/>
     </row>
     <row r="28" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A28" s="7"/>
+      <c r="A28" s="71"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -26022,7 +26045,7 @@
       <c r="AA28" s="15"/>
     </row>
     <row r="29" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A29" s="7"/>
+      <c r="A29" s="71"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -26051,7 +26074,7 @@
       <c r="AA29" s="15"/>
     </row>
     <row r="30" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A30" s="7"/>
+      <c r="A30" s="71"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
@@ -26080,7 +26103,7 @@
       <c r="AA30" s="15"/>
     </row>
     <row r="31" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A31" s="7"/>
+      <c r="A31" s="71"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -26109,7 +26132,7 @@
       <c r="AA31" s="15"/>
     </row>
     <row r="32" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A32" s="7"/>
+      <c r="A32" s="71"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -26138,7 +26161,7 @@
       <c r="AA32" s="15"/>
     </row>
     <row r="33" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A33" s="15"/>
+      <c r="A33" s="91"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
       <c r="D33" s="15"/>
@@ -26167,7 +26190,7 @@
       <c r="AA33" s="15"/>
     </row>
     <row r="34" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A34" s="15"/>
+      <c r="A34" s="91"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
       <c r="D34" s="15"/>
@@ -26196,7 +26219,7 @@
       <c r="AA34" s="15"/>
     </row>
     <row r="35" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A35" s="15"/>
+      <c r="A35" s="91"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
       <c r="D35" s="15"/>
@@ -26225,7 +26248,7 @@
       <c r="AA35" s="15"/>
     </row>
     <row r="36" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A36" s="15"/>
+      <c r="A36" s="91"/>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
       <c r="D36" s="15"/>
@@ -26254,7 +26277,7 @@
       <c r="AA36" s="15"/>
     </row>
     <row r="37" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A37" s="15"/>
+      <c r="A37" s="91"/>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
       <c r="D37" s="15"/>
@@ -26283,7 +26306,7 @@
       <c r="AA37" s="15"/>
     </row>
     <row r="38" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A38" s="15"/>
+      <c r="A38" s="91"/>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
       <c r="D38" s="15"/>
@@ -26312,7 +26335,7 @@
       <c r="AA38" s="15"/>
     </row>
     <row r="39" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A39" s="15"/>
+      <c r="A39" s="91"/>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
       <c r="D39" s="15"/>
@@ -26341,7 +26364,7 @@
       <c r="AA39" s="15"/>
     </row>
     <row r="40" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A40" s="15"/>
+      <c r="A40" s="91"/>
       <c r="B40" s="15"/>
       <c r="C40" s="15"/>
       <c r="D40" s="15"/>
@@ -26370,7 +26393,7 @@
       <c r="AA40" s="15"/>
     </row>
     <row r="41" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A41" s="15"/>
+      <c r="A41" s="91"/>
       <c r="B41" s="15"/>
       <c r="C41" s="15"/>
       <c r="D41" s="15"/>
@@ -26399,7 +26422,7 @@
       <c r="AA41" s="15"/>
     </row>
     <row r="42" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A42" s="15"/>
+      <c r="A42" s="91"/>
       <c r="B42" s="15"/>
       <c r="C42" s="15"/>
       <c r="D42" s="15"/>
@@ -26428,7 +26451,7 @@
       <c r="AA42" s="15"/>
     </row>
     <row r="43" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A43" s="15"/>
+      <c r="A43" s="91"/>
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
       <c r="D43" s="15"/>
@@ -26457,7 +26480,7 @@
       <c r="AA43" s="15"/>
     </row>
     <row r="44" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A44" s="15"/>
+      <c r="A44" s="91"/>
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
       <c r="D44" s="15"/>
@@ -26486,7 +26509,7 @@
       <c r="AA44" s="15"/>
     </row>
     <row r="45" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A45" s="15"/>
+      <c r="A45" s="91"/>
       <c r="B45" s="15"/>
       <c r="C45" s="15"/>
       <c r="D45" s="15"/>
@@ -26515,7 +26538,7 @@
       <c r="AA45" s="15"/>
     </row>
     <row r="46" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A46" s="15"/>
+      <c r="A46" s="91"/>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
       <c r="D46" s="15"/>
@@ -26544,7 +26567,7 @@
       <c r="AA46" s="15"/>
     </row>
     <row r="47" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A47" s="15"/>
+      <c r="A47" s="91"/>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>
       <c r="D47" s="15"/>
@@ -26573,7 +26596,7 @@
       <c r="AA47" s="15"/>
     </row>
     <row r="48" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A48" s="15"/>
+      <c r="A48" s="91"/>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
       <c r="D48" s="15"/>
@@ -26602,7 +26625,7 @@
       <c r="AA48" s="15"/>
     </row>
     <row r="49" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A49" s="15"/>
+      <c r="A49" s="91"/>
       <c r="B49" s="15"/>
       <c r="C49" s="15"/>
       <c r="D49" s="15"/>
@@ -26631,7 +26654,7 @@
       <c r="AA49" s="15"/>
     </row>
     <row r="50" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A50" s="15"/>
+      <c r="A50" s="91"/>
       <c r="B50" s="15"/>
       <c r="C50" s="15"/>
       <c r="D50" s="15"/>
@@ -26660,7 +26683,7 @@
       <c r="AA50" s="15"/>
     </row>
     <row r="51" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A51" s="15"/>
+      <c r="A51" s="91"/>
       <c r="B51" s="15"/>
       <c r="C51" s="15"/>
       <c r="D51" s="15"/>
@@ -26689,7 +26712,7 @@
       <c r="AA51" s="15"/>
     </row>
     <row r="52" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A52" s="15"/>
+      <c r="A52" s="91"/>
       <c r="B52" s="15"/>
       <c r="C52" s="15"/>
       <c r="D52" s="15"/>
@@ -26718,7 +26741,7 @@
       <c r="AA52" s="15"/>
     </row>
     <row r="53" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A53" s="15"/>
+      <c r="A53" s="91"/>
       <c r="B53" s="15"/>
       <c r="C53" s="15"/>
       <c r="D53" s="15"/>
@@ -26747,7 +26770,7 @@
       <c r="AA53" s="15"/>
     </row>
     <row r="54" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A54" s="15"/>
+      <c r="A54" s="91"/>
       <c r="B54" s="15"/>
       <c r="C54" s="15"/>
       <c r="D54" s="15"/>
@@ -26776,7 +26799,7 @@
       <c r="AA54" s="15"/>
     </row>
     <row r="55" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A55" s="15"/>
+      <c r="A55" s="91"/>
       <c r="B55" s="15"/>
       <c r="C55" s="15"/>
       <c r="D55" s="15"/>
@@ -26805,7 +26828,7 @@
       <c r="AA55" s="15"/>
     </row>
     <row r="56" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A56" s="15"/>
+      <c r="A56" s="91"/>
       <c r="B56" s="15"/>
       <c r="C56" s="15"/>
       <c r="D56" s="15"/>
@@ -26834,7 +26857,7 @@
       <c r="AA56" s="15"/>
     </row>
     <row r="57" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A57" s="15"/>
+      <c r="A57" s="91"/>
       <c r="B57" s="15"/>
       <c r="C57" s="15"/>
       <c r="D57" s="15"/>
@@ -26863,7 +26886,7 @@
       <c r="AA57" s="15"/>
     </row>
     <row r="58" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A58" s="15"/>
+      <c r="A58" s="91"/>
       <c r="B58" s="15"/>
       <c r="C58" s="15"/>
       <c r="D58" s="15"/>
@@ -26892,7 +26915,7 @@
       <c r="AA58" s="15"/>
     </row>
     <row r="59" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A59" s="15"/>
+      <c r="A59" s="91"/>
       <c r="B59" s="15"/>
       <c r="C59" s="15"/>
       <c r="D59" s="15"/>
@@ -26921,7 +26944,7 @@
       <c r="AA59" s="15"/>
     </row>
     <row r="60" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A60" s="15"/>
+      <c r="A60" s="91"/>
       <c r="B60" s="15"/>
       <c r="C60" s="15"/>
       <c r="D60" s="15"/>
@@ -26950,7 +26973,7 @@
       <c r="AA60" s="15"/>
     </row>
     <row r="61" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A61" s="15"/>
+      <c r="A61" s="91"/>
       <c r="B61" s="15"/>
       <c r="C61" s="15"/>
       <c r="D61" s="15"/>
@@ -26979,7 +27002,7 @@
       <c r="AA61" s="15"/>
     </row>
     <row r="62" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A62" s="15"/>
+      <c r="A62" s="91"/>
       <c r="B62" s="15"/>
       <c r="C62" s="15"/>
       <c r="D62" s="15"/>
@@ -27008,7 +27031,7 @@
       <c r="AA62" s="15"/>
     </row>
     <row r="63" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A63" s="15"/>
+      <c r="A63" s="91"/>
       <c r="B63" s="15"/>
       <c r="C63" s="15"/>
       <c r="D63" s="15"/>
@@ -27037,7 +27060,7 @@
       <c r="AA63" s="15"/>
     </row>
     <row r="64" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A64" s="15"/>
+      <c r="A64" s="91"/>
       <c r="B64" s="15"/>
       <c r="C64" s="15"/>
       <c r="D64" s="15"/>
@@ -27066,7 +27089,7 @@
       <c r="AA64" s="15"/>
     </row>
     <row r="65" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A65" s="15"/>
+      <c r="A65" s="91"/>
       <c r="B65" s="15"/>
       <c r="C65" s="15"/>
       <c r="D65" s="15"/>
@@ -27095,7 +27118,7 @@
       <c r="AA65" s="15"/>
     </row>
     <row r="66" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A66" s="15"/>
+      <c r="A66" s="91"/>
       <c r="B66" s="15"/>
       <c r="C66" s="15"/>
       <c r="D66" s="15"/>
@@ -27124,7 +27147,7 @@
       <c r="AA66" s="15"/>
     </row>
     <row r="67" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A67" s="15"/>
+      <c r="A67" s="91"/>
       <c r="B67" s="15"/>
       <c r="C67" s="15"/>
       <c r="D67" s="15"/>
@@ -27153,7 +27176,7 @@
       <c r="AA67" s="15"/>
     </row>
     <row r="68" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A68" s="15"/>
+      <c r="A68" s="91"/>
       <c r="B68" s="15"/>
       <c r="C68" s="15"/>
       <c r="D68" s="15"/>
@@ -27182,7 +27205,7 @@
       <c r="AA68" s="15"/>
     </row>
     <row r="69" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A69" s="15"/>
+      <c r="A69" s="91"/>
       <c r="B69" s="15"/>
       <c r="C69" s="15"/>
       <c r="D69" s="15"/>
@@ -27211,7 +27234,7 @@
       <c r="AA69" s="15"/>
     </row>
     <row r="70" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A70" s="15"/>
+      <c r="A70" s="91"/>
       <c r="B70" s="15"/>
       <c r="C70" s="15"/>
       <c r="D70" s="15"/>
@@ -27240,7 +27263,7 @@
       <c r="AA70" s="15"/>
     </row>
     <row r="71" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A71" s="15"/>
+      <c r="A71" s="91"/>
       <c r="B71" s="15"/>
       <c r="C71" s="15"/>
       <c r="D71" s="15"/>
@@ -27269,7 +27292,7 @@
       <c r="AA71" s="15"/>
     </row>
     <row r="72" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A72" s="15"/>
+      <c r="A72" s="91"/>
       <c r="B72" s="15"/>
       <c r="C72" s="15"/>
       <c r="D72" s="15"/>
@@ -27298,7 +27321,7 @@
       <c r="AA72" s="15"/>
     </row>
     <row r="73" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A73" s="15"/>
+      <c r="A73" s="91"/>
       <c r="B73" s="15"/>
       <c r="C73" s="15"/>
       <c r="D73" s="15"/>
@@ -27327,7 +27350,7 @@
       <c r="AA73" s="15"/>
     </row>
     <row r="74" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A74" s="15"/>
+      <c r="A74" s="91"/>
       <c r="B74" s="15"/>
       <c r="C74" s="15"/>
       <c r="D74" s="15"/>
@@ -27356,7 +27379,7 @@
       <c r="AA74" s="15"/>
     </row>
     <row r="75" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A75" s="15"/>
+      <c r="A75" s="91"/>
       <c r="B75" s="15"/>
       <c r="C75" s="15"/>
       <c r="D75" s="15"/>
@@ -27385,7 +27408,7 @@
       <c r="AA75" s="15"/>
     </row>
     <row r="76" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A76" s="15"/>
+      <c r="A76" s="91"/>
       <c r="B76" s="15"/>
       <c r="C76" s="15"/>
       <c r="D76" s="15"/>
@@ -27414,7 +27437,7 @@
       <c r="AA76" s="15"/>
     </row>
     <row r="77" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A77" s="15"/>
+      <c r="A77" s="91"/>
       <c r="B77" s="15"/>
       <c r="C77" s="15"/>
       <c r="D77" s="15"/>
@@ -27443,7 +27466,7 @@
       <c r="AA77" s="15"/>
     </row>
     <row r="78" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A78" s="15"/>
+      <c r="A78" s="91"/>
       <c r="B78" s="15"/>
       <c r="C78" s="15"/>
       <c r="D78" s="15"/>
@@ -27472,7 +27495,7 @@
       <c r="AA78" s="15"/>
     </row>
     <row r="79" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A79" s="15"/>
+      <c r="A79" s="91"/>
       <c r="B79" s="15"/>
       <c r="C79" s="15"/>
       <c r="D79" s="15"/>
@@ -27501,7 +27524,7 @@
       <c r="AA79" s="15"/>
     </row>
     <row r="80" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A80" s="15"/>
+      <c r="A80" s="91"/>
       <c r="B80" s="15"/>
       <c r="C80" s="15"/>
       <c r="D80" s="15"/>
@@ -27530,7 +27553,7 @@
       <c r="AA80" s="15"/>
     </row>
     <row r="81" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A81" s="15"/>
+      <c r="A81" s="91"/>
       <c r="B81" s="15"/>
       <c r="C81" s="15"/>
       <c r="D81" s="15"/>
@@ -27559,7 +27582,7 @@
       <c r="AA81" s="15"/>
     </row>
     <row r="82" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A82" s="15"/>
+      <c r="A82" s="91"/>
       <c r="B82" s="15"/>
       <c r="C82" s="15"/>
       <c r="D82" s="15"/>
@@ -27588,7 +27611,7 @@
       <c r="AA82" s="15"/>
     </row>
     <row r="83" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A83" s="15"/>
+      <c r="A83" s="91"/>
       <c r="B83" s="15"/>
       <c r="C83" s="15"/>
       <c r="D83" s="15"/>
@@ -27617,7 +27640,7 @@
       <c r="AA83" s="15"/>
     </row>
     <row r="84" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A84" s="15"/>
+      <c r="A84" s="91"/>
       <c r="B84" s="15"/>
       <c r="C84" s="15"/>
       <c r="D84" s="15"/>
@@ -27646,7 +27669,7 @@
       <c r="AA84" s="15"/>
     </row>
     <row r="85" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A85" s="15"/>
+      <c r="A85" s="91"/>
       <c r="B85" s="15"/>
       <c r="C85" s="15"/>
       <c r="D85" s="15"/>
@@ -27675,7 +27698,7 @@
       <c r="AA85" s="15"/>
     </row>
     <row r="86" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A86" s="15"/>
+      <c r="A86" s="91"/>
       <c r="B86" s="15"/>
       <c r="C86" s="15"/>
       <c r="D86" s="15"/>
@@ -27704,7 +27727,7 @@
       <c r="AA86" s="15"/>
     </row>
     <row r="87" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A87" s="15"/>
+      <c r="A87" s="91"/>
       <c r="B87" s="15"/>
       <c r="C87" s="15"/>
       <c r="D87" s="15"/>
@@ -27733,7 +27756,7 @@
       <c r="AA87" s="15"/>
     </row>
     <row r="88" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A88" s="15"/>
+      <c r="A88" s="91"/>
       <c r="B88" s="15"/>
       <c r="C88" s="15"/>
       <c r="D88" s="15"/>
@@ -27762,7 +27785,7 @@
       <c r="AA88" s="15"/>
     </row>
     <row r="89" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A89" s="15"/>
+      <c r="A89" s="91"/>
       <c r="B89" s="15"/>
       <c r="C89" s="15"/>
       <c r="D89" s="15"/>
@@ -27791,7 +27814,7 @@
       <c r="AA89" s="15"/>
     </row>
     <row r="90" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A90" s="15"/>
+      <c r="A90" s="91"/>
       <c r="B90" s="15"/>
       <c r="C90" s="15"/>
       <c r="D90" s="15"/>
@@ -27820,7 +27843,7 @@
       <c r="AA90" s="15"/>
     </row>
     <row r="91" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A91" s="15"/>
+      <c r="A91" s="91"/>
       <c r="B91" s="15"/>
       <c r="C91" s="15"/>
       <c r="D91" s="15"/>
@@ -27849,7 +27872,7 @@
       <c r="AA91" s="15"/>
     </row>
     <row r="92" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A92" s="15"/>
+      <c r="A92" s="91"/>
       <c r="B92" s="15"/>
       <c r="C92" s="15"/>
       <c r="D92" s="15"/>
@@ -27878,7 +27901,7 @@
       <c r="AA92" s="15"/>
     </row>
     <row r="93" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A93" s="15"/>
+      <c r="A93" s="91"/>
       <c r="B93" s="15"/>
       <c r="C93" s="15"/>
       <c r="D93" s="15"/>
@@ -27907,7 +27930,7 @@
       <c r="AA93" s="15"/>
     </row>
     <row r="94" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A94" s="15"/>
+      <c r="A94" s="91"/>
       <c r="B94" s="15"/>
       <c r="C94" s="15"/>
       <c r="D94" s="15"/>
@@ -27936,7 +27959,7 @@
       <c r="AA94" s="15"/>
     </row>
     <row r="95" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A95" s="15"/>
+      <c r="A95" s="91"/>
       <c r="B95" s="15"/>
       <c r="C95" s="15"/>
       <c r="D95" s="15"/>
@@ -27965,7 +27988,7 @@
       <c r="AA95" s="15"/>
     </row>
     <row r="96" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A96" s="15"/>
+      <c r="A96" s="91"/>
       <c r="B96" s="15"/>
       <c r="C96" s="15"/>
       <c r="D96" s="15"/>
@@ -27994,7 +28017,7 @@
       <c r="AA96" s="15"/>
     </row>
     <row r="97" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A97" s="15"/>
+      <c r="A97" s="91"/>
       <c r="B97" s="15"/>
       <c r="C97" s="15"/>
       <c r="D97" s="15"/>
@@ -28023,7 +28046,7 @@
       <c r="AA97" s="15"/>
     </row>
     <row r="98" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A98" s="15"/>
+      <c r="A98" s="91"/>
       <c r="B98" s="15"/>
       <c r="C98" s="15"/>
       <c r="D98" s="15"/>
@@ -28052,7 +28075,7 @@
       <c r="AA98" s="15"/>
     </row>
     <row r="99" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A99" s="15"/>
+      <c r="A99" s="91"/>
       <c r="B99" s="15"/>
       <c r="C99" s="15"/>
       <c r="D99" s="15"/>
@@ -28081,7 +28104,7 @@
       <c r="AA99" s="15"/>
     </row>
     <row r="100" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A100" s="15"/>
+      <c r="A100" s="91"/>
       <c r="B100" s="15"/>
       <c r="C100" s="15"/>
       <c r="D100" s="15"/>
@@ -28110,7 +28133,7 @@
       <c r="AA100" s="15"/>
     </row>
     <row r="101" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A101" s="15"/>
+      <c r="A101" s="91"/>
       <c r="B101" s="15"/>
       <c r="C101" s="15"/>
       <c r="D101" s="15"/>
@@ -28139,7 +28162,7 @@
       <c r="AA101" s="15"/>
     </row>
     <row r="102" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A102" s="15"/>
+      <c r="A102" s="91"/>
       <c r="B102" s="15"/>
       <c r="C102" s="15"/>
       <c r="D102" s="15"/>
@@ -28168,7 +28191,7 @@
       <c r="AA102" s="15"/>
     </row>
     <row r="103" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A103" s="15"/>
+      <c r="A103" s="91"/>
       <c r="B103" s="15"/>
       <c r="C103" s="15"/>
       <c r="D103" s="15"/>
@@ -28197,7 +28220,7 @@
       <c r="AA103" s="15"/>
     </row>
     <row r="104" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A104" s="15"/>
+      <c r="A104" s="91"/>
       <c r="B104" s="15"/>
       <c r="C104" s="15"/>
       <c r="D104" s="15"/>
@@ -28226,7 +28249,7 @@
       <c r="AA104" s="15"/>
     </row>
     <row r="105" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A105" s="15"/>
+      <c r="A105" s="91"/>
       <c r="B105" s="15"/>
       <c r="C105" s="15"/>
       <c r="D105" s="15"/>
@@ -28255,7 +28278,7 @@
       <c r="AA105" s="15"/>
     </row>
     <row r="106" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A106" s="15"/>
+      <c r="A106" s="91"/>
       <c r="B106" s="15"/>
       <c r="C106" s="15"/>
       <c r="D106" s="15"/>
@@ -28284,7 +28307,7 @@
       <c r="AA106" s="15"/>
     </row>
     <row r="107" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A107" s="15"/>
+      <c r="A107" s="91"/>
       <c r="B107" s="15"/>
       <c r="C107" s="15"/>
       <c r="D107" s="15"/>
@@ -28313,7 +28336,7 @@
       <c r="AA107" s="15"/>
     </row>
     <row r="108" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A108" s="15"/>
+      <c r="A108" s="91"/>
       <c r="B108" s="15"/>
       <c r="C108" s="15"/>
       <c r="D108" s="15"/>
@@ -28342,7 +28365,7 @@
       <c r="AA108" s="15"/>
     </row>
     <row r="109" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A109" s="15"/>
+      <c r="A109" s="91"/>
       <c r="B109" s="15"/>
       <c r="C109" s="15"/>
       <c r="D109" s="15"/>
@@ -28371,7 +28394,7 @@
       <c r="AA109" s="15"/>
     </row>
     <row r="110" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A110" s="15"/>
+      <c r="A110" s="91"/>
       <c r="B110" s="15"/>
       <c r="C110" s="15"/>
       <c r="D110" s="15"/>
@@ -28400,7 +28423,7 @@
       <c r="AA110" s="15"/>
     </row>
     <row r="111" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A111" s="15"/>
+      <c r="A111" s="91"/>
       <c r="B111" s="15"/>
       <c r="C111" s="15"/>
       <c r="D111" s="15"/>
@@ -28429,7 +28452,7 @@
       <c r="AA111" s="15"/>
     </row>
     <row r="112" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A112" s="15"/>
+      <c r="A112" s="91"/>
       <c r="B112" s="15"/>
       <c r="C112" s="15"/>
       <c r="D112" s="15"/>
@@ -28458,7 +28481,7 @@
       <c r="AA112" s="15"/>
     </row>
     <row r="113" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A113" s="15"/>
+      <c r="A113" s="91"/>
       <c r="B113" s="15"/>
       <c r="C113" s="15"/>
       <c r="D113" s="15"/>
@@ -28487,7 +28510,7 @@
       <c r="AA113" s="15"/>
     </row>
     <row r="114" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A114" s="15"/>
+      <c r="A114" s="91"/>
       <c r="B114" s="15"/>
       <c r="C114" s="15"/>
       <c r="D114" s="15"/>
@@ -28516,7 +28539,7 @@
       <c r="AA114" s="15"/>
     </row>
     <row r="115" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A115" s="15"/>
+      <c r="A115" s="91"/>
       <c r="B115" s="15"/>
       <c r="C115" s="15"/>
       <c r="D115" s="15"/>
@@ -28545,7 +28568,7 @@
       <c r="AA115" s="15"/>
     </row>
     <row r="116" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A116" s="15"/>
+      <c r="A116" s="91"/>
       <c r="B116" s="15"/>
       <c r="C116" s="15"/>
       <c r="D116" s="15"/>
@@ -28574,7 +28597,7 @@
       <c r="AA116" s="15"/>
     </row>
     <row r="117" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A117" s="15"/>
+      <c r="A117" s="91"/>
       <c r="B117" s="15"/>
       <c r="C117" s="15"/>
       <c r="D117" s="15"/>
@@ -28603,7 +28626,7 @@
       <c r="AA117" s="15"/>
     </row>
     <row r="118" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A118" s="15"/>
+      <c r="A118" s="91"/>
       <c r="B118" s="15"/>
       <c r="C118" s="15"/>
       <c r="D118" s="15"/>
@@ -28632,7 +28655,7 @@
       <c r="AA118" s="15"/>
     </row>
     <row r="119" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A119" s="15"/>
+      <c r="A119" s="91"/>
       <c r="B119" s="15"/>
       <c r="C119" s="15"/>
       <c r="D119" s="15"/>
@@ -28661,7 +28684,7 @@
       <c r="AA119" s="15"/>
     </row>
     <row r="120" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A120" s="15"/>
+      <c r="A120" s="91"/>
       <c r="B120" s="15"/>
       <c r="C120" s="15"/>
       <c r="D120" s="15"/>
@@ -28690,7 +28713,7 @@
       <c r="AA120" s="15"/>
     </row>
     <row r="121" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A121" s="15"/>
+      <c r="A121" s="91"/>
       <c r="B121" s="15"/>
       <c r="C121" s="15"/>
       <c r="D121" s="15"/>
@@ -28719,7 +28742,7 @@
       <c r="AA121" s="15"/>
     </row>
     <row r="122" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A122" s="15"/>
+      <c r="A122" s="91"/>
       <c r="B122" s="15"/>
       <c r="C122" s="15"/>
       <c r="D122" s="15"/>
@@ -28748,7 +28771,7 @@
       <c r="AA122" s="15"/>
     </row>
     <row r="123" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A123" s="15"/>
+      <c r="A123" s="91"/>
       <c r="B123" s="15"/>
       <c r="C123" s="15"/>
       <c r="D123" s="15"/>
@@ -28777,7 +28800,7 @@
       <c r="AA123" s="15"/>
     </row>
     <row r="124" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A124" s="15"/>
+      <c r="A124" s="91"/>
       <c r="B124" s="15"/>
       <c r="C124" s="15"/>
       <c r="D124" s="15"/>
@@ -28806,7 +28829,7 @@
       <c r="AA124" s="15"/>
     </row>
     <row r="125" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A125" s="15"/>
+      <c r="A125" s="91"/>
       <c r="B125" s="15"/>
       <c r="C125" s="15"/>
       <c r="D125" s="15"/>
@@ -28835,7 +28858,7 @@
       <c r="AA125" s="15"/>
     </row>
     <row r="126" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A126" s="15"/>
+      <c r="A126" s="91"/>
       <c r="B126" s="15"/>
       <c r="C126" s="15"/>
       <c r="D126" s="15"/>
@@ -28864,7 +28887,7 @@
       <c r="AA126" s="15"/>
     </row>
     <row r="127" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A127" s="15"/>
+      <c r="A127" s="91"/>
       <c r="B127" s="15"/>
       <c r="C127" s="15"/>
       <c r="D127" s="15"/>
@@ -28893,7 +28916,7 @@
       <c r="AA127" s="15"/>
     </row>
     <row r="128" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A128" s="15"/>
+      <c r="A128" s="91"/>
       <c r="B128" s="15"/>
       <c r="C128" s="15"/>
       <c r="D128" s="15"/>
@@ -28922,7 +28945,7 @@
       <c r="AA128" s="15"/>
     </row>
     <row r="129" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A129" s="15"/>
+      <c r="A129" s="91"/>
       <c r="B129" s="15"/>
       <c r="C129" s="15"/>
       <c r="D129" s="15"/>
@@ -28951,7 +28974,7 @@
       <c r="AA129" s="15"/>
     </row>
     <row r="130" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A130" s="15"/>
+      <c r="A130" s="91"/>
       <c r="B130" s="15"/>
       <c r="C130" s="15"/>
       <c r="D130" s="15"/>
@@ -28980,7 +29003,7 @@
       <c r="AA130" s="15"/>
     </row>
     <row r="131" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A131" s="15"/>
+      <c r="A131" s="91"/>
       <c r="B131" s="15"/>
       <c r="C131" s="15"/>
       <c r="D131" s="15"/>
@@ -29009,7 +29032,7 @@
       <c r="AA131" s="15"/>
     </row>
     <row r="132" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A132" s="15"/>
+      <c r="A132" s="91"/>
       <c r="B132" s="15"/>
       <c r="C132" s="15"/>
       <c r="D132" s="15"/>
@@ -29038,7 +29061,7 @@
       <c r="AA132" s="15"/>
     </row>
     <row r="133" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A133" s="15"/>
+      <c r="A133" s="91"/>
       <c r="B133" s="15"/>
       <c r="C133" s="15"/>
       <c r="D133" s="15"/>
@@ -29067,7 +29090,7 @@
       <c r="AA133" s="15"/>
     </row>
     <row r="134" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A134" s="15"/>
+      <c r="A134" s="91"/>
       <c r="B134" s="15"/>
       <c r="C134" s="15"/>
       <c r="D134" s="15"/>
@@ -29096,7 +29119,7 @@
       <c r="AA134" s="15"/>
     </row>
     <row r="135" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A135" s="15"/>
+      <c r="A135" s="91"/>
       <c r="B135" s="15"/>
       <c r="C135" s="15"/>
       <c r="D135" s="15"/>
@@ -29125,7 +29148,7 @@
       <c r="AA135" s="15"/>
     </row>
     <row r="136" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A136" s="15"/>
+      <c r="A136" s="91"/>
       <c r="B136" s="15"/>
       <c r="C136" s="15"/>
       <c r="D136" s="15"/>
@@ -29154,7 +29177,7 @@
       <c r="AA136" s="15"/>
     </row>
     <row r="137" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A137" s="15"/>
+      <c r="A137" s="91"/>
       <c r="B137" s="15"/>
       <c r="C137" s="15"/>
       <c r="D137" s="15"/>
@@ -29183,7 +29206,7 @@
       <c r="AA137" s="15"/>
     </row>
     <row r="138" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A138" s="15"/>
+      <c r="A138" s="91"/>
       <c r="B138" s="15"/>
       <c r="C138" s="15"/>
       <c r="D138" s="15"/>
@@ -29212,7 +29235,7 @@
       <c r="AA138" s="15"/>
     </row>
     <row r="139" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A139" s="15"/>
+      <c r="A139" s="91"/>
       <c r="B139" s="15"/>
       <c r="C139" s="15"/>
       <c r="D139" s="15"/>
@@ -29241,7 +29264,7 @@
       <c r="AA139" s="15"/>
     </row>
     <row r="140" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A140" s="15"/>
+      <c r="A140" s="91"/>
       <c r="B140" s="15"/>
       <c r="C140" s="15"/>
       <c r="D140" s="15"/>
@@ -29270,7 +29293,7 @@
       <c r="AA140" s="15"/>
     </row>
     <row r="141" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A141" s="15"/>
+      <c r="A141" s="91"/>
       <c r="B141" s="15"/>
       <c r="C141" s="15"/>
       <c r="D141" s="15"/>
@@ -29299,7 +29322,7 @@
       <c r="AA141" s="15"/>
     </row>
     <row r="142" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A142" s="15"/>
+      <c r="A142" s="91"/>
       <c r="B142" s="15"/>
       <c r="C142" s="15"/>
       <c r="D142" s="15"/>
@@ -29328,7 +29351,7 @@
       <c r="AA142" s="15"/>
     </row>
     <row r="143" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A143" s="15"/>
+      <c r="A143" s="91"/>
       <c r="B143" s="15"/>
       <c r="C143" s="15"/>
       <c r="D143" s="15"/>
@@ -29357,7 +29380,7 @@
       <c r="AA143" s="15"/>
     </row>
     <row r="144" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A144" s="15"/>
+      <c r="A144" s="91"/>
       <c r="B144" s="15"/>
       <c r="C144" s="15"/>
       <c r="D144" s="15"/>
@@ -29386,7 +29409,7 @@
       <c r="AA144" s="15"/>
     </row>
     <row r="145" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A145" s="15"/>
+      <c r="A145" s="91"/>
       <c r="B145" s="15"/>
       <c r="C145" s="15"/>
       <c r="D145" s="15"/>
@@ -29415,7 +29438,7 @@
       <c r="AA145" s="15"/>
     </row>
     <row r="146" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A146" s="15"/>
+      <c r="A146" s="91"/>
       <c r="B146" s="15"/>
       <c r="C146" s="15"/>
       <c r="D146" s="15"/>
@@ -29444,7 +29467,7 @@
       <c r="AA146" s="15"/>
     </row>
     <row r="147" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A147" s="15"/>
+      <c r="A147" s="91"/>
       <c r="B147" s="15"/>
       <c r="C147" s="15"/>
       <c r="D147" s="15"/>
@@ -29473,7 +29496,7 @@
       <c r="AA147" s="15"/>
     </row>
     <row r="148" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A148" s="15"/>
+      <c r="A148" s="91"/>
       <c r="B148" s="15"/>
       <c r="C148" s="15"/>
       <c r="D148" s="15"/>
@@ -29502,7 +29525,7 @@
       <c r="AA148" s="15"/>
     </row>
     <row r="149" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A149" s="15"/>
+      <c r="A149" s="91"/>
       <c r="B149" s="15"/>
       <c r="C149" s="15"/>
       <c r="D149" s="15"/>
@@ -29531,7 +29554,7 @@
       <c r="AA149" s="15"/>
     </row>
     <row r="150" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A150" s="15"/>
+      <c r="A150" s="91"/>
       <c r="B150" s="15"/>
       <c r="C150" s="15"/>
       <c r="D150" s="15"/>
@@ -29560,7 +29583,7 @@
       <c r="AA150" s="15"/>
     </row>
     <row r="151" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A151" s="15"/>
+      <c r="A151" s="91"/>
       <c r="B151" s="15"/>
       <c r="C151" s="15"/>
       <c r="D151" s="15"/>
@@ -29589,7 +29612,7 @@
       <c r="AA151" s="15"/>
     </row>
     <row r="152" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A152" s="15"/>
+      <c r="A152" s="91"/>
       <c r="B152" s="15"/>
       <c r="C152" s="15"/>
       <c r="D152" s="15"/>
@@ -29618,7 +29641,7 @@
       <c r="AA152" s="15"/>
     </row>
     <row r="153" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A153" s="15"/>
+      <c r="A153" s="91"/>
       <c r="B153" s="15"/>
       <c r="C153" s="15"/>
       <c r="D153" s="15"/>
@@ -29647,7 +29670,7 @@
       <c r="AA153" s="15"/>
     </row>
     <row r="154" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A154" s="15"/>
+      <c r="A154" s="91"/>
       <c r="B154" s="15"/>
       <c r="C154" s="15"/>
       <c r="D154" s="15"/>
@@ -29676,7 +29699,7 @@
       <c r="AA154" s="15"/>
     </row>
     <row r="155" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A155" s="15"/>
+      <c r="A155" s="91"/>
       <c r="B155" s="15"/>
       <c r="C155" s="15"/>
       <c r="D155" s="15"/>
@@ -29705,7 +29728,7 @@
       <c r="AA155" s="15"/>
     </row>
     <row r="156" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A156" s="15"/>
+      <c r="A156" s="91"/>
       <c r="B156" s="15"/>
       <c r="C156" s="15"/>
       <c r="D156" s="15"/>
@@ -29734,7 +29757,7 @@
       <c r="AA156" s="15"/>
     </row>
     <row r="157" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A157" s="15"/>
+      <c r="A157" s="91"/>
       <c r="B157" s="15"/>
       <c r="C157" s="15"/>
       <c r="D157" s="15"/>
@@ -29763,7 +29786,7 @@
       <c r="AA157" s="15"/>
     </row>
     <row r="158" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A158" s="15"/>
+      <c r="A158" s="91"/>
       <c r="B158" s="15"/>
       <c r="C158" s="15"/>
       <c r="D158" s="15"/>
@@ -29792,7 +29815,7 @@
       <c r="AA158" s="15"/>
     </row>
     <row r="159" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A159" s="15"/>
+      <c r="A159" s="91"/>
       <c r="B159" s="15"/>
       <c r="C159" s="15"/>
       <c r="D159" s="15"/>
@@ -29821,7 +29844,7 @@
       <c r="AA159" s="15"/>
     </row>
     <row r="160" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A160" s="15"/>
+      <c r="A160" s="91"/>
       <c r="B160" s="15"/>
       <c r="C160" s="15"/>
       <c r="D160" s="15"/>
@@ -29850,7 +29873,7 @@
       <c r="AA160" s="15"/>
     </row>
     <row r="161" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A161" s="15"/>
+      <c r="A161" s="91"/>
       <c r="B161" s="15"/>
       <c r="C161" s="15"/>
       <c r="D161" s="15"/>
@@ -29879,7 +29902,7 @@
       <c r="AA161" s="15"/>
     </row>
     <row r="162" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A162" s="15"/>
+      <c r="A162" s="91"/>
       <c r="B162" s="15"/>
       <c r="C162" s="15"/>
       <c r="D162" s="15"/>
@@ -29908,7 +29931,7 @@
       <c r="AA162" s="15"/>
     </row>
     <row r="163" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A163" s="15"/>
+      <c r="A163" s="91"/>
       <c r="B163" s="15"/>
       <c r="C163" s="15"/>
       <c r="D163" s="15"/>
@@ -29937,7 +29960,7 @@
       <c r="AA163" s="15"/>
     </row>
     <row r="164" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A164" s="15"/>
+      <c r="A164" s="91"/>
       <c r="B164" s="15"/>
       <c r="C164" s="15"/>
       <c r="D164" s="15"/>
@@ -29966,7 +29989,7 @@
       <c r="AA164" s="15"/>
     </row>
     <row r="165" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A165" s="15"/>
+      <c r="A165" s="91"/>
       <c r="B165" s="15"/>
       <c r="C165" s="15"/>
       <c r="D165" s="15"/>
@@ -29995,7 +30018,7 @@
       <c r="AA165" s="15"/>
     </row>
     <row r="166" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A166" s="15"/>
+      <c r="A166" s="91"/>
       <c r="B166" s="15"/>
       <c r="C166" s="15"/>
       <c r="D166" s="15"/>
@@ -30024,7 +30047,7 @@
       <c r="AA166" s="15"/>
     </row>
     <row r="167" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A167" s="15"/>
+      <c r="A167" s="91"/>
       <c r="B167" s="15"/>
       <c r="C167" s="15"/>
       <c r="D167" s="15"/>
@@ -30053,7 +30076,7 @@
       <c r="AA167" s="15"/>
     </row>
     <row r="168" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A168" s="15"/>
+      <c r="A168" s="91"/>
       <c r="B168" s="15"/>
       <c r="C168" s="15"/>
       <c r="D168" s="15"/>
@@ -30082,7 +30105,7 @@
       <c r="AA168" s="15"/>
     </row>
     <row r="169" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A169" s="15"/>
+      <c r="A169" s="91"/>
       <c r="B169" s="15"/>
       <c r="C169" s="15"/>
       <c r="D169" s="15"/>
@@ -30111,7 +30134,7 @@
       <c r="AA169" s="15"/>
     </row>
     <row r="170" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A170" s="15"/>
+      <c r="A170" s="91"/>
       <c r="B170" s="15"/>
       <c r="C170" s="15"/>
       <c r="D170" s="15"/>
@@ -30140,7 +30163,7 @@
       <c r="AA170" s="15"/>
     </row>
     <row r="171" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A171" s="15"/>
+      <c r="A171" s="91"/>
       <c r="B171" s="15"/>
       <c r="C171" s="15"/>
       <c r="D171" s="15"/>
@@ -30169,7 +30192,7 @@
       <c r="AA171" s="15"/>
     </row>
     <row r="172" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A172" s="15"/>
+      <c r="A172" s="91"/>
       <c r="B172" s="15"/>
       <c r="C172" s="15"/>
       <c r="D172" s="15"/>
@@ -30198,7 +30221,7 @@
       <c r="AA172" s="15"/>
     </row>
     <row r="173" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A173" s="15"/>
+      <c r="A173" s="91"/>
       <c r="B173" s="15"/>
       <c r="C173" s="15"/>
       <c r="D173" s="15"/>
@@ -30227,7 +30250,7 @@
       <c r="AA173" s="15"/>
     </row>
     <row r="174" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A174" s="15"/>
+      <c r="A174" s="91"/>
       <c r="B174" s="15"/>
       <c r="C174" s="15"/>
       <c r="D174" s="15"/>
@@ -30256,7 +30279,7 @@
       <c r="AA174" s="15"/>
     </row>
     <row r="175" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A175" s="15"/>
+      <c r="A175" s="91"/>
       <c r="B175" s="15"/>
       <c r="C175" s="15"/>
       <c r="D175" s="15"/>
@@ -30285,7 +30308,7 @@
       <c r="AA175" s="15"/>
     </row>
     <row r="176" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A176" s="15"/>
+      <c r="A176" s="91"/>
       <c r="B176" s="15"/>
       <c r="C176" s="15"/>
       <c r="D176" s="15"/>
@@ -30314,7 +30337,7 @@
       <c r="AA176" s="15"/>
     </row>
     <row r="177" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A177" s="15"/>
+      <c r="A177" s="91"/>
       <c r="B177" s="15"/>
       <c r="C177" s="15"/>
       <c r="D177" s="15"/>
@@ -30343,7 +30366,7 @@
       <c r="AA177" s="15"/>
     </row>
     <row r="178" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A178" s="15"/>
+      <c r="A178" s="91"/>
       <c r="B178" s="15"/>
       <c r="C178" s="15"/>
       <c r="D178" s="15"/>
@@ -30372,7 +30395,7 @@
       <c r="AA178" s="15"/>
     </row>
     <row r="179" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A179" s="15"/>
+      <c r="A179" s="91"/>
       <c r="B179" s="15"/>
       <c r="C179" s="15"/>
       <c r="D179" s="15"/>
@@ -30401,7 +30424,7 @@
       <c r="AA179" s="15"/>
     </row>
     <row r="180" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A180" s="15"/>
+      <c r="A180" s="91"/>
       <c r="B180" s="15"/>
       <c r="C180" s="15"/>
       <c r="D180" s="15"/>
@@ -30430,7 +30453,7 @@
       <c r="AA180" s="15"/>
     </row>
     <row r="181" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A181" s="15"/>
+      <c r="A181" s="91"/>
       <c r="B181" s="15"/>
       <c r="C181" s="15"/>
       <c r="D181" s="15"/>
@@ -30459,7 +30482,7 @@
       <c r="AA181" s="15"/>
     </row>
     <row r="182" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A182" s="15"/>
+      <c r="A182" s="91"/>
       <c r="B182" s="15"/>
       <c r="C182" s="15"/>
       <c r="D182" s="15"/>
@@ -30488,7 +30511,7 @@
       <c r="AA182" s="15"/>
     </row>
     <row r="183" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A183" s="15"/>
+      <c r="A183" s="91"/>
       <c r="B183" s="15"/>
       <c r="C183" s="15"/>
       <c r="D183" s="15"/>
@@ -30517,7 +30540,7 @@
       <c r="AA183" s="15"/>
     </row>
     <row r="184" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A184" s="15"/>
+      <c r="A184" s="91"/>
       <c r="B184" s="15"/>
       <c r="C184" s="15"/>
       <c r="D184" s="15"/>
@@ -30546,7 +30569,7 @@
       <c r="AA184" s="15"/>
     </row>
     <row r="185" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A185" s="15"/>
+      <c r="A185" s="91"/>
       <c r="B185" s="15"/>
       <c r="C185" s="15"/>
       <c r="D185" s="15"/>
@@ -30575,7 +30598,7 @@
       <c r="AA185" s="15"/>
     </row>
     <row r="186" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A186" s="15"/>
+      <c r="A186" s="91"/>
       <c r="B186" s="15"/>
       <c r="C186" s="15"/>
       <c r="D186" s="15"/>
@@ -30604,7 +30627,7 @@
       <c r="AA186" s="15"/>
     </row>
     <row r="187" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A187" s="15"/>
+      <c r="A187" s="91"/>
       <c r="B187" s="15"/>
       <c r="C187" s="15"/>
       <c r="D187" s="15"/>
@@ -30633,7 +30656,7 @@
       <c r="AA187" s="15"/>
     </row>
     <row r="188" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A188" s="15"/>
+      <c r="A188" s="91"/>
       <c r="B188" s="15"/>
       <c r="C188" s="15"/>
       <c r="D188" s="15"/>
@@ -30662,7 +30685,7 @@
       <c r="AA188" s="15"/>
     </row>
     <row r="189" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A189" s="15"/>
+      <c r="A189" s="91"/>
       <c r="B189" s="15"/>
       <c r="C189" s="15"/>
       <c r="D189" s="15"/>
@@ -30691,7 +30714,7 @@
       <c r="AA189" s="15"/>
     </row>
     <row r="190" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A190" s="15"/>
+      <c r="A190" s="91"/>
       <c r="B190" s="15"/>
       <c r="C190" s="15"/>
       <c r="D190" s="15"/>
@@ -30720,7 +30743,7 @@
       <c r="AA190" s="15"/>
     </row>
     <row r="191" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A191" s="15"/>
+      <c r="A191" s="91"/>
       <c r="B191" s="15"/>
       <c r="C191" s="15"/>
       <c r="D191" s="15"/>
@@ -30749,7 +30772,7 @@
       <c r="AA191" s="15"/>
     </row>
     <row r="192" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A192" s="15"/>
+      <c r="A192" s="91"/>
       <c r="B192" s="15"/>
       <c r="C192" s="15"/>
       <c r="D192" s="15"/>
@@ -30778,7 +30801,7 @@
       <c r="AA192" s="15"/>
     </row>
     <row r="193" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A193" s="15"/>
+      <c r="A193" s="91"/>
       <c r="B193" s="15"/>
       <c r="C193" s="15"/>
       <c r="D193" s="15"/>
@@ -30807,7 +30830,7 @@
       <c r="AA193" s="15"/>
     </row>
     <row r="194" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A194" s="15"/>
+      <c r="A194" s="91"/>
       <c r="B194" s="15"/>
       <c r="C194" s="15"/>
       <c r="D194" s="15"/>
@@ -30836,7 +30859,7 @@
       <c r="AA194" s="15"/>
     </row>
     <row r="195" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A195" s="15"/>
+      <c r="A195" s="91"/>
       <c r="B195" s="15"/>
       <c r="C195" s="15"/>
       <c r="D195" s="15"/>
@@ -30865,7 +30888,7 @@
       <c r="AA195" s="15"/>
     </row>
     <row r="196" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A196" s="15"/>
+      <c r="A196" s="91"/>
       <c r="B196" s="15"/>
       <c r="C196" s="15"/>
       <c r="D196" s="15"/>
@@ -30894,7 +30917,7 @@
       <c r="AA196" s="15"/>
     </row>
     <row r="197" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A197" s="15"/>
+      <c r="A197" s="91"/>
       <c r="B197" s="15"/>
       <c r="C197" s="15"/>
       <c r="D197" s="15"/>
@@ -30923,7 +30946,7 @@
       <c r="AA197" s="15"/>
     </row>
     <row r="198" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A198" s="15"/>
+      <c r="A198" s="91"/>
       <c r="B198" s="15"/>
       <c r="C198" s="15"/>
       <c r="D198" s="15"/>
@@ -30952,7 +30975,7 @@
       <c r="AA198" s="15"/>
     </row>
     <row r="199" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A199" s="15"/>
+      <c r="A199" s="91"/>
       <c r="B199" s="15"/>
       <c r="C199" s="15"/>
       <c r="D199" s="15"/>
@@ -30981,7 +31004,7 @@
       <c r="AA199" s="15"/>
     </row>
     <row r="200" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A200" s="15"/>
+      <c r="A200" s="91"/>
       <c r="B200" s="15"/>
       <c r="C200" s="15"/>
       <c r="D200" s="15"/>
@@ -31010,7 +31033,7 @@
       <c r="AA200" s="15"/>
     </row>
     <row r="201" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A201" s="15"/>
+      <c r="A201" s="91"/>
       <c r="B201" s="15"/>
       <c r="C201" s="15"/>
       <c r="D201" s="15"/>
@@ -31039,7 +31062,7 @@
       <c r="AA201" s="15"/>
     </row>
     <row r="202" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A202" s="15"/>
+      <c r="A202" s="91"/>
       <c r="B202" s="15"/>
       <c r="C202" s="15"/>
       <c r="D202" s="15"/>
@@ -31068,7 +31091,7 @@
       <c r="AA202" s="15"/>
     </row>
     <row r="203" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A203" s="15"/>
+      <c r="A203" s="91"/>
       <c r="B203" s="15"/>
       <c r="C203" s="15"/>
       <c r="D203" s="15"/>
@@ -31097,7 +31120,7 @@
       <c r="AA203" s="15"/>
     </row>
     <row r="204" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A204" s="15"/>
+      <c r="A204" s="91"/>
       <c r="B204" s="15"/>
       <c r="C204" s="15"/>
       <c r="D204" s="15"/>
@@ -31126,7 +31149,7 @@
       <c r="AA204" s="15"/>
     </row>
     <row r="205" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A205" s="15"/>
+      <c r="A205" s="91"/>
       <c r="B205" s="15"/>
       <c r="C205" s="15"/>
       <c r="D205" s="15"/>
@@ -31155,7 +31178,7 @@
       <c r="AA205" s="15"/>
     </row>
     <row r="206" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A206" s="15"/>
+      <c r="A206" s="91"/>
       <c r="B206" s="15"/>
       <c r="C206" s="15"/>
       <c r="D206" s="15"/>
@@ -31184,7 +31207,7 @@
       <c r="AA206" s="15"/>
     </row>
     <row r="207" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A207" s="15"/>
+      <c r="A207" s="91"/>
       <c r="B207" s="15"/>
       <c r="C207" s="15"/>
       <c r="D207" s="15"/>
@@ -31213,7 +31236,7 @@
       <c r="AA207" s="15"/>
     </row>
     <row r="208" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A208" s="15"/>
+      <c r="A208" s="91"/>
       <c r="B208" s="15"/>
       <c r="C208" s="15"/>
       <c r="D208" s="15"/>
@@ -31242,7 +31265,7 @@
       <c r="AA208" s="15"/>
     </row>
     <row r="209" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A209" s="15"/>
+      <c r="A209" s="91"/>
       <c r="B209" s="15"/>
       <c r="C209" s="15"/>
       <c r="D209" s="15"/>
@@ -31271,7 +31294,7 @@
       <c r="AA209" s="15"/>
     </row>
     <row r="210" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A210" s="15"/>
+      <c r="A210" s="91"/>
       <c r="B210" s="15"/>
       <c r="C210" s="15"/>
       <c r="D210" s="15"/>
@@ -31300,7 +31323,7 @@
       <c r="AA210" s="15"/>
     </row>
     <row r="211" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A211" s="15"/>
+      <c r="A211" s="91"/>
       <c r="B211" s="15"/>
       <c r="C211" s="15"/>
       <c r="D211" s="15"/>
@@ -31329,7 +31352,7 @@
       <c r="AA211" s="15"/>
     </row>
     <row r="212" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A212" s="15"/>
+      <c r="A212" s="91"/>
       <c r="B212" s="15"/>
       <c r="C212" s="15"/>
       <c r="D212" s="15"/>
@@ -31358,7 +31381,7 @@
       <c r="AA212" s="15"/>
     </row>
     <row r="213" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A213" s="15"/>
+      <c r="A213" s="91"/>
       <c r="B213" s="15"/>
       <c r="C213" s="15"/>
       <c r="D213" s="15"/>
@@ -31387,7 +31410,7 @@
       <c r="AA213" s="15"/>
     </row>
     <row r="214" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A214" s="15"/>
+      <c r="A214" s="91"/>
       <c r="B214" s="15"/>
       <c r="C214" s="15"/>
       <c r="D214" s="15"/>
@@ -31416,7 +31439,7 @@
       <c r="AA214" s="15"/>
     </row>
     <row r="215" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A215" s="15"/>
+      <c r="A215" s="91"/>
       <c r="B215" s="15"/>
       <c r="C215" s="15"/>
       <c r="D215" s="15"/>
@@ -31445,7 +31468,7 @@
       <c r="AA215" s="15"/>
     </row>
     <row r="216" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A216" s="15"/>
+      <c r="A216" s="91"/>
       <c r="B216" s="15"/>
       <c r="C216" s="15"/>
       <c r="D216" s="15"/>
@@ -31474,7 +31497,7 @@
       <c r="AA216" s="15"/>
     </row>
     <row r="217" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A217" s="15"/>
+      <c r="A217" s="91"/>
       <c r="B217" s="15"/>
       <c r="C217" s="15"/>
       <c r="D217" s="15"/>
@@ -31503,7 +31526,7 @@
       <c r="AA217" s="15"/>
     </row>
     <row r="218" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A218" s="15"/>
+      <c r="A218" s="91"/>
       <c r="B218" s="15"/>
       <c r="C218" s="15"/>
       <c r="D218" s="15"/>
@@ -31532,7 +31555,7 @@
       <c r="AA218" s="15"/>
     </row>
     <row r="219" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A219" s="15"/>
+      <c r="A219" s="91"/>
       <c r="B219" s="15"/>
       <c r="C219" s="15"/>
       <c r="D219" s="15"/>
@@ -31561,7 +31584,7 @@
       <c r="AA219" s="15"/>
     </row>
     <row r="220" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A220" s="15"/>
+      <c r="A220" s="91"/>
       <c r="B220" s="15"/>
       <c r="C220" s="15"/>
       <c r="D220" s="15"/>
@@ -32393,13 +32416,13 @@
   <sheetData>
     <row r="1" spans="1:25" ht="15.75" customHeight="1">
       <c r="A1" s="62" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B1" s="62" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C1" s="62" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D1" s="15"/>
       <c r="E1" s="15"/>
@@ -39169,7 +39192,7 @@
     <row r="2" spans="1:25" ht="15.75" customHeight="1">
       <c r="A2" s="65"/>
       <c r="B2" s="66" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C2" s="67"/>
       <c r="D2" s="15"/>
@@ -39198,7 +39221,7 @@
     <row r="3" spans="1:25" ht="15.75" customHeight="1">
       <c r="A3" s="65"/>
       <c r="B3" s="66" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C3" s="67"/>
       <c r="D3" s="15"/>
@@ -39227,7 +39250,7 @@
     <row r="4" spans="1:25" ht="15.75" customHeight="1">
       <c r="A4" s="65"/>
       <c r="B4" s="68" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C4" s="67"/>
       <c r="D4" s="15"/>
@@ -39256,7 +39279,7 @@
     <row r="5" spans="1:25" ht="15.75" customHeight="1">
       <c r="A5" s="65"/>
       <c r="B5" s="68" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C5" s="67"/>
       <c r="D5" s="15"/>

</xml_diff>